<commit_message>
added new translations for dialogs and hard coded text
</commit_message>
<xml_diff>
--- a/translations/translations.xlsx
+++ b/translations/translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bp51\Development\gpssample\translations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cdc.sharepoint.com/teams/CGH-GPSSample/Shared Documents/General/Bolivia/App_Translation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA288CA-BBAE-4D72-9D2B-1C2581202596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{BBA288CA-BBAE-4D72-9D2B-1C2581202596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6649869-17D5-489F-8C38-0413CBF145B2}"/>
   <bookViews>
-    <workbookView xWindow="6375" yWindow="765" windowWidth="21600" windowHeight="13185" xr2:uid="{C8C8ACD1-4E76-7942-B525-8D880B4ECA80}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C8C8ACD1-4E76-7942-B525-8D880B4ECA80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="910">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="1052">
   <si>
     <t>Settings</t>
   </si>
@@ -2783,14 +2783,447 @@
   <si>
     <t>&gt;Location not found</t>
   </si>
+  <si>
+    <t>Importar datos de enumeración</t>
+  </si>
+  <si>
+    <t>Exportar configuración</t>
+  </si>
+  <si>
+    <t>¿Está seguro de que desea eliminar permanentemente este estudio?</t>
+  </si>
+  <si>
+    <t>¿Está seguro de que desea eliminar permanentemente este campo?</t>
+  </si>
+  <si>
+    <t>¿Está seguro de que desea eliminar permanentemente esta regla?</t>
+  </si>
+  <si>
+    <t>¿Está seguro de que desea eliminar permanentemente este equipo?</t>
+  </si>
+  <si>
+    <t>¿Está seguro de que desea eliminar permanentemente esta configuración?</t>
+  </si>
+  <si>
+    <t>¿Está seguro de que desea eliminar permanentemente este hogar?</t>
+  </si>
+  <si>
+    <t>Debe crear al menos un campo antes de poder crear una regla</t>
+  </si>
+  <si>
+    <t>Debe crear al menos una regla antes de poder crear un filtro</t>
+  </si>
+  <si>
+    <t>Seleccione un método de importación</t>
+  </si>
+  <si>
+    <t>Seleccione un método de exportación</t>
+  </si>
+  <si>
+    <t>¿Está seguro de que desea borrar todas las selecciones?</t>
+  </si>
+  <si>
+    <t>Debe introducir un nombre de equipo</t>
+  </si>
+  <si>
+    <t>La configuración se ha guardado en el directorio Documentos.</t>
+  </si>
+  <si>
+    <t>¿Está seguro de que desea borrar permanentemente el Área de Enumeración?</t>
+  </si>
+  <si>
+    <t>Introduzca un nombre de archivo para la exportación</t>
+  </si>
+  <si>
+    <t>¡Ups! La importación ha fallado.  Vuelva a intentarlo.</t>
+  </si>
+  <si>
+    <t>Seleccione una tarea</t>
+  </si>
+  <si>
+    <t>Sí</t>
+  </si>
+  <si>
+    <t>Código QR</t>
+  </si>
+  <si>
+    <t>Sistema de archivos</t>
+  </si>
+  <si>
+    <t>Encuesta</t>
+  </si>
+  <si>
+    <t>Sin definir</t>
+  </si>
+  <si>
+    <t>Configuración de importación</t>
+  </si>
+  <si>
+    <t>Seleccione una configuración</t>
+  </si>
+  <si>
+    <t>Exportar datos de enumeración</t>
+  </si>
+  <si>
+    <t>Los datos de enumeración se han guardado en el directorio Documentos.</t>
+  </si>
+  <si>
+    <t>&gt;Localización no encontrada</t>
+  </si>
+  <si>
+    <t>¡Oops! Por favor, seleccione una razón para incompleto</t>
+  </si>
+  <si>
+    <t>Importer les données d'énumération</t>
+  </si>
+  <si>
+    <t>Exporter la configuration</t>
+  </si>
+  <si>
+    <t>Êtes-vous sûr de vouloir supprimer définitivement cette étude ?</t>
+  </si>
+  <si>
+    <t>Êtes-vous sûr de vouloir supprimer définitivement ce champ ?</t>
+  </si>
+  <si>
+    <t>Êtes-vous sûr de vouloir supprimer définitivement cette règle ?</t>
+  </si>
+  <si>
+    <t>Êtes-vous sûr de vouloir supprimer définitivement cette équipe ?</t>
+  </si>
+  <si>
+    <t>Êtes-vous sûr de vouloir supprimer définitivement cette configuration ?</t>
+  </si>
+  <si>
+    <t>Êtes-vous sûr de vouloir supprimer définitivement ce ménage ?</t>
+  </si>
+  <si>
+    <t>Vous devez créer au moins un champ avant de pouvoir créer une règle.</t>
+  </si>
+  <si>
+    <t>Vous devez créer au moins une règle avant de pouvoir créer un filtre</t>
+  </si>
+  <si>
+    <t>Sélectionner une méthode d'importation</t>
+  </si>
+  <si>
+    <t>Sélectionnez une méthode d'exportation</t>
+  </si>
+  <si>
+    <t>Etes-vous sûr de vouloir effacer toutes les sélections ?</t>
+  </si>
+  <si>
+    <t>Vous devez saisir un nom d'équipe</t>
+  </si>
+  <si>
+    <t>La configuration a été sauvegardée dans le répertoire Documents.</t>
+  </si>
+  <si>
+    <t>Etes-vous sûr de vouloir supprimer définitivement la zone de dénombrement ?</t>
+  </si>
+  <si>
+    <t>Vous n'avez pas d'étude associée à cette zone de dénombrement.</t>
+  </si>
+  <si>
+    <t>Entrez un nom de fichier pour l'exportation</t>
+  </si>
+  <si>
+    <t>Oups ! L'importation a échoué.  Veuillez réessayer.</t>
+  </si>
+  <si>
+    <t>Sélectionner une tâche</t>
+  </si>
+  <si>
+    <t>Oui</t>
+  </si>
+  <si>
+    <t>Non</t>
+  </si>
+  <si>
+    <t>Code QR</t>
+  </si>
+  <si>
+    <t>Système de fichiers</t>
+  </si>
+  <si>
+    <t>Enquête</t>
+  </si>
+  <si>
+    <t>Non défini</t>
+  </si>
+  <si>
+    <t>Veuillez saisir un nom</t>
+  </si>
+  <si>
+    <t>Veuillez saisir la précision GPS minimale souhaitée</t>
+  </si>
+  <si>
+    <t>Configuration de l'importation</t>
+  </si>
+  <si>
+    <t>Sélectionnez une méthode d'importation</t>
+  </si>
+  <si>
+    <t>Sélectionner une configuration</t>
+  </si>
+  <si>
+    <t>Exporter les données de dénombrement</t>
+  </si>
+  <si>
+    <t>Les données d'énumération ont été sauvegardées dans le répertoire Documents.</t>
+  </si>
+  <si>
+    <t>&gt;La configuration a été sauvegardée dans le répertoire Documents.</t>
+  </si>
+  <si>
+    <t>Le domicile n'existe pas</t>
+  </si>
+  <si>
+    <t>Oups ! Veuillez sélectionner une raison pour l'incomplétude</t>
+  </si>
+  <si>
+    <t>Importar dados de enumeração</t>
+  </si>
+  <si>
+    <t>Exportar configuração</t>
+  </si>
+  <si>
+    <t>A configuração foi guardada no diretório Documentos.</t>
+  </si>
+  <si>
+    <t>Oops! A importação falhou.  Por favor, tente novamente.</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>Sistema de ficheiros</t>
+  </si>
+  <si>
+    <t>Indefinido</t>
+  </si>
+  <si>
+    <t>Configuração de importação</t>
+  </si>
+  <si>
+    <t>Exportar dados de enumeração</t>
+  </si>
+  <si>
+    <t>Os dados de enumeração foram guardados no diretório Documentos.</t>
+  </si>
+  <si>
+    <t>&gt;Localização não encontrada</t>
+  </si>
+  <si>
+    <t>Пожалуйста, подтвердите</t>
+  </si>
+  <si>
+    <t>Импорт данных перечисления</t>
+  </si>
+  <si>
+    <t>Экспорт конфигурации</t>
+  </si>
+  <si>
+    <t>Вы уверены, что хотите безвозвратно удалить это исследование?</t>
+  </si>
+  <si>
+    <t>Вы уверены, что хотите безвозвратно удалить это поле?</t>
+  </si>
+  <si>
+    <t>Вы уверены, что хотите навсегда удалить это правило?</t>
+  </si>
+  <si>
+    <t>Вы уверены, что хотите навсегда удалить эту команду?</t>
+  </si>
+  <si>
+    <t>Вы уверены, что хотите навсегда удалить эту конфигурацию?</t>
+  </si>
+  <si>
+    <t>Вы уверены, что хотите навсегда удалить это домохозяйство?</t>
+  </si>
+  <si>
+    <t>Перед созданием правила необходимо создать хотя бы одно поле</t>
+  </si>
+  <si>
+    <t>Перед созданием фильтра необходимо создать хотя бы одно правило</t>
+  </si>
+  <si>
+    <t>Выберите метод импорта</t>
+  </si>
+  <si>
+    <t>Выберите метод экспорта</t>
+  </si>
+  <si>
+    <t>Вы уверены, что хотите снять все выделения?</t>
+  </si>
+  <si>
+    <t>Необходимо ввести имя команды</t>
+  </si>
+  <si>
+    <t>Конфигурация была сохранена в директории Documents.</t>
+  </si>
+  <si>
+    <t>Вы уверены, что хотите навсегда удалить область пересчета</t>
+  </si>
+  <si>
+    <t>У вас нет исследования, связанного с этим экспертом.</t>
+  </si>
+  <si>
+    <t>Введите имя файла для экспорта</t>
+  </si>
+  <si>
+    <t>Упс! Импорт не удался.  Пожалуйста, попробуйте еще раз.</t>
+  </si>
+  <si>
+    <t>Выберите задачу</t>
+  </si>
+  <si>
+    <t>Да</t>
+  </si>
+  <si>
+    <t>Нет</t>
+  </si>
+  <si>
+    <t>QR-код</t>
+  </si>
+  <si>
+    <t>Файловая система</t>
+  </si>
+  <si>
+    <t>Опрос</t>
+  </si>
+  <si>
+    <t>Неопределенный</t>
+  </si>
+  <si>
+    <t>Пожалуйста, введите имя</t>
+  </si>
+  <si>
+    <t>Введите минимальную желаемую точность GPS</t>
+  </si>
+  <si>
+    <t>Конфигурация импорта</t>
+  </si>
+  <si>
+    <t>Выберите конфигурацию</t>
+  </si>
+  <si>
+    <t>Экспорт данных переписи</t>
+  </si>
+  <si>
+    <t>Данные переписи были сохранены в директории Documents.</t>
+  </si>
+  <si>
+    <t>Конфигурация была сохранена в каталог Documents.</t>
+  </si>
+  <si>
+    <t>&gt;Местонахождение не найдено</t>
+  </si>
+  <si>
+    <t>Дом не существует</t>
+  </si>
+  <si>
+    <t>Упс! Пожалуйста, выберите причину неполного заполнения</t>
+  </si>
+  <si>
+    <t>Por favor, confirme</t>
+  </si>
+  <si>
+    <t>No tiene ningún estudio asociado a esta Área de Enumeración.</t>
+  </si>
+  <si>
+    <t>Por favor, introduzca un nombre</t>
+  </si>
+  <si>
+    <t>Por favor, introduzca la precisión GPS mínima deseada</t>
+  </si>
+  <si>
+    <t>SVP, veuillez confirmer</t>
+  </si>
+  <si>
+    <t>Tem a certeza de que deseja eliminar permanentemente este estudo?</t>
+  </si>
+  <si>
+    <t>Tem a certeza de que deseja eliminar permanentemente este campo?</t>
+  </si>
+  <si>
+    <t>Tem a certeza de que deseja eliminar permanentemente esta regra?</t>
+  </si>
+  <si>
+    <t>Tem a certeza de que deseja eliminar permanentemente esta equipa?</t>
+  </si>
+  <si>
+    <t>Tem a certeza de que deseja eliminar permanentemente esta configuração?</t>
+  </si>
+  <si>
+    <t>Tem a certeza de que deseja eliminar permanentemente este agregado familiar?</t>
+  </si>
+  <si>
+    <t>Você deve criar pelo menos um campo antes de criar uma regra</t>
+  </si>
+  <si>
+    <t>Selecione um método de importação</t>
+  </si>
+  <si>
+    <t>Selecione um método de exportação</t>
+  </si>
+  <si>
+    <t>Tem a certeza de que deseja apagar todas as selecções?</t>
+  </si>
+  <si>
+    <t>Você deve inserir um nome de equipe</t>
+  </si>
+  <si>
+    <t>Tem a certeza de que deseja eliminar permanentemente a Área de Enumeração</t>
+  </si>
+  <si>
+    <t>Não tem um estudo associado a esta Área de Enumeração.</t>
+  </si>
+  <si>
+    <t>Insira um nome de ficheiro para a exportação</t>
+  </si>
+  <si>
+    <t>Selecione uma tarefa</t>
+  </si>
+  <si>
+    <t>Questionário</t>
+  </si>
+  <si>
+    <t>Por favor, insira um nome</t>
+  </si>
+  <si>
+    <t>Por favor, insira a precisão GPS mínima pretendida</t>
+  </si>
+  <si>
+    <t>Selecione uma configuração</t>
+  </si>
+  <si>
+    <t>Oops! Por favor, seleccione um razão para incompleto</t>
+  </si>
+  <si>
+    <t>O agregado familiar não existe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La hogar no existe </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2824,12 +3257,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2844,17 +3283,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3171,20 +3612,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD3E6CC-854C-5841-9577-D3ADD2982DB6}">
   <dimension ref="A1:F189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A149" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B146" sqref="B146"/>
+    <sheetView tabSelected="1" topLeftCell="C174" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C189" sqref="C189"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="52" customWidth="1"/>
     <col min="2" max="2" width="62" customWidth="1"/>
-    <col min="3" max="3" width="48.375" customWidth="1"/>
+    <col min="3" max="3" width="48.33203125" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
-    <col min="5" max="5" width="41.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>145</v>
       </c>
@@ -3204,7 +3645,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>146</v>
       </c>
@@ -3224,7 +3665,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>147</v>
       </c>
@@ -3244,7 +3685,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>148</v>
       </c>
@@ -3264,7 +3705,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>149</v>
       </c>
@@ -3284,7 +3725,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>150</v>
       </c>
@@ -3304,7 +3745,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>151</v>
       </c>
@@ -3324,7 +3765,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>152</v>
       </c>
@@ -3344,7 +3785,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>153</v>
       </c>
@@ -3364,7 +3805,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>154</v>
       </c>
@@ -3384,7 +3825,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>155</v>
       </c>
@@ -3404,7 +3845,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>156</v>
       </c>
@@ -3424,7 +3865,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>157</v>
       </c>
@@ -3444,7 +3885,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>158</v>
       </c>
@@ -3464,7 +3905,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>159</v>
       </c>
@@ -3484,7 +3925,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>160</v>
       </c>
@@ -3504,7 +3945,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>161</v>
       </c>
@@ -3524,7 +3965,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>162</v>
       </c>
@@ -3544,7 +3985,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>162</v>
       </c>
@@ -3564,7 +4005,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>162</v>
       </c>
@@ -3584,7 +4025,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>162</v>
       </c>
@@ -3604,7 +4045,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>162</v>
       </c>
@@ -3624,7 +4065,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>162</v>
       </c>
@@ -3644,7 +4085,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>162</v>
       </c>
@@ -3664,7 +4105,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>833</v>
       </c>
@@ -3684,7 +4125,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>833</v>
       </c>
@@ -3704,7 +4145,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>834</v>
       </c>
@@ -3724,7 +4165,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>834</v>
       </c>
@@ -3744,7 +4185,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>164</v>
       </c>
@@ -3764,7 +4205,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>164</v>
       </c>
@@ -3784,7 +4225,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>164</v>
       </c>
@@ -3804,7 +4245,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>164</v>
       </c>
@@ -3824,7 +4265,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>164</v>
       </c>
@@ -3844,7 +4285,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>165</v>
       </c>
@@ -3864,7 +4305,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>165</v>
       </c>
@@ -3884,7 +4325,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>165</v>
       </c>
@@ -3904,7 +4345,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>165</v>
       </c>
@@ -3924,7 +4365,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>165</v>
       </c>
@@ -3944,7 +4385,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>166</v>
       </c>
@@ -3964,7 +4405,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>166</v>
       </c>
@@ -3984,7 +4425,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>166</v>
       </c>
@@ -4004,7 +4445,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>167</v>
       </c>
@@ -4024,7 +4465,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>167</v>
       </c>
@@ -4044,7 +4485,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>167</v>
       </c>
@@ -4064,7 +4505,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>167</v>
       </c>
@@ -4084,7 +4525,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>168</v>
       </c>
@@ -4104,7 +4545,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>169</v>
       </c>
@@ -4124,7 +4565,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>170</v>
       </c>
@@ -4144,7 +4585,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>171</v>
       </c>
@@ -4164,7 +4605,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>174</v>
       </c>
@@ -4184,7 +4625,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>175</v>
       </c>
@@ -4204,7 +4645,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>176</v>
       </c>
@@ -4224,7 +4665,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>177</v>
       </c>
@@ -4244,7 +4685,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>178</v>
       </c>
@@ -4264,7 +4705,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>179</v>
       </c>
@@ -4284,7 +4725,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>180</v>
       </c>
@@ -4304,7 +4745,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>181</v>
       </c>
@@ -4324,7 +4765,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>182</v>
       </c>
@@ -4344,7 +4785,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>183</v>
       </c>
@@ -4364,7 +4805,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>184</v>
       </c>
@@ -4384,7 +4825,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>185</v>
       </c>
@@ -4404,7 +4845,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>186</v>
       </c>
@@ -4424,7 +4865,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>187</v>
       </c>
@@ -4444,7 +4885,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>188</v>
       </c>
@@ -4464,7 +4905,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>189</v>
       </c>
@@ -4484,7 +4925,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>190</v>
       </c>
@@ -4504,7 +4945,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>191</v>
       </c>
@@ -4524,7 +4965,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>192</v>
       </c>
@@ -4544,7 +4985,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>193</v>
       </c>
@@ -4564,7 +5005,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>194</v>
       </c>
@@ -4584,7 +5025,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>195</v>
       </c>
@@ -4604,7 +5045,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>196</v>
       </c>
@@ -4624,7 +5065,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>197</v>
       </c>
@@ -4644,7 +5085,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>198</v>
       </c>
@@ -4664,7 +5105,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>199</v>
       </c>
@@ -4684,7 +5125,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>200</v>
       </c>
@@ -4704,7 +5145,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>201</v>
       </c>
@@ -4724,7 +5165,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>202</v>
       </c>
@@ -4744,7 +5185,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>203</v>
       </c>
@@ -4764,7 +5205,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>204</v>
       </c>
@@ -4784,7 +5225,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>205</v>
       </c>
@@ -4804,7 +5245,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>206</v>
       </c>
@@ -4824,7 +5265,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>207</v>
       </c>
@@ -4844,7 +5285,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>208</v>
       </c>
@@ -4864,7 +5305,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>209</v>
       </c>
@@ -4884,7 +5325,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>210</v>
       </c>
@@ -4904,7 +5345,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>211</v>
       </c>
@@ -4924,7 +5365,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>212</v>
       </c>
@@ -4944,7 +5385,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>213</v>
       </c>
@@ -4964,7 +5405,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>214</v>
       </c>
@@ -4984,7 +5425,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>215</v>
       </c>
@@ -5004,7 +5445,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>216</v>
       </c>
@@ -5024,7 +5465,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>217</v>
       </c>
@@ -5044,7 +5485,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>218</v>
       </c>
@@ -5064,7 +5505,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>219</v>
       </c>
@@ -5084,7 +5525,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>220</v>
       </c>
@@ -5104,7 +5545,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>221</v>
       </c>
@@ -5124,7 +5565,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>163</v>
       </c>
@@ -5144,7 +5585,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>222</v>
       </c>
@@ -5164,7 +5605,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>223</v>
       </c>
@@ -5184,7 +5625,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>224</v>
       </c>
@@ -5204,7 +5645,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>225</v>
       </c>
@@ -5224,7 +5665,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>226</v>
       </c>
@@ -5244,7 +5685,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>227</v>
       </c>
@@ -5264,7 +5705,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>228</v>
       </c>
@@ -5284,7 +5725,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>229</v>
       </c>
@@ -5304,7 +5745,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>230</v>
       </c>
@@ -5324,7 +5765,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>231</v>
       </c>
@@ -5344,7 +5785,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>232</v>
       </c>
@@ -5364,7 +5805,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>233</v>
       </c>
@@ -5384,7 +5825,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>234</v>
       </c>
@@ -5404,7 +5845,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>235</v>
       </c>
@@ -5424,7 +5865,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>236</v>
       </c>
@@ -5444,7 +5885,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>237</v>
       </c>
@@ -5464,7 +5905,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>238</v>
       </c>
@@ -5484,7 +5925,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>239</v>
       </c>
@@ -5504,7 +5945,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>240</v>
       </c>
@@ -5524,7 +5965,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>241</v>
       </c>
@@ -5544,7 +5985,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>242</v>
       </c>
@@ -5564,7 +6005,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>243</v>
       </c>
@@ -5584,7 +6025,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>244</v>
       </c>
@@ -5604,7 +6045,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>245</v>
       </c>
@@ -5624,7 +6065,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>246</v>
       </c>
@@ -5644,7 +6085,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>247</v>
       </c>
@@ -5664,7 +6105,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>248</v>
       </c>
@@ -5684,7 +6125,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>249</v>
       </c>
@@ -5704,7 +6145,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>250</v>
       </c>
@@ -5724,7 +6165,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>251</v>
       </c>
@@ -5744,7 +6185,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>252</v>
       </c>
@@ -5764,7 +6205,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>253</v>
       </c>
@@ -5784,7 +6225,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>254</v>
       </c>
@@ -5804,7 +6245,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>255</v>
       </c>
@@ -5824,7 +6265,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>256</v>
       </c>
@@ -5844,7 +6285,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>257</v>
       </c>
@@ -5864,7 +6305,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>258</v>
       </c>
@@ -5884,7 +6325,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>259</v>
       </c>
@@ -5904,7 +6345,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>260</v>
       </c>
@@ -5924,7 +6365,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>261</v>
       </c>
@@ -5944,7 +6385,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>262</v>
       </c>
@@ -5964,7 +6405,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>263</v>
       </c>
@@ -5984,7 +6425,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>264</v>
       </c>
@@ -6004,7 +6445,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>265</v>
       </c>
@@ -6024,7 +6465,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>266</v>
       </c>
@@ -6044,7 +6485,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>267</v>
       </c>
@@ -6064,7 +6505,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>268</v>
       </c>
@@ -6084,7 +6525,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>269</v>
       </c>
@@ -6104,7 +6545,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>270</v>
       </c>
@@ -6124,7 +6565,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>271</v>
       </c>
@@ -6144,7 +6585,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>272</v>
       </c>
@@ -6164,7 +6605,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>273</v>
       </c>
@@ -6184,316 +6625,784 @@
         <v>647</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151" s="4" t="s">
         <v>835</v>
       </c>
       <c r="B151" s="5" t="s">
         <v>908</v>
       </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C151" t="s">
+        <v>1025</v>
+      </c>
+      <c r="D151" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E151" t="s">
+        <v>1025</v>
+      </c>
+      <c r="F151" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152" s="4" t="s">
         <v>836</v>
       </c>
       <c r="B152" s="5" t="s">
         <v>907</v>
       </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C152" t="s">
+        <v>910</v>
+      </c>
+      <c r="D152" t="s">
+        <v>940</v>
+      </c>
+      <c r="E152" t="s">
+        <v>976</v>
+      </c>
+      <c r="F152" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153" s="4" t="s">
         <v>837</v>
       </c>
       <c r="B153" s="5" t="s">
         <v>906</v>
       </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C153" t="s">
+        <v>911</v>
+      </c>
+      <c r="D153" t="s">
+        <v>941</v>
+      </c>
+      <c r="E153" t="s">
+        <v>977</v>
+      </c>
+      <c r="F153" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A154" s="4" t="s">
         <v>838</v>
       </c>
       <c r="B154" s="5" t="s">
         <v>905</v>
       </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C154" t="s">
+        <v>912</v>
+      </c>
+      <c r="D154" t="s">
+        <v>942</v>
+      </c>
+      <c r="E154" t="s">
+        <v>1030</v>
+      </c>
+      <c r="F154" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A155" s="4" t="s">
         <v>839</v>
       </c>
       <c r="B155" s="5" t="s">
         <v>904</v>
       </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C155" t="s">
+        <v>913</v>
+      </c>
+      <c r="D155" t="s">
+        <v>943</v>
+      </c>
+      <c r="E155" t="s">
+        <v>1031</v>
+      </c>
+      <c r="F155" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A156" s="4" t="s">
         <v>840</v>
       </c>
       <c r="B156" s="5" t="s">
         <v>903</v>
       </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C156" t="s">
+        <v>914</v>
+      </c>
+      <c r="D156" t="s">
+        <v>944</v>
+      </c>
+      <c r="E156" t="s">
+        <v>1032</v>
+      </c>
+      <c r="F156" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A157" s="4" t="s">
         <v>841</v>
       </c>
       <c r="B157" s="5" t="s">
         <v>902</v>
       </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C157" t="s">
+        <v>915</v>
+      </c>
+      <c r="D157" t="s">
+        <v>945</v>
+      </c>
+      <c r="E157" t="s">
+        <v>1033</v>
+      </c>
+      <c r="F157" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158" s="4" t="s">
         <v>842</v>
       </c>
       <c r="B158" s="5" t="s">
         <v>901</v>
       </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C158" t="s">
+        <v>916</v>
+      </c>
+      <c r="D158" t="s">
+        <v>946</v>
+      </c>
+      <c r="E158" t="s">
+        <v>1034</v>
+      </c>
+      <c r="F158" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A159" s="4" t="s">
         <v>843</v>
       </c>
       <c r="B159" s="5" t="s">
         <v>900</v>
       </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C159" t="s">
+        <v>917</v>
+      </c>
+      <c r="D159" t="s">
+        <v>947</v>
+      </c>
+      <c r="E159" t="s">
+        <v>1035</v>
+      </c>
+      <c r="F159" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A160" s="4" t="s">
         <v>844</v>
       </c>
       <c r="B160" s="5" t="s">
         <v>899</v>
       </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C160" t="s">
+        <v>918</v>
+      </c>
+      <c r="D160" t="s">
+        <v>948</v>
+      </c>
+      <c r="E160" t="s">
+        <v>1036</v>
+      </c>
+      <c r="F160" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161" s="4" t="s">
         <v>845</v>
       </c>
       <c r="B161" s="5" t="s">
         <v>898</v>
       </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C161" t="s">
+        <v>919</v>
+      </c>
+      <c r="D161" t="s">
+        <v>949</v>
+      </c>
+      <c r="E161" t="s">
+        <v>1036</v>
+      </c>
+      <c r="F161" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A162" s="4" t="s">
         <v>846</v>
       </c>
       <c r="B162" s="5" t="s">
         <v>880</v>
       </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C162" t="s">
+        <v>920</v>
+      </c>
+      <c r="D162" t="s">
+        <v>950</v>
+      </c>
+      <c r="E162" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F162" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A163" s="4" t="s">
         <v>847</v>
       </c>
       <c r="B163" s="5" t="s">
         <v>897</v>
       </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C163" t="s">
+        <v>921</v>
+      </c>
+      <c r="D163" t="s">
+        <v>951</v>
+      </c>
+      <c r="E163" t="s">
+        <v>1038</v>
+      </c>
+      <c r="F163" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A164" s="4" t="s">
         <v>848</v>
       </c>
       <c r="B164" s="5" t="s">
         <v>896</v>
       </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C164" t="s">
+        <v>922</v>
+      </c>
+      <c r="D164" t="s">
+        <v>952</v>
+      </c>
+      <c r="E164" t="s">
+        <v>1039</v>
+      </c>
+      <c r="F164" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A165" s="4" t="s">
         <v>849</v>
       </c>
       <c r="B165" s="5" t="s">
         <v>895</v>
       </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C165" t="s">
+        <v>923</v>
+      </c>
+      <c r="D165" t="s">
+        <v>953</v>
+      </c>
+      <c r="E165" t="s">
+        <v>1040</v>
+      </c>
+      <c r="F165" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A166" s="4" t="s">
         <v>850</v>
       </c>
       <c r="B166" s="5" t="s">
         <v>876</v>
       </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C166" t="s">
+        <v>924</v>
+      </c>
+      <c r="D166" t="s">
+        <v>954</v>
+      </c>
+      <c r="E166" t="s">
+        <v>978</v>
+      </c>
+      <c r="F166" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A167" s="4" t="s">
         <v>851</v>
       </c>
       <c r="B167" s="5" t="s">
         <v>894</v>
       </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C167" t="s">
+        <v>925</v>
+      </c>
+      <c r="D167" t="s">
+        <v>955</v>
+      </c>
+      <c r="E167" t="s">
+        <v>1041</v>
+      </c>
+      <c r="F167" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A168" s="4" t="s">
         <v>852</v>
       </c>
       <c r="B168" s="5" t="s">
         <v>892</v>
       </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C168" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D168" t="s">
+        <v>956</v>
+      </c>
+      <c r="E168" t="s">
+        <v>1042</v>
+      </c>
+      <c r="F168" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A169" s="4" t="s">
         <v>853</v>
       </c>
       <c r="B169" s="5" t="s">
         <v>893</v>
       </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C169" t="s">
+        <v>926</v>
+      </c>
+      <c r="D169" t="s">
+        <v>957</v>
+      </c>
+      <c r="E169" t="s">
+        <v>1043</v>
+      </c>
+      <c r="F169" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A170" s="4" t="s">
         <v>854</v>
       </c>
       <c r="B170" s="5" t="s">
         <v>891</v>
       </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C170" t="s">
+        <v>927</v>
+      </c>
+      <c r="D170" t="s">
+        <v>958</v>
+      </c>
+      <c r="E170" t="s">
+        <v>979</v>
+      </c>
+      <c r="F170" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A171" s="4" t="s">
         <v>855</v>
       </c>
       <c r="B171" s="5" t="s">
         <v>890</v>
       </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C171" t="s">
+        <v>928</v>
+      </c>
+      <c r="D171" t="s">
+        <v>959</v>
+      </c>
+      <c r="E171" t="s">
+        <v>1044</v>
+      </c>
+      <c r="F171" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A172" s="4" t="s">
         <v>856</v>
       </c>
-      <c r="B172" s="1" t="s">
+      <c r="B172" s="6" t="s">
         <v>889</v>
       </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C172" t="s">
+        <v>929</v>
+      </c>
+      <c r="D172" t="s">
+        <v>960</v>
+      </c>
+      <c r="E172" t="s">
+        <v>980</v>
+      </c>
+      <c r="F172" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A173" s="4" t="s">
         <v>857</v>
       </c>
       <c r="B173" s="5" t="s">
         <v>888</v>
       </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C173" t="s">
+        <v>888</v>
+      </c>
+      <c r="D173" t="s">
+        <v>961</v>
+      </c>
+      <c r="E173" t="s">
+        <v>981</v>
+      </c>
+      <c r="F173" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A174" s="4" t="s">
         <v>858</v>
       </c>
       <c r="B174" s="5" t="s">
         <v>887</v>
       </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C174" t="s">
+        <v>930</v>
+      </c>
+      <c r="D174" t="s">
+        <v>962</v>
+      </c>
+      <c r="E174" t="s">
+        <v>930</v>
+      </c>
+      <c r="F174" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A175" s="4" t="s">
         <v>859</v>
       </c>
       <c r="B175" s="5" t="s">
         <v>886</v>
       </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C175" t="s">
+        <v>931</v>
+      </c>
+      <c r="D175" t="s">
+        <v>963</v>
+      </c>
+      <c r="E175" t="s">
+        <v>982</v>
+      </c>
+      <c r="F175" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A176" s="4" t="s">
         <v>860</v>
       </c>
       <c r="B176" s="5" t="s">
         <v>885</v>
       </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C176" t="s">
+        <v>932</v>
+      </c>
+      <c r="D176" t="s">
+        <v>964</v>
+      </c>
+      <c r="E176" t="s">
+        <v>1045</v>
+      </c>
+      <c r="F176" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A177" s="4" t="s">
         <v>861</v>
       </c>
       <c r="B177" s="5" t="s">
         <v>884</v>
       </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C177" t="s">
+        <v>933</v>
+      </c>
+      <c r="D177" t="s">
+        <v>965</v>
+      </c>
+      <c r="E177" t="s">
+        <v>983</v>
+      </c>
+      <c r="F177" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A178" s="4" t="s">
         <v>862</v>
       </c>
       <c r="B178" s="5" t="s">
         <v>883</v>
       </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C178" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D178" t="s">
+        <v>966</v>
+      </c>
+      <c r="E178" t="s">
+        <v>1046</v>
+      </c>
+      <c r="F178" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A179" s="4" t="s">
         <v>863</v>
       </c>
       <c r="B179" s="5" t="s">
         <v>882</v>
       </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C179" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D179" t="s">
+        <v>967</v>
+      </c>
+      <c r="E179" t="s">
+        <v>1047</v>
+      </c>
+      <c r="F179" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A180" s="4" t="s">
         <v>864</v>
       </c>
       <c r="B180" s="5" t="s">
         <v>881</v>
       </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C180" t="s">
+        <v>934</v>
+      </c>
+      <c r="D180" t="s">
+        <v>968</v>
+      </c>
+      <c r="E180" t="s">
+        <v>984</v>
+      </c>
+      <c r="F180" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A181" s="4" t="s">
         <v>865</v>
       </c>
       <c r="B181" s="5" t="s">
         <v>880</v>
       </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C181" t="s">
+        <v>920</v>
+      </c>
+      <c r="D181" t="s">
+        <v>969</v>
+      </c>
+      <c r="E181" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F181" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A182" s="4" t="s">
         <v>866</v>
       </c>
       <c r="B182" s="5" t="s">
         <v>879</v>
       </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C182" t="s">
+        <v>935</v>
+      </c>
+      <c r="D182" t="s">
+        <v>970</v>
+      </c>
+      <c r="E182" t="s">
+        <v>1048</v>
+      </c>
+      <c r="F182" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A183" s="4" t="s">
         <v>867</v>
       </c>
       <c r="B183" s="5" t="s">
         <v>879</v>
       </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C183" t="s">
+        <v>935</v>
+      </c>
+      <c r="D183" t="s">
+        <v>970</v>
+      </c>
+      <c r="E183" t="s">
+        <v>1048</v>
+      </c>
+      <c r="F183" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A184" s="4" t="s">
         <v>868</v>
       </c>
       <c r="B184" s="5" t="s">
         <v>878</v>
       </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C184" t="s">
+        <v>936</v>
+      </c>
+      <c r="D184" t="s">
+        <v>971</v>
+      </c>
+      <c r="E184" t="s">
+        <v>985</v>
+      </c>
+      <c r="F184" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A185" s="4" t="s">
         <v>869</v>
       </c>
       <c r="B185" s="5" t="s">
         <v>877</v>
       </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C185" t="s">
+        <v>937</v>
+      </c>
+      <c r="D185" t="s">
+        <v>972</v>
+      </c>
+      <c r="E185" t="s">
+        <v>986</v>
+      </c>
+      <c r="F185" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A186" s="4" t="s">
         <v>870</v>
       </c>
       <c r="B186" s="5" t="s">
         <v>876</v>
       </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C186" t="s">
+        <v>924</v>
+      </c>
+      <c r="D186" t="s">
+        <v>954</v>
+      </c>
+      <c r="E186" t="s">
+        <v>978</v>
+      </c>
+      <c r="F186" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A187" s="4" t="s">
         <v>871</v>
       </c>
       <c r="B187" s="5" t="s">
         <v>909</v>
       </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C187" t="s">
+        <v>938</v>
+      </c>
+      <c r="D187" t="s">
+        <v>973</v>
+      </c>
+      <c r="E187" t="s">
+        <v>987</v>
+      </c>
+      <c r="F187" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A188" s="4" t="s">
         <v>872</v>
       </c>
       <c r="B188" s="5" t="s">
         <v>875</v>
       </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C188" s="7" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D188" t="s">
+        <v>974</v>
+      </c>
+      <c r="E188" s="7" t="s">
+        <v>1050</v>
+      </c>
+      <c r="F188" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A189" s="4" t="s">
         <v>873</v>
       </c>
       <c r="B189" s="5" t="s">
         <v>874</v>
+      </c>
+      <c r="C189" t="s">
+        <v>939</v>
+      </c>
+      <c r="D189" t="s">
+        <v>975</v>
+      </c>
+      <c r="E189" t="s">
+        <v>1049</v>
+      </c>
+      <c r="F189" t="s">
+        <v>1024</v>
       </c>
     </row>
   </sheetData>
@@ -6503,19 +7412,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="6e0cf07b-8188-4b76-8f54-3cda03d37414" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="43e153a8-5ef1-4f65-aac7-dc4685f18eaa">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F12BE0DB4A3DF641BF113FBF1C7EA261" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c8be6a489b436af36cb92f29085c3c08">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="43e153a8-5ef1-4f65-aac7-dc4685f18eaa" xmlns:ns3="6e0cf07b-8188-4b76-8f54-3cda03d37414" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="66c1592365447f698e441c0cbf70562a" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F12BE0DB4A3DF641BF113FBF1C7EA261" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="718598463bd34fa12e450bcb3a6783b8">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="43e153a8-5ef1-4f65-aac7-dc4685f18eaa" xmlns:ns3="6e0cf07b-8188-4b76-8f54-3cda03d37414" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="54cbcd1ebcb6479b13808205dc2a6520" ns2:_="" ns3:_="">
     <xsd:import namespace="43e153a8-5ef1-4f65-aac7-dc4685f18eaa"/>
     <xsd:import namespace="6e0cf07b-8188-4b76-8f54-3cda03d37414"/>
     <xsd:element name="properties">
@@ -6535,6 +7433,8 @@
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -6587,6 +7487,16 @@
     <xsd:element name="MediaServiceLocation" ma:index="19" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="20" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="21" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -6730,6 +7640,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="6e0cf07b-8188-4b76-8f54-3cda03d37414" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="43e153a8-5ef1-4f65-aac7-dc4685f18eaa">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -6740,24 +7661,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E20926E-9EFB-4B7E-90D4-905B08F8E59C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="6e0cf07b-8188-4b76-8f54-3cda03d37414"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="43e153a8-5ef1-4f65-aac7-dc4685f18eaa"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C30A135-2C3F-4204-8766-0B8E815003D7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBDDFBA8-FF97-4684-8DBF-782A9A0E4D0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -6775,6 +7679,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E20926E-9EFB-4B7E-90D4-905B08F8E59C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6e0cf07b-8188-4b76-8f54-3cda03d37414"/>
+    <ds:schemaRef ds:uri="43e153a8-5ef1-4f65-aac7-dc4685f18eaa"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04FEE910-FEC8-48C6-9CF9-BF01BA5AD6FE}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
removed MORE hard coded strings......
</commit_message>
<xml_diff>
--- a/translations/translations.xlsx
+++ b/translations/translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cdc.sharepoint.com/teams/CGH-GPSSample/Shared Documents/General/Bolivia/App_Translation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bp51/Development/GTRI/Android/gpssample/translations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{BBA288CA-BBAE-4D72-9D2B-1C2581202596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6649869-17D5-489F-8C38-0413CBF145B2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBF2040-1CB0-8C40-9A9B-AB703C33B5D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C8C8ACD1-4E76-7942-B525-8D880B4ECA80}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="29220" windowHeight="18960" xr2:uid="{C8C8ACD1-4E76-7942-B525-8D880B4ECA80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="1052">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="1083">
   <si>
     <t>Settings</t>
   </si>
@@ -3208,6 +3208,99 @@
   </si>
   <si>
     <t xml:space="preserve">La hogar no existe </t>
+  </si>
+  <si>
+    <t>enter_enum_area_name</t>
+  </si>
+  <si>
+    <t>select_enumeration</t>
+  </si>
+  <si>
+    <t>select_time</t>
+  </si>
+  <si>
+    <t>select_date</t>
+  </si>
+  <si>
+    <t>your_pin_is</t>
+  </si>
+  <si>
+    <t>incorrect_answer_message</t>
+  </si>
+  <si>
+    <t>enter_other_question</t>
+  </si>
+  <si>
+    <t>reenter_pin</t>
+  </si>
+  <si>
+    <t>enter_pin</t>
+  </si>
+  <si>
+    <t>other_question</t>
+  </si>
+  <si>
+    <t>enter_answer</t>
+  </si>
+  <si>
+    <t>pin_not_match</t>
+  </si>
+  <si>
+    <t>enter_file_name</t>
+  </si>
+  <si>
+    <t>pin_incorrect</t>
+  </si>
+  <si>
+    <t>config_not_found</t>
+  </si>
+  <si>
+    <t>missing_parameter_rule</t>
+  </si>
+  <si>
+    <t>Fatal! Missing required parameter: role</t>
+  </si>
+  <si>
+    <t>Fatal! Config not found.</t>
+  </si>
+  <si>
+    <t>The current PIN is incorrect</t>
+  </si>
+  <si>
+    <t>You must enter a file name</t>
+  </si>
+  <si>
+    <t>The PIN's do not match</t>
+  </si>
+  <si>
+    <t>Please enter an answer.</t>
+  </si>
+  <si>
+    <t>Please enter a PIN</t>
+  </si>
+  <si>
+    <t>Please re-enter the PIN</t>
+  </si>
+  <si>
+    <t>Enter Other Question</t>
+  </si>
+  <si>
+    <t>Oops! Incorrect answer.  Please try again.</t>
+  </si>
+  <si>
+    <t>Your PIN is:</t>
+  </si>
+  <si>
+    <t>Select Date</t>
+  </si>
+  <si>
+    <t>Select Time</t>
+  </si>
+  <si>
+    <t>Select an Enumeration</t>
+  </si>
+  <si>
+    <t>Enter the Enumeration Area name</t>
   </si>
 </sst>
 </file>
@@ -3283,12 +3376,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3296,6 +3389,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3610,22 +3707,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD3E6CC-854C-5841-9577-D3ADD2982DB6}">
-  <dimension ref="A1:F189"/>
+  <dimension ref="A1:F205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C174" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C189" sqref="C189"/>
+    <sheetView tabSelected="1" topLeftCell="A172" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B208" sqref="B208"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="52" customWidth="1"/>
     <col min="2" max="2" width="62" customWidth="1"/>
     <col min="3" max="3" width="48.33203125" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
-    <col min="5" max="5" width="41.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>145</v>
       </c>
@@ -3645,7 +3742,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>146</v>
       </c>
@@ -3665,7 +3762,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>147</v>
       </c>
@@ -3685,7 +3782,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>148</v>
       </c>
@@ -3705,7 +3802,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>149</v>
       </c>
@@ -3725,7 +3822,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>150</v>
       </c>
@@ -3745,7 +3842,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>151</v>
       </c>
@@ -3765,7 +3862,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>152</v>
       </c>
@@ -3785,7 +3882,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>153</v>
       </c>
@@ -3805,7 +3902,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>154</v>
       </c>
@@ -3825,7 +3922,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>155</v>
       </c>
@@ -3845,7 +3942,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>156</v>
       </c>
@@ -3865,7 +3962,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>157</v>
       </c>
@@ -3885,7 +3982,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>158</v>
       </c>
@@ -3905,7 +4002,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>159</v>
       </c>
@@ -3925,7 +4022,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>160</v>
       </c>
@@ -3945,7 +4042,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>161</v>
       </c>
@@ -3965,7 +4062,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>162</v>
       </c>
@@ -3985,7 +4082,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>162</v>
       </c>
@@ -4005,7 +4102,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>162</v>
       </c>
@@ -4025,7 +4122,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>162</v>
       </c>
@@ -4045,7 +4142,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>162</v>
       </c>
@@ -4065,7 +4162,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>162</v>
       </c>
@@ -4085,7 +4182,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>162</v>
       </c>
@@ -4105,7 +4202,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>833</v>
       </c>
@@ -4125,7 +4222,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>833</v>
       </c>
@@ -4145,7 +4242,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>834</v>
       </c>
@@ -4165,7 +4262,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>834</v>
       </c>
@@ -4185,7 +4282,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>164</v>
       </c>
@@ -4205,7 +4302,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>164</v>
       </c>
@@ -4225,7 +4322,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>164</v>
       </c>
@@ -4245,7 +4342,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>164</v>
       </c>
@@ -4265,7 +4362,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>164</v>
       </c>
@@ -4285,7 +4382,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>165</v>
       </c>
@@ -4305,7 +4402,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>165</v>
       </c>
@@ -4325,7 +4422,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>165</v>
       </c>
@@ -4345,7 +4442,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>165</v>
       </c>
@@ -4365,7 +4462,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>165</v>
       </c>
@@ -4385,7 +4482,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>166</v>
       </c>
@@ -4405,7 +4502,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>166</v>
       </c>
@@ -4425,7 +4522,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>166</v>
       </c>
@@ -4445,7 +4542,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>167</v>
       </c>
@@ -4465,7 +4562,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>167</v>
       </c>
@@ -4485,7 +4582,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>167</v>
       </c>
@@ -4505,7 +4602,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>167</v>
       </c>
@@ -4525,7 +4622,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>168</v>
       </c>
@@ -4545,7 +4642,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>169</v>
       </c>
@@ -4565,7 +4662,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>170</v>
       </c>
@@ -4585,7 +4682,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>171</v>
       </c>
@@ -4605,7 +4702,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>174</v>
       </c>
@@ -4625,7 +4722,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>175</v>
       </c>
@@ -4645,7 +4742,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>176</v>
       </c>
@@ -4665,7 +4762,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>177</v>
       </c>
@@ -4685,7 +4782,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>178</v>
       </c>
@@ -4705,7 +4802,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>179</v>
       </c>
@@ -4725,7 +4822,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>180</v>
       </c>
@@ -4745,7 +4842,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>181</v>
       </c>
@@ -4765,7 +4862,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>182</v>
       </c>
@@ -4785,7 +4882,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>183</v>
       </c>
@@ -4805,7 +4902,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>184</v>
       </c>
@@ -4825,7 +4922,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>185</v>
       </c>
@@ -4845,7 +4942,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>186</v>
       </c>
@@ -4865,7 +4962,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>187</v>
       </c>
@@ -4885,7 +4982,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>188</v>
       </c>
@@ -4905,7 +5002,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>189</v>
       </c>
@@ -4925,7 +5022,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>190</v>
       </c>
@@ -4945,7 +5042,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>191</v>
       </c>
@@ -4965,7 +5062,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>192</v>
       </c>
@@ -4985,7 +5082,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>193</v>
       </c>
@@ -5005,7 +5102,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>194</v>
       </c>
@@ -5025,7 +5122,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>195</v>
       </c>
@@ -5045,7 +5142,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>196</v>
       </c>
@@ -5065,7 +5162,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>197</v>
       </c>
@@ -5085,7 +5182,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>198</v>
       </c>
@@ -5105,7 +5202,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>199</v>
       </c>
@@ -5125,7 +5222,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>200</v>
       </c>
@@ -5145,7 +5242,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>201</v>
       </c>
@@ -5165,7 +5262,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>202</v>
       </c>
@@ -5185,7 +5282,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>203</v>
       </c>
@@ -5205,7 +5302,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>204</v>
       </c>
@@ -5225,7 +5322,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>205</v>
       </c>
@@ -5245,7 +5342,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>206</v>
       </c>
@@ -5265,7 +5362,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>207</v>
       </c>
@@ -5285,7 +5382,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>208</v>
       </c>
@@ -5305,7 +5402,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>209</v>
       </c>
@@ -5325,7 +5422,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>210</v>
       </c>
@@ -5345,7 +5442,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>211</v>
       </c>
@@ -5365,7 +5462,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>212</v>
       </c>
@@ -5385,7 +5482,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>213</v>
       </c>
@@ -5405,7 +5502,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>214</v>
       </c>
@@ -5425,7 +5522,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>215</v>
       </c>
@@ -5445,7 +5542,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>216</v>
       </c>
@@ -5465,7 +5562,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>217</v>
       </c>
@@ -5485,7 +5582,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>218</v>
       </c>
@@ -5505,7 +5602,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>219</v>
       </c>
@@ -5525,7 +5622,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>220</v>
       </c>
@@ -5545,7 +5642,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>221</v>
       </c>
@@ -5565,7 +5662,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>163</v>
       </c>
@@ -5585,7 +5682,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>222</v>
       </c>
@@ -5605,7 +5702,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>223</v>
       </c>
@@ -5625,7 +5722,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>224</v>
       </c>
@@ -5645,7 +5742,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>225</v>
       </c>
@@ -5665,7 +5762,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>226</v>
       </c>
@@ -5685,7 +5782,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>227</v>
       </c>
@@ -5705,7 +5802,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>228</v>
       </c>
@@ -5725,7 +5822,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>229</v>
       </c>
@@ -5745,7 +5842,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>230</v>
       </c>
@@ -5765,7 +5862,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>231</v>
       </c>
@@ -5785,7 +5882,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>232</v>
       </c>
@@ -5805,7 +5902,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>233</v>
       </c>
@@ -5825,7 +5922,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>234</v>
       </c>
@@ -5845,7 +5942,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>235</v>
       </c>
@@ -5865,7 +5962,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>236</v>
       </c>
@@ -5885,7 +5982,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>237</v>
       </c>
@@ -5905,7 +6002,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>238</v>
       </c>
@@ -5925,7 +6022,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>239</v>
       </c>
@@ -5945,7 +6042,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>240</v>
       </c>
@@ -5965,7 +6062,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>241</v>
       </c>
@@ -5985,7 +6082,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>242</v>
       </c>
@@ -6005,7 +6102,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>243</v>
       </c>
@@ -6025,7 +6122,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>244</v>
       </c>
@@ -6045,7 +6142,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>245</v>
       </c>
@@ -6065,7 +6162,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>246</v>
       </c>
@@ -6085,7 +6182,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>247</v>
       </c>
@@ -6105,7 +6202,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>248</v>
       </c>
@@ -6125,7 +6222,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>249</v>
       </c>
@@ -6145,7 +6242,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>250</v>
       </c>
@@ -6165,7 +6262,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>251</v>
       </c>
@@ -6185,7 +6282,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>252</v>
       </c>
@@ -6205,7 +6302,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>253</v>
       </c>
@@ -6225,7 +6322,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>254</v>
       </c>
@@ -6245,7 +6342,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>255</v>
       </c>
@@ -6265,7 +6362,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>256</v>
       </c>
@@ -6285,7 +6382,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>257</v>
       </c>
@@ -6305,7 +6402,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>258</v>
       </c>
@@ -6325,7 +6422,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>259</v>
       </c>
@@ -6345,7 +6442,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>260</v>
       </c>
@@ -6365,7 +6462,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>261</v>
       </c>
@@ -6385,7 +6482,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>262</v>
       </c>
@@ -6405,7 +6502,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>263</v>
       </c>
@@ -6425,7 +6522,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>264</v>
       </c>
@@ -6445,7 +6542,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>265</v>
       </c>
@@ -6465,7 +6562,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>266</v>
       </c>
@@ -6485,7 +6582,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>267</v>
       </c>
@@ -6505,7 +6602,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>268</v>
       </c>
@@ -6525,7 +6622,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>269</v>
       </c>
@@ -6545,7 +6642,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>270</v>
       </c>
@@ -6565,7 +6662,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>271</v>
       </c>
@@ -6585,7 +6682,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>272</v>
       </c>
@@ -6605,7 +6702,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>273</v>
       </c>
@@ -6625,7 +6722,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" s="4" t="s">
         <v>835</v>
       </c>
@@ -6645,7 +6742,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
         <v>836</v>
       </c>
@@ -6665,7 +6762,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" s="4" t="s">
         <v>837</v>
       </c>
@@ -6685,7 +6782,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" s="4" t="s">
         <v>838</v>
       </c>
@@ -6705,7 +6802,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" s="4" t="s">
         <v>839</v>
       </c>
@@ -6725,7 +6822,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" s="4" t="s">
         <v>840</v>
       </c>
@@ -6745,7 +6842,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" s="4" t="s">
         <v>841</v>
       </c>
@@ -6765,7 +6862,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" s="4" t="s">
         <v>842</v>
       </c>
@@ -6785,7 +6882,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" s="4" t="s">
         <v>843</v>
       </c>
@@ -6805,7 +6902,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" s="4" t="s">
         <v>844</v>
       </c>
@@ -6825,7 +6922,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" s="4" t="s">
         <v>845</v>
       </c>
@@ -6845,7 +6942,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" s="4" t="s">
         <v>846</v>
       </c>
@@ -6865,7 +6962,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" s="4" t="s">
         <v>847</v>
       </c>
@@ -6885,7 +6982,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" s="4" t="s">
         <v>848</v>
       </c>
@@ -6905,7 +7002,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" s="4" t="s">
         <v>849</v>
       </c>
@@ -6925,7 +7022,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" s="4" t="s">
         <v>850</v>
       </c>
@@ -6945,7 +7042,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" s="4" t="s">
         <v>851</v>
       </c>
@@ -6965,7 +7062,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" s="4" t="s">
         <v>852</v>
       </c>
@@ -6985,7 +7082,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" s="4" t="s">
         <v>853</v>
       </c>
@@ -7005,7 +7102,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" s="4" t="s">
         <v>854</v>
       </c>
@@ -7025,7 +7122,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" s="4" t="s">
         <v>855</v>
       </c>
@@ -7045,7 +7142,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" s="4" t="s">
         <v>856</v>
       </c>
@@ -7065,7 +7162,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" s="4" t="s">
         <v>857</v>
       </c>
@@ -7085,7 +7182,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" s="4" t="s">
         <v>858</v>
       </c>
@@ -7105,7 +7202,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" s="4" t="s">
         <v>859</v>
       </c>
@@ -7125,7 +7222,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" s="4" t="s">
         <v>860</v>
       </c>
@@ -7145,7 +7242,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" s="4" t="s">
         <v>861</v>
       </c>
@@ -7165,7 +7262,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178" s="4" t="s">
         <v>862</v>
       </c>
@@ -7185,7 +7282,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179" s="4" t="s">
         <v>863</v>
       </c>
@@ -7205,7 +7302,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" s="4" t="s">
         <v>864</v>
       </c>
@@ -7225,7 +7322,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" s="4" t="s">
         <v>865</v>
       </c>
@@ -7245,7 +7342,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" s="4" t="s">
         <v>866</v>
       </c>
@@ -7265,7 +7362,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" s="4" t="s">
         <v>867</v>
       </c>
@@ -7285,7 +7382,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184" s="4" t="s">
         <v>868</v>
       </c>
@@ -7305,7 +7402,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" s="4" t="s">
         <v>869</v>
       </c>
@@ -7325,7 +7422,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186" s="4" t="s">
         <v>870</v>
       </c>
@@ -7345,7 +7442,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187" s="4" t="s">
         <v>871</v>
       </c>
@@ -7365,7 +7462,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" s="4" t="s">
         <v>872</v>
       </c>
@@ -7385,7 +7482,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189" s="4" t="s">
         <v>873</v>
       </c>
@@ -7403,6 +7500,134 @@
       </c>
       <c r="F189" t="s">
         <v>1024</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A190" s="8" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B190" s="9" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A191" s="8" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B191" s="5" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A192" s="8" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B192" s="9" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A193" s="8" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B193" s="9" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194" s="8" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B194" s="9" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195" s="8" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B195" s="9" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196" s="8" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B196" s="9" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197" s="9" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B197" s="9" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198" s="8" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B198" s="9" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199" s="9" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B199" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200" s="9" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B200" s="9" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A201" s="9" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B201" s="9" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A202" s="9" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B202" s="9" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A203" s="9" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B203" s="9" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A204" s="9" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B204" s="9" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A205" s="9" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B205" s="9" t="s">
+        <v>1068</v>
       </c>
     </row>
   </sheetData>
@@ -7412,6 +7637,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="6e0cf07b-8188-4b76-8f54-3cda03d37414" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="43e153a8-5ef1-4f65-aac7-dc4685f18eaa">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F12BE0DB4A3DF641BF113FBF1C7EA261" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="718598463bd34fa12e450bcb3a6783b8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="43e153a8-5ef1-4f65-aac7-dc4685f18eaa" xmlns:ns3="6e0cf07b-8188-4b76-8f54-3cda03d37414" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="54cbcd1ebcb6479b13808205dc2a6520" ns2:_="" ns3:_="">
     <xsd:import namespace="43e153a8-5ef1-4f65-aac7-dc4685f18eaa"/>
@@ -7640,41 +7885,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="6e0cf07b-8188-4b76-8f54-3cda03d37414" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="43e153a8-5ef1-4f65-aac7-dc4685f18eaa">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBDDFBA8-FF97-4684-8DBF-782A9A0E4D0B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04FEE910-FEC8-48C6-9CF9-BF01BA5AD6FE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="43e153a8-5ef1-4f65-aac7-dc4685f18eaa"/>
-    <ds:schemaRef ds:uri="6e0cf07b-8188-4b76-8f54-3cda03d37414"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7697,9 +7911,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04FEE910-FEC8-48C6-9CF9-BF01BA5AD6FE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBDDFBA8-FF97-4684-8DBF-782A9A0E4D0B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="43e153a8-5ef1-4f65-aac7-dc4685f18eaa"/>
+    <ds:schemaRef ds:uri="6e0cf07b-8188-4b76-8f54-3cda03d37414"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added ability to detect if wifi is disabled
</commit_message>
<xml_diff>
--- a/translations/translations.xlsx
+++ b/translations/translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cdc.sharepoint.com/teams/CGH-GPSSample/Shared Documents/General/Bolivia/App_Translation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bp51/Development/GTRI/Android/gpssample/translations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{BBA288CA-BBAE-4D72-9D2B-1C2581202596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C4F6107-097C-4E77-850B-4866395B689B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C287E5D-3523-B64C-A54B-1FF0FDB33A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C8C8ACD1-4E76-7942-B525-8D880B4ECA80}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="23360" windowHeight="17440" xr2:uid="{C8C8ACD1-4E76-7942-B525-8D880B4ECA80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="1143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="1149">
   <si>
     <t>Settings</t>
   </si>
@@ -3481,6 +3481,24 @@
   </si>
   <si>
     <t>Fatal! Отсутствует необходимый параметр: правило</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>wifi_disabled</t>
+  </si>
+  <si>
+    <t>WiFi disabled</t>
+  </si>
+  <si>
+    <t>wifi_disabled_message</t>
+  </si>
+  <si>
+    <t>WiFi is disabled. Please make sure Wifi is turned on</t>
   </si>
 </sst>
 </file>
@@ -3569,12 +3587,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3582,9 +3600,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -3901,22 +3916,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD3E6CC-854C-5841-9577-D3ADD2982DB6}">
-  <dimension ref="A1:F205"/>
+  <dimension ref="A1:F208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D190" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E200" sqref="E200"/>
+    <sheetView tabSelected="1" topLeftCell="A191" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B208" sqref="B208"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="52" customWidth="1"/>
     <col min="2" max="2" width="62" customWidth="1"/>
     <col min="3" max="3" width="48.33203125" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
-    <col min="5" max="5" width="41.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>145</v>
       </c>
@@ -3936,7 +3951,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>146</v>
       </c>
@@ -3956,7 +3971,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>147</v>
       </c>
@@ -3976,7 +3991,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>148</v>
       </c>
@@ -3996,7 +4011,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>149</v>
       </c>
@@ -4016,7 +4031,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>150</v>
       </c>
@@ -4036,7 +4051,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>151</v>
       </c>
@@ -4056,7 +4071,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>152</v>
       </c>
@@ -4076,7 +4091,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>153</v>
       </c>
@@ -4096,7 +4111,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>154</v>
       </c>
@@ -4116,7 +4131,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>155</v>
       </c>
@@ -4136,7 +4151,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>156</v>
       </c>
@@ -4156,7 +4171,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>157</v>
       </c>
@@ -4176,7 +4191,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>158</v>
       </c>
@@ -4196,7 +4211,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>159</v>
       </c>
@@ -4216,7 +4231,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>160</v>
       </c>
@@ -4236,7 +4251,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>161</v>
       </c>
@@ -4256,7 +4271,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>162</v>
       </c>
@@ -4276,7 +4291,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>162</v>
       </c>
@@ -4296,7 +4311,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>162</v>
       </c>
@@ -4316,7 +4331,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>162</v>
       </c>
@@ -4336,7 +4351,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>162</v>
       </c>
@@ -4356,7 +4371,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>162</v>
       </c>
@@ -4376,7 +4391,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>162</v>
       </c>
@@ -4396,7 +4411,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>833</v>
       </c>
@@ -4416,7 +4431,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>833</v>
       </c>
@@ -4436,7 +4451,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>834</v>
       </c>
@@ -4456,7 +4471,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>834</v>
       </c>
@@ -4476,7 +4491,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>164</v>
       </c>
@@ -4496,7 +4511,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>164</v>
       </c>
@@ -4516,7 +4531,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>164</v>
       </c>
@@ -4536,7 +4551,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>164</v>
       </c>
@@ -4556,7 +4571,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>164</v>
       </c>
@@ -4576,7 +4591,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>165</v>
       </c>
@@ -4596,7 +4611,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>165</v>
       </c>
@@ -4616,7 +4631,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>165</v>
       </c>
@@ -4636,7 +4651,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>165</v>
       </c>
@@ -4656,7 +4671,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>165</v>
       </c>
@@ -4676,7 +4691,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>166</v>
       </c>
@@ -4696,7 +4711,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>166</v>
       </c>
@@ -4716,7 +4731,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>166</v>
       </c>
@@ -4736,7 +4751,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>167</v>
       </c>
@@ -4756,7 +4771,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>167</v>
       </c>
@@ -4776,7 +4791,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>167</v>
       </c>
@@ -4796,7 +4811,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>167</v>
       </c>
@@ -4816,7 +4831,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>168</v>
       </c>
@@ -4836,7 +4851,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>169</v>
       </c>
@@ -4856,7 +4871,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>170</v>
       </c>
@@ -4876,7 +4891,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>171</v>
       </c>
@@ -4896,7 +4911,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>174</v>
       </c>
@@ -4916,7 +4931,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>175</v>
       </c>
@@ -4936,7 +4951,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>176</v>
       </c>
@@ -4956,7 +4971,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>177</v>
       </c>
@@ -4976,7 +4991,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>178</v>
       </c>
@@ -4996,7 +5011,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>179</v>
       </c>
@@ -5016,7 +5031,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>180</v>
       </c>
@@ -5036,7 +5051,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>181</v>
       </c>
@@ -5056,7 +5071,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>182</v>
       </c>
@@ -5076,7 +5091,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>183</v>
       </c>
@@ -5096,7 +5111,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>184</v>
       </c>
@@ -5116,7 +5131,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>185</v>
       </c>
@@ -5136,7 +5151,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>186</v>
       </c>
@@ -5156,7 +5171,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>187</v>
       </c>
@@ -5176,7 +5191,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>188</v>
       </c>
@@ -5196,7 +5211,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>189</v>
       </c>
@@ -5216,7 +5231,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>190</v>
       </c>
@@ -5236,7 +5251,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>191</v>
       </c>
@@ -5256,7 +5271,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>192</v>
       </c>
@@ -5276,7 +5291,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>193</v>
       </c>
@@ -5296,7 +5311,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>194</v>
       </c>
@@ -5316,7 +5331,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>195</v>
       </c>
@@ -5336,7 +5351,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>196</v>
       </c>
@@ -5356,7 +5371,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>197</v>
       </c>
@@ -5376,7 +5391,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>198</v>
       </c>
@@ -5396,7 +5411,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>199</v>
       </c>
@@ -5416,7 +5431,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>200</v>
       </c>
@@ -5436,7 +5451,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>201</v>
       </c>
@@ -5456,7 +5471,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>202</v>
       </c>
@@ -5476,7 +5491,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>203</v>
       </c>
@@ -5496,7 +5511,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>204</v>
       </c>
@@ -5516,7 +5531,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>205</v>
       </c>
@@ -5536,7 +5551,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>206</v>
       </c>
@@ -5556,7 +5571,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>207</v>
       </c>
@@ -5576,7 +5591,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>208</v>
       </c>
@@ -5596,7 +5611,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>209</v>
       </c>
@@ -5616,7 +5631,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>210</v>
       </c>
@@ -5636,7 +5651,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>211</v>
       </c>
@@ -5656,7 +5671,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>212</v>
       </c>
@@ -5676,7 +5691,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>213</v>
       </c>
@@ -5696,7 +5711,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>214</v>
       </c>
@@ -5716,7 +5731,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>215</v>
       </c>
@@ -5736,7 +5751,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>216</v>
       </c>
@@ -5756,7 +5771,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>217</v>
       </c>
@@ -5776,7 +5791,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>218</v>
       </c>
@@ -5796,7 +5811,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>219</v>
       </c>
@@ -5816,7 +5831,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>220</v>
       </c>
@@ -5836,7 +5851,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>221</v>
       </c>
@@ -5856,7 +5871,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>163</v>
       </c>
@@ -5876,7 +5891,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>222</v>
       </c>
@@ -5896,7 +5911,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>223</v>
       </c>
@@ -5916,7 +5931,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>224</v>
       </c>
@@ -5936,7 +5951,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>225</v>
       </c>
@@ -5956,7 +5971,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>226</v>
       </c>
@@ -5976,7 +5991,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>227</v>
       </c>
@@ -5996,7 +6011,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>228</v>
       </c>
@@ -6016,7 +6031,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>229</v>
       </c>
@@ -6036,7 +6051,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>230</v>
       </c>
@@ -6056,7 +6071,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>231</v>
       </c>
@@ -6076,7 +6091,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>232</v>
       </c>
@@ -6096,7 +6111,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>233</v>
       </c>
@@ -6116,7 +6131,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>234</v>
       </c>
@@ -6136,7 +6151,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>235</v>
       </c>
@@ -6156,7 +6171,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>236</v>
       </c>
@@ -6176,7 +6191,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>237</v>
       </c>
@@ -6196,7 +6211,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>238</v>
       </c>
@@ -6216,7 +6231,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>239</v>
       </c>
@@ -6236,7 +6251,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>240</v>
       </c>
@@ -6256,7 +6271,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>241</v>
       </c>
@@ -6276,7 +6291,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>242</v>
       </c>
@@ -6296,7 +6311,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>243</v>
       </c>
@@ -6316,7 +6331,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>244</v>
       </c>
@@ -6336,7 +6351,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>245</v>
       </c>
@@ -6356,7 +6371,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>246</v>
       </c>
@@ -6376,7 +6391,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>247</v>
       </c>
@@ -6396,7 +6411,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>248</v>
       </c>
@@ -6416,7 +6431,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>249</v>
       </c>
@@ -6436,7 +6451,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>250</v>
       </c>
@@ -6456,7 +6471,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>251</v>
       </c>
@@ -6476,7 +6491,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>252</v>
       </c>
@@ -6496,7 +6511,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>253</v>
       </c>
@@ -6516,7 +6531,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>254</v>
       </c>
@@ -6536,7 +6551,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>255</v>
       </c>
@@ -6556,7 +6571,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>256</v>
       </c>
@@ -6576,7 +6591,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>257</v>
       </c>
@@ -6596,7 +6611,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>258</v>
       </c>
@@ -6616,7 +6631,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>259</v>
       </c>
@@ -6636,7 +6651,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>260</v>
       </c>
@@ -6656,7 +6671,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>261</v>
       </c>
@@ -6676,7 +6691,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>262</v>
       </c>
@@ -6696,7 +6711,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>263</v>
       </c>
@@ -6716,7 +6731,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>264</v>
       </c>
@@ -6736,7 +6751,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>265</v>
       </c>
@@ -6756,7 +6771,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>266</v>
       </c>
@@ -6776,7 +6791,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>267</v>
       </c>
@@ -6796,7 +6811,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>268</v>
       </c>
@@ -6816,7 +6831,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>269</v>
       </c>
@@ -6836,7 +6851,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>270</v>
       </c>
@@ -6856,7 +6871,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>271</v>
       </c>
@@ -6876,7 +6891,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>272</v>
       </c>
@@ -6896,7 +6911,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>273</v>
       </c>
@@ -6916,7 +6931,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" s="4" t="s">
         <v>835</v>
       </c>
@@ -6936,7 +6951,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
         <v>836</v>
       </c>
@@ -6956,7 +6971,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" s="4" t="s">
         <v>837</v>
       </c>
@@ -6976,7 +6991,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" s="4" t="s">
         <v>838</v>
       </c>
@@ -6996,7 +7011,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" s="4" t="s">
         <v>839</v>
       </c>
@@ -7016,7 +7031,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" s="4" t="s">
         <v>840</v>
       </c>
@@ -7036,7 +7051,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" s="4" t="s">
         <v>841</v>
       </c>
@@ -7056,7 +7071,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" s="4" t="s">
         <v>842</v>
       </c>
@@ -7076,7 +7091,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" s="4" t="s">
         <v>843</v>
       </c>
@@ -7096,7 +7111,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" s="4" t="s">
         <v>844</v>
       </c>
@@ -7116,7 +7131,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" s="4" t="s">
         <v>845</v>
       </c>
@@ -7136,7 +7151,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" s="4" t="s">
         <v>846</v>
       </c>
@@ -7156,7 +7171,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" s="4" t="s">
         <v>847</v>
       </c>
@@ -7176,7 +7191,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" s="4" t="s">
         <v>848</v>
       </c>
@@ -7196,7 +7211,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" s="4" t="s">
         <v>849</v>
       </c>
@@ -7216,7 +7231,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" s="4" t="s">
         <v>850</v>
       </c>
@@ -7236,7 +7251,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" s="4" t="s">
         <v>851</v>
       </c>
@@ -7256,7 +7271,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" s="4" t="s">
         <v>852</v>
       </c>
@@ -7276,7 +7291,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" s="4" t="s">
         <v>853</v>
       </c>
@@ -7296,7 +7311,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" s="4" t="s">
         <v>854</v>
       </c>
@@ -7316,7 +7331,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" s="4" t="s">
         <v>855</v>
       </c>
@@ -7336,7 +7351,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" s="4" t="s">
         <v>856</v>
       </c>
@@ -7356,7 +7371,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" s="4" t="s">
         <v>857</v>
       </c>
@@ -7376,7 +7391,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" s="4" t="s">
         <v>858</v>
       </c>
@@ -7396,7 +7411,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" s="4" t="s">
         <v>859</v>
       </c>
@@ -7416,7 +7431,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" s="4" t="s">
         <v>860</v>
       </c>
@@ -7436,7 +7451,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" s="4" t="s">
         <v>861</v>
       </c>
@@ -7456,7 +7471,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178" s="4" t="s">
         <v>862</v>
       </c>
@@ -7476,7 +7491,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179" s="4" t="s">
         <v>863</v>
       </c>
@@ -7496,7 +7511,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" s="4" t="s">
         <v>864</v>
       </c>
@@ -7516,7 +7531,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" s="4" t="s">
         <v>865</v>
       </c>
@@ -7536,7 +7551,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" s="4" t="s">
         <v>866</v>
       </c>
@@ -7556,7 +7571,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" s="4" t="s">
         <v>867</v>
       </c>
@@ -7576,7 +7591,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184" s="4" t="s">
         <v>868</v>
       </c>
@@ -7596,7 +7611,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" s="4" t="s">
         <v>869</v>
       </c>
@@ -7616,7 +7631,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186" s="4" t="s">
         <v>870</v>
       </c>
@@ -7636,7 +7651,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187" s="4" t="s">
         <v>871</v>
       </c>
@@ -7656,7 +7671,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" s="4" t="s">
         <v>872</v>
       </c>
@@ -7669,14 +7684,14 @@
       <c r="D188" t="s">
         <v>974</v>
       </c>
-      <c r="E188" s="10" t="s">
+      <c r="E188" s="9" t="s">
         <v>1050</v>
       </c>
       <c r="F188" t="s">
         <v>1023</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189" s="4" t="s">
         <v>873</v>
       </c>
@@ -7696,8 +7711,8 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A190" s="8" t="s">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A190" s="4" t="s">
         <v>1052</v>
       </c>
       <c r="B190" t="s">
@@ -7716,8 +7731,8 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A191" s="8" t="s">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A191" s="4" t="s">
         <v>1054</v>
       </c>
       <c r="B191" s="5" t="s">
@@ -7736,8 +7751,8 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A192" s="8" t="s">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A192" s="4" t="s">
         <v>1056</v>
       </c>
       <c r="B192" t="s">
@@ -7756,8 +7771,8 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A193" s="8" t="s">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A193" s="4" t="s">
         <v>1058</v>
       </c>
       <c r="B193" t="s">
@@ -7776,8 +7791,8 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A194" s="8" t="s">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A194" s="4" t="s">
         <v>1060</v>
       </c>
       <c r="B194" t="s">
@@ -7796,8 +7811,8 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A195" s="8" t="s">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A195" s="4" t="s">
         <v>1062</v>
       </c>
       <c r="B195" t="s">
@@ -7816,8 +7831,8 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A196" s="8" t="s">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A196" s="4" t="s">
         <v>1064</v>
       </c>
       <c r="B196" t="s">
@@ -7836,7 +7851,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>1066</v>
       </c>
@@ -7856,8 +7871,8 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A198" s="8" t="s">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A198" s="4" t="s">
         <v>1068</v>
       </c>
       <c r="B198" t="s">
@@ -7876,7 +7891,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>1070</v>
       </c>
@@ -7896,7 +7911,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>1071</v>
       </c>
@@ -7916,7 +7931,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>1073</v>
       </c>
@@ -7936,7 +7951,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>1075</v>
       </c>
@@ -7956,7 +7971,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>1077</v>
       </c>
@@ -7976,7 +7991,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>1079</v>
       </c>
@@ -7996,11 +8011,11 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>1080</v>
       </c>
-      <c r="B205" s="9" t="s">
+      <c r="B205" s="8" t="s">
         <v>1139</v>
       </c>
       <c r="C205" t="s">
@@ -8014,6 +8029,30 @@
       </c>
       <c r="F205" t="s">
         <v>1142</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B206" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B207" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B208" t="s">
+        <v>1148</v>
       </c>
     </row>
   </sheetData>
@@ -8034,6 +8073,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F12BE0DB4A3DF641BF113FBF1C7EA261" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="718598463bd34fa12e450bcb3a6783b8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="43e153a8-5ef1-4f65-aac7-dc4685f18eaa" xmlns:ns3="6e0cf07b-8188-4b76-8f54-3cda03d37414" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="54cbcd1ebcb6479b13808205dc2a6520" ns2:_="" ns3:_="">
     <xsd:import namespace="43e153a8-5ef1-4f65-aac7-dc4685f18eaa"/>
@@ -8262,15 +8310,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E20926E-9EFB-4B7E-90D4-905B08F8E59C}">
   <ds:schemaRefs>
@@ -8289,6 +8328,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04FEE910-FEC8-48C6-9CF9-BF01BA5AD6FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBDDFBA8-FF97-4684-8DBF-782A9A0E4D0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8305,12 +8352,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04FEE910-FEC8-48C6-9CF9-BF01BA5AD6FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixed additional info dialog per Amber's recomendations
</commit_message>
<xml_diff>
--- a/translations/translations.xlsx
+++ b/translations/translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cdc.sharepoint.com/teams/CGH-GPSSample/Shared Documents/General/Bolivia/App_Translation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rmitchell64/Desktop/Projects/GPSSample/gpssample/translations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{BBA288CA-BBAE-4D72-9D2B-1C2581202596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4947A2B9-1EBA-41F7-8890-8CF53CA605AC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B73F7C-35A1-4E40-9EAA-53F8CEB12804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C8C8ACD1-4E76-7942-B525-8D880B4ECA80}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28300" windowHeight="14580" xr2:uid="{C8C8ACD1-4E76-7942-B525-8D880B4ECA80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1290" uniqueCount="1197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="1191">
   <si>
     <t>Settings</t>
   </si>
@@ -2667,9 +2667,6 @@
     <t>location_not_found</t>
   </si>
   <si>
-    <t>nobody_home</t>
-  </si>
-  <si>
     <t>home_not_exist</t>
   </si>
   <si>
@@ -2781,9 +2778,6 @@
     <t>Please Confirm</t>
   </si>
   <si>
-    <t>&gt;Location not found</t>
-  </si>
-  <si>
     <t>Importar datos de enumeración</t>
   </si>
   <si>
@@ -2868,9 +2862,6 @@
     <t>Los datos de enumeración se han guardado en el directorio Documentos.</t>
   </si>
   <si>
-    <t>&gt;Localización no encontrada</t>
-  </si>
-  <si>
     <t>¡Oops! Por favor, seleccione una razón para incompleto</t>
   </si>
   <si>
@@ -2973,9 +2964,6 @@
     <t>Les données d'énumération ont été sauvegardées dans le répertoire Documents.</t>
   </si>
   <si>
-    <t>&gt;La configuration a été sauvegardée dans le répertoire Documents.</t>
-  </si>
-  <si>
     <t>Le domicile n'existe pas</t>
   </si>
   <si>
@@ -3015,9 +3003,6 @@
     <t>Os dados de enumeração foram guardados no diretório Documentos.</t>
   </si>
   <si>
-    <t>&gt;Localização não encontrada</t>
-  </si>
-  <si>
     <t>Пожалуйста, подтвердите</t>
   </si>
   <si>
@@ -3118,9 +3103,6 @@
   </si>
   <si>
     <t>Конфигурация была сохранена в каталог Documents.</t>
-  </si>
-  <si>
-    <t>&gt;Местонахождение не найдено</t>
   </si>
   <si>
     <t>Дом не существует</t>
@@ -3731,12 +3713,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3744,9 +3726,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4066,22 +4045,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD3E6CC-854C-5841-9577-D3ADD2982DB6}">
-  <dimension ref="A1:F215"/>
+  <dimension ref="A1:F214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C199" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F209" sqref="F209:F215"/>
+    <sheetView tabSelected="1" topLeftCell="A178" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A187" sqref="A187:XFD187"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="52" customWidth="1"/>
     <col min="2" max="2" width="62" customWidth="1"/>
     <col min="3" max="3" width="48.33203125" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
-    <col min="5" max="5" width="41.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>145</v>
       </c>
@@ -4101,7 +4080,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>146</v>
       </c>
@@ -4121,7 +4100,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>147</v>
       </c>
@@ -4141,7 +4120,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>148</v>
       </c>
@@ -4161,7 +4140,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>149</v>
       </c>
@@ -4181,7 +4160,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>150</v>
       </c>
@@ -4201,7 +4180,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>151</v>
       </c>
@@ -4221,7 +4200,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>152</v>
       </c>
@@ -4241,7 +4220,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>153</v>
       </c>
@@ -4261,7 +4240,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>154</v>
       </c>
@@ -4281,7 +4260,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>155</v>
       </c>
@@ -4301,7 +4280,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>156</v>
       </c>
@@ -4321,7 +4300,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>157</v>
       </c>
@@ -4341,7 +4320,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>158</v>
       </c>
@@ -4361,7 +4340,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>159</v>
       </c>
@@ -4381,7 +4360,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>160</v>
       </c>
@@ -4401,7 +4380,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>161</v>
       </c>
@@ -4421,7 +4400,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>162</v>
       </c>
@@ -4441,7 +4420,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>162</v>
       </c>
@@ -4461,7 +4440,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>162</v>
       </c>
@@ -4481,7 +4460,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>162</v>
       </c>
@@ -4501,7 +4480,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>162</v>
       </c>
@@ -4521,7 +4500,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>162</v>
       </c>
@@ -4541,7 +4520,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>162</v>
       </c>
@@ -4561,7 +4540,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>833</v>
       </c>
@@ -4581,7 +4560,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>833</v>
       </c>
@@ -4601,7 +4580,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>834</v>
       </c>
@@ -4621,7 +4600,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>834</v>
       </c>
@@ -4641,7 +4620,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>164</v>
       </c>
@@ -4661,7 +4640,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>164</v>
       </c>
@@ -4681,7 +4660,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>164</v>
       </c>
@@ -4701,7 +4680,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>164</v>
       </c>
@@ -4721,7 +4700,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>164</v>
       </c>
@@ -4741,7 +4720,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>165</v>
       </c>
@@ -4761,7 +4740,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>165</v>
       </c>
@@ -4781,7 +4760,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>165</v>
       </c>
@@ -4801,7 +4780,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>165</v>
       </c>
@@ -4821,7 +4800,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>165</v>
       </c>
@@ -4841,7 +4820,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>166</v>
       </c>
@@ -4861,7 +4840,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>166</v>
       </c>
@@ -4881,7 +4860,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>166</v>
       </c>
@@ -4901,7 +4880,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>167</v>
       </c>
@@ -4921,7 +4900,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>167</v>
       </c>
@@ -4941,7 +4920,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>167</v>
       </c>
@@ -4961,7 +4940,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>167</v>
       </c>
@@ -4981,7 +4960,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>168</v>
       </c>
@@ -5001,7 +4980,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>169</v>
       </c>
@@ -5021,7 +5000,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>170</v>
       </c>
@@ -5041,7 +5020,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>171</v>
       </c>
@@ -5061,7 +5040,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>174</v>
       </c>
@@ -5081,7 +5060,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>175</v>
       </c>
@@ -5101,7 +5080,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>176</v>
       </c>
@@ -5121,7 +5100,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>177</v>
       </c>
@@ -5141,7 +5120,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>178</v>
       </c>
@@ -5161,7 +5140,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>179</v>
       </c>
@@ -5181,7 +5160,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>180</v>
       </c>
@@ -5201,7 +5180,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>181</v>
       </c>
@@ -5221,7 +5200,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>182</v>
       </c>
@@ -5241,7 +5220,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>183</v>
       </c>
@@ -5261,7 +5240,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>184</v>
       </c>
@@ -5281,7 +5260,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>185</v>
       </c>
@@ -5301,7 +5280,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>186</v>
       </c>
@@ -5321,7 +5300,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>187</v>
       </c>
@@ -5341,7 +5320,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>188</v>
       </c>
@@ -5361,7 +5340,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>189</v>
       </c>
@@ -5381,7 +5360,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>190</v>
       </c>
@@ -5401,7 +5380,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>191</v>
       </c>
@@ -5421,7 +5400,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>192</v>
       </c>
@@ -5441,7 +5420,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>193</v>
       </c>
@@ -5461,7 +5440,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>194</v>
       </c>
@@ -5481,7 +5460,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>195</v>
       </c>
@@ -5501,7 +5480,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>196</v>
       </c>
@@ -5521,7 +5500,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>197</v>
       </c>
@@ -5541,7 +5520,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>198</v>
       </c>
@@ -5561,7 +5540,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>199</v>
       </c>
@@ -5581,7 +5560,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>200</v>
       </c>
@@ -5601,7 +5580,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>201</v>
       </c>
@@ -5621,7 +5600,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>202</v>
       </c>
@@ -5641,7 +5620,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>203</v>
       </c>
@@ -5661,7 +5640,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>204</v>
       </c>
@@ -5681,7 +5660,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>205</v>
       </c>
@@ -5701,7 +5680,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>206</v>
       </c>
@@ -5721,7 +5700,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>207</v>
       </c>
@@ -5741,7 +5720,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>208</v>
       </c>
@@ -5761,7 +5740,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>209</v>
       </c>
@@ -5781,7 +5760,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>210</v>
       </c>
@@ -5801,7 +5780,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>211</v>
       </c>
@@ -5821,7 +5800,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>212</v>
       </c>
@@ -5841,7 +5820,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>213</v>
       </c>
@@ -5861,7 +5840,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>214</v>
       </c>
@@ -5881,7 +5860,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>215</v>
       </c>
@@ -5901,7 +5880,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>216</v>
       </c>
@@ -5921,7 +5900,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>217</v>
       </c>
@@ -5941,7 +5920,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>218</v>
       </c>
@@ -5961,7 +5940,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>219</v>
       </c>
@@ -5981,7 +5960,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>220</v>
       </c>
@@ -6001,7 +5980,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>221</v>
       </c>
@@ -6021,7 +6000,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>163</v>
       </c>
@@ -6041,7 +6020,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>222</v>
       </c>
@@ -6061,7 +6040,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>223</v>
       </c>
@@ -6081,7 +6060,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>224</v>
       </c>
@@ -6101,7 +6080,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>225</v>
       </c>
@@ -6121,7 +6100,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>226</v>
       </c>
@@ -6141,7 +6120,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>227</v>
       </c>
@@ -6161,7 +6140,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>228</v>
       </c>
@@ -6181,7 +6160,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>229</v>
       </c>
@@ -6201,7 +6180,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>230</v>
       </c>
@@ -6221,7 +6200,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>231</v>
       </c>
@@ -6241,7 +6220,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>232</v>
       </c>
@@ -6261,7 +6240,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>233</v>
       </c>
@@ -6281,7 +6260,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>234</v>
       </c>
@@ -6301,7 +6280,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>235</v>
       </c>
@@ -6321,7 +6300,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>236</v>
       </c>
@@ -6341,7 +6320,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>237</v>
       </c>
@@ -6361,7 +6340,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>238</v>
       </c>
@@ -6381,7 +6360,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>239</v>
       </c>
@@ -6401,7 +6380,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>240</v>
       </c>
@@ -6421,7 +6400,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>241</v>
       </c>
@@ -6441,7 +6420,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>242</v>
       </c>
@@ -6461,7 +6440,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>243</v>
       </c>
@@ -6481,7 +6460,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>244</v>
       </c>
@@ -6501,7 +6480,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>245</v>
       </c>
@@ -6521,7 +6500,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>246</v>
       </c>
@@ -6541,7 +6520,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>247</v>
       </c>
@@ -6561,7 +6540,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>248</v>
       </c>
@@ -6581,7 +6560,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>249</v>
       </c>
@@ -6601,7 +6580,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>250</v>
       </c>
@@ -6621,7 +6600,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>251</v>
       </c>
@@ -6641,7 +6620,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>252</v>
       </c>
@@ -6661,7 +6640,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>253</v>
       </c>
@@ -6681,7 +6660,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>254</v>
       </c>
@@ -6701,7 +6680,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>255</v>
       </c>
@@ -6721,7 +6700,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>256</v>
       </c>
@@ -6741,7 +6720,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>257</v>
       </c>
@@ -6761,7 +6740,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>258</v>
       </c>
@@ -6781,7 +6760,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>259</v>
       </c>
@@ -6801,7 +6780,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>260</v>
       </c>
@@ -6821,7 +6800,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>261</v>
       </c>
@@ -6841,7 +6820,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>262</v>
       </c>
@@ -6861,7 +6840,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>263</v>
       </c>
@@ -6881,7 +6860,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>264</v>
       </c>
@@ -6901,7 +6880,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>265</v>
       </c>
@@ -6921,7 +6900,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>266</v>
       </c>
@@ -6941,7 +6920,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>267</v>
       </c>
@@ -6961,7 +6940,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>268</v>
       </c>
@@ -6981,7 +6960,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>269</v>
       </c>
@@ -7001,7 +6980,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>270</v>
       </c>
@@ -7021,7 +7000,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>271</v>
       </c>
@@ -7041,7 +7020,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>272</v>
       </c>
@@ -7061,7 +7040,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>273</v>
       </c>
@@ -7081,1304 +7060,1284 @@
         <v>647</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" s="4" t="s">
         <v>835</v>
       </c>
       <c r="B151" s="5" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="C151" t="s">
-        <v>1025</v>
+        <v>1019</v>
       </c>
       <c r="D151" t="s">
-        <v>1029</v>
+        <v>1023</v>
       </c>
       <c r="E151" t="s">
-        <v>1025</v>
+        <v>1019</v>
       </c>
       <c r="F151" t="s">
-        <v>988</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
         <v>836</v>
       </c>
       <c r="B152" s="5" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="C152" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D152" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
       <c r="E152" t="s">
-        <v>976</v>
+        <v>972</v>
       </c>
       <c r="F152" t="s">
-        <v>989</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" s="4" t="s">
         <v>837</v>
       </c>
       <c r="B153" s="5" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="C153" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="D153" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
       <c r="E153" t="s">
-        <v>977</v>
+        <v>973</v>
       </c>
       <c r="F153" t="s">
-        <v>990</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" s="4" t="s">
         <v>838</v>
       </c>
       <c r="B154" s="5" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="C154" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="D154" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
       <c r="E154" t="s">
-        <v>1030</v>
+        <v>1024</v>
       </c>
       <c r="F154" t="s">
-        <v>991</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" s="4" t="s">
         <v>839</v>
       </c>
       <c r="B155" s="5" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="C155" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="D155" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
       <c r="E155" t="s">
-        <v>1031</v>
+        <v>1025</v>
       </c>
       <c r="F155" t="s">
-        <v>992</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" s="4" t="s">
         <v>840</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="C156" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D156" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
       <c r="E156" t="s">
-        <v>1032</v>
+        <v>1026</v>
       </c>
       <c r="F156" t="s">
-        <v>993</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" s="4" t="s">
         <v>841</v>
       </c>
       <c r="B157" s="5" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="C157" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D157" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="E157" t="s">
-        <v>1033</v>
+        <v>1027</v>
       </c>
       <c r="F157" t="s">
-        <v>994</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" s="4" t="s">
         <v>842</v>
       </c>
       <c r="B158" s="5" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="C158" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="D158" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="E158" t="s">
-        <v>1034</v>
+        <v>1028</v>
       </c>
       <c r="F158" t="s">
-        <v>995</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" s="4" t="s">
         <v>843</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="C159" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="D159" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
       <c r="E159" t="s">
-        <v>1035</v>
+        <v>1029</v>
       </c>
       <c r="F159" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" s="4" t="s">
         <v>844</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="C160" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="D160" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
       <c r="E160" t="s">
-        <v>1036</v>
+        <v>1030</v>
       </c>
       <c r="F160" t="s">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" s="4" t="s">
         <v>845</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="C161" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="D161" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
       <c r="E161" t="s">
-        <v>1036</v>
+        <v>1030</v>
       </c>
       <c r="F161" t="s">
-        <v>998</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" s="4" t="s">
         <v>846</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="C162" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="D162" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
       <c r="E162" t="s">
-        <v>1037</v>
+        <v>1031</v>
       </c>
       <c r="F162" t="s">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" s="4" t="s">
         <v>847</v>
       </c>
       <c r="B163" s="5" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="C163" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="D163" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
       <c r="E163" t="s">
-        <v>1038</v>
+        <v>1032</v>
       </c>
       <c r="F163" t="s">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" s="4" t="s">
         <v>848</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="C164" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="D164" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
       <c r="E164" t="s">
-        <v>1039</v>
+        <v>1033</v>
       </c>
       <c r="F164" t="s">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" s="4" t="s">
         <v>849</v>
       </c>
       <c r="B165" s="5" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="C165" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="D165" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
       <c r="E165" t="s">
-        <v>1040</v>
+        <v>1034</v>
       </c>
       <c r="F165" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" s="4" t="s">
         <v>850</v>
       </c>
       <c r="B166" s="5" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="C166" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="D166" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
       <c r="E166" t="s">
-        <v>978</v>
+        <v>974</v>
       </c>
       <c r="F166" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" s="4" t="s">
         <v>851</v>
       </c>
       <c r="B167" s="5" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="C167" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="D167" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
       <c r="E167" t="s">
-        <v>1041</v>
+        <v>1035</v>
       </c>
       <c r="F167" t="s">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" s="4" t="s">
         <v>852</v>
       </c>
       <c r="B168" s="5" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="C168" t="s">
-        <v>1026</v>
+        <v>1020</v>
       </c>
       <c r="D168" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
       <c r="E168" t="s">
-        <v>1042</v>
+        <v>1036</v>
       </c>
       <c r="F168" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" s="4" t="s">
         <v>853</v>
       </c>
       <c r="B169" s="5" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="C169" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="D169" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
       <c r="E169" t="s">
-        <v>1043</v>
+        <v>1037</v>
       </c>
       <c r="F169" t="s">
-        <v>1006</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" s="4" t="s">
         <v>854</v>
       </c>
       <c r="B170" s="5" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="C170" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="D170" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
       <c r="E170" t="s">
-        <v>979</v>
+        <v>975</v>
       </c>
       <c r="F170" t="s">
-        <v>1007</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" s="4" t="s">
         <v>855</v>
       </c>
       <c r="B171" s="5" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="C171" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="D171" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
       <c r="E171" t="s">
-        <v>1044</v>
+        <v>1038</v>
       </c>
       <c r="F171" t="s">
-        <v>1008</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" s="4" t="s">
         <v>856</v>
       </c>
       <c r="B172" s="6" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="C172" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="D172" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
       <c r="E172" t="s">
-        <v>980</v>
+        <v>976</v>
       </c>
       <c r="F172" t="s">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" s="4" t="s">
         <v>857</v>
       </c>
       <c r="B173" s="5" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="C173" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="D173" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
       <c r="E173" t="s">
-        <v>981</v>
+        <v>977</v>
       </c>
       <c r="F173" t="s">
-        <v>1010</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" s="4" t="s">
         <v>858</v>
       </c>
       <c r="B174" s="5" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="C174" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="D174" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
       <c r="E174" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="F174" t="s">
-        <v>1011</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" s="4" t="s">
         <v>859</v>
       </c>
       <c r="B175" s="5" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="C175" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="D175" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
       <c r="E175" t="s">
-        <v>982</v>
+        <v>978</v>
       </c>
       <c r="F175" t="s">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" s="4" t="s">
         <v>860</v>
       </c>
       <c r="B176" s="5" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="C176" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="D176" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
       <c r="E176" t="s">
-        <v>1045</v>
+        <v>1039</v>
       </c>
       <c r="F176" t="s">
-        <v>1013</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" s="4" t="s">
         <v>861</v>
       </c>
       <c r="B177" s="5" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C177" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="D177" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="E177" t="s">
-        <v>983</v>
+        <v>979</v>
       </c>
       <c r="F177" t="s">
-        <v>1014</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178" s="4" t="s">
         <v>862</v>
       </c>
       <c r="B178" s="5" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C178" t="s">
-        <v>1027</v>
+        <v>1021</v>
       </c>
       <c r="D178" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="E178" t="s">
-        <v>1046</v>
+        <v>1040</v>
       </c>
       <c r="F178" t="s">
-        <v>1015</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179" s="4" t="s">
         <v>863</v>
       </c>
       <c r="B179" s="5" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="C179" t="s">
-        <v>1028</v>
+        <v>1022</v>
       </c>
       <c r="D179" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="E179" t="s">
-        <v>1047</v>
+        <v>1041</v>
       </c>
       <c r="F179" t="s">
-        <v>1016</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" s="4" t="s">
         <v>864</v>
       </c>
       <c r="B180" s="5" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="C180" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="D180" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
       <c r="E180" t="s">
-        <v>984</v>
+        <v>980</v>
       </c>
       <c r="F180" t="s">
-        <v>1017</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" s="4" t="s">
         <v>865</v>
       </c>
       <c r="B181" s="5" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="C181" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="D181" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
       <c r="E181" t="s">
-        <v>1037</v>
+        <v>1031</v>
       </c>
       <c r="F181" t="s">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" s="4" t="s">
         <v>866</v>
       </c>
       <c r="B182" s="5" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="C182" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="D182" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
       <c r="E182" t="s">
-        <v>1048</v>
+        <v>1042</v>
       </c>
       <c r="F182" t="s">
-        <v>1018</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" s="4" t="s">
         <v>867</v>
       </c>
       <c r="B183" s="5" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="C183" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="D183" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
       <c r="E183" t="s">
-        <v>1048</v>
+        <v>1042</v>
       </c>
       <c r="F183" t="s">
-        <v>1018</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184" s="4" t="s">
         <v>868</v>
       </c>
       <c r="B184" s="5" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C184" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="D184" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
       <c r="E184" t="s">
-        <v>985</v>
+        <v>981</v>
       </c>
       <c r="F184" t="s">
-        <v>1019</v>
-      </c>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" s="4" t="s">
         <v>869</v>
       </c>
       <c r="B185" s="5" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="C185" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="D185" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
       <c r="E185" t="s">
-        <v>986</v>
+        <v>982</v>
       </c>
       <c r="F185" t="s">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186" s="4" t="s">
         <v>870</v>
       </c>
       <c r="B186" s="5" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="C186" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="D186" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
       <c r="E186" t="s">
-        <v>978</v>
+        <v>974</v>
       </c>
       <c r="F186" t="s">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187" s="4" t="s">
         <v>871</v>
       </c>
       <c r="B187" s="5" t="s">
-        <v>909</v>
-      </c>
-      <c r="C187" t="s">
-        <v>938</v>
+        <v>874</v>
+      </c>
+      <c r="C187" s="7" t="s">
+        <v>1045</v>
       </c>
       <c r="D187" t="s">
-        <v>973</v>
-      </c>
-      <c r="E187" t="s">
-        <v>987</v>
+        <v>970</v>
+      </c>
+      <c r="E187" s="9" t="s">
+        <v>1044</v>
       </c>
       <c r="F187" t="s">
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" s="4" t="s">
         <v>872</v>
       </c>
       <c r="B188" s="5" t="s">
-        <v>875</v>
-      </c>
-      <c r="C188" s="7" t="s">
+        <v>873</v>
+      </c>
+      <c r="C188" t="s">
+        <v>936</v>
+      </c>
+      <c r="D188" t="s">
+        <v>971</v>
+      </c>
+      <c r="E188" t="s">
+        <v>1043</v>
+      </c>
+      <c r="F188" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A189" s="4" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B189" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C189" t="s">
+        <v>1076</v>
+      </c>
+      <c r="D189" t="s">
+        <v>1090</v>
+      </c>
+      <c r="E189" t="s">
+        <v>1123</v>
+      </c>
+      <c r="F189" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A190" s="4" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B190" s="5" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C190" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D190" t="s">
+        <v>1103</v>
+      </c>
+      <c r="E190" t="s">
+        <v>1124</v>
+      </c>
+      <c r="F190" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A191" s="4" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B191" t="s">
         <v>1051</v>
       </c>
-      <c r="D188" t="s">
-        <v>974</v>
-      </c>
-      <c r="E188" s="10" t="s">
-        <v>1050</v>
-      </c>
-      <c r="F188" t="s">
-        <v>1023</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A189" s="4" t="s">
-        <v>873</v>
-      </c>
-      <c r="B189" s="5" t="s">
-        <v>874</v>
-      </c>
-      <c r="C189" t="s">
-        <v>939</v>
-      </c>
-      <c r="D189" t="s">
-        <v>975</v>
-      </c>
-      <c r="E189" t="s">
-        <v>1049</v>
-      </c>
-      <c r="F189" t="s">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A190" s="8" t="s">
+      <c r="C191" t="s">
+        <v>1078</v>
+      </c>
+      <c r="D191" t="s">
+        <v>1091</v>
+      </c>
+      <c r="E191" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F191" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A192" s="4" t="s">
         <v>1052</v>
       </c>
-      <c r="B190" t="s">
+      <c r="B192" t="s">
         <v>1053</v>
       </c>
-      <c r="C190" t="s">
+      <c r="C192" t="s">
+        <v>1079</v>
+      </c>
+      <c r="D192" t="s">
+        <v>1092</v>
+      </c>
+      <c r="E192" t="s">
+        <v>1126</v>
+      </c>
+      <c r="F192" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A193" s="4" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B193" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C193" t="s">
+        <v>1080</v>
+      </c>
+      <c r="D193" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E193" t="s">
+        <v>1104</v>
+      </c>
+      <c r="F193" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A194" s="4" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B194" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C194" t="s">
+        <v>1081</v>
+      </c>
+      <c r="D194" t="s">
+        <v>1094</v>
+      </c>
+      <c r="E194" t="s">
+        <v>1105</v>
+      </c>
+      <c r="F194" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A195" s="4" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B195" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C195" t="s">
         <v>1082</v>
       </c>
-      <c r="D190" t="s">
+      <c r="D195" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E195" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F195" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B196" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C196" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D196" t="s">
         <v>1096</v>
       </c>
-      <c r="E190" t="s">
+      <c r="E196" t="s">
+        <v>1128</v>
+      </c>
+      <c r="F196" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A197" s="4" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B197" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C197" t="s">
+        <v>1084</v>
+      </c>
+      <c r="D197" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E197" t="s">
         <v>1129</v>
       </c>
-      <c r="F190" t="s">
-        <v>1115</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A191" s="8" t="s">
-        <v>1054</v>
-      </c>
-      <c r="B191" s="5" t="s">
-        <v>1055</v>
-      </c>
-      <c r="C191" t="s">
-        <v>1083</v>
-      </c>
-      <c r="D191" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E191" t="s">
+      <c r="F197" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B198" t="s">
+        <v>22</v>
+      </c>
+      <c r="C198" t="s">
+        <v>321</v>
+      </c>
+      <c r="D198" t="s">
+        <v>423</v>
+      </c>
+      <c r="E198" t="s">
+        <v>529</v>
+      </c>
+      <c r="F198" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B199" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C199" t="s">
+        <v>1085</v>
+      </c>
+      <c r="D199" t="s">
+        <v>1098</v>
+      </c>
+      <c r="E199" t="s">
         <v>1130</v>
       </c>
-      <c r="F191" t="s">
-        <v>1116</v>
-      </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A192" s="8" t="s">
-        <v>1056</v>
-      </c>
-      <c r="B192" t="s">
-        <v>1057</v>
-      </c>
-      <c r="C192" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D192" t="s">
-        <v>1097</v>
-      </c>
-      <c r="E192" t="s">
+      <c r="F199" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B200" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C200" t="s">
+        <v>1086</v>
+      </c>
+      <c r="D200" t="s">
+        <v>1099</v>
+      </c>
+      <c r="E200" t="s">
+        <v>1106</v>
+      </c>
+      <c r="F200" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B201" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C201" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D201" t="s">
+        <v>1100</v>
+      </c>
+      <c r="E201" t="s">
         <v>1131</v>
       </c>
-      <c r="F192" t="s">
-        <v>1117</v>
-      </c>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A193" s="8" t="s">
-        <v>1058</v>
-      </c>
-      <c r="B193" t="s">
-        <v>1059</v>
-      </c>
-      <c r="C193" t="s">
-        <v>1085</v>
-      </c>
-      <c r="D193" t="s">
-        <v>1098</v>
-      </c>
-      <c r="E193" t="s">
+      <c r="F201" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B202" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C202" t="s">
+        <v>1088</v>
+      </c>
+      <c r="D202" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E202" t="s">
+        <v>1107</v>
+      </c>
+      <c r="F202" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B203" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C203" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D203" t="s">
+        <v>1102</v>
+      </c>
+      <c r="E203" t="s">
+        <v>1108</v>
+      </c>
+      <c r="F203" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B204" s="8" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C204" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D204" t="s">
+        <v>1135</v>
+      </c>
+      <c r="E204" t="s">
         <v>1132</v>
       </c>
-      <c r="F193" t="s">
-        <v>1118</v>
-      </c>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A194" s="8" t="s">
-        <v>1060</v>
-      </c>
-      <c r="B194" t="s">
-        <v>1061</v>
-      </c>
-      <c r="C194" t="s">
-        <v>1086</v>
-      </c>
-      <c r="D194" t="s">
-        <v>1099</v>
-      </c>
-      <c r="E194" t="s">
-        <v>1110</v>
-      </c>
-      <c r="F194" t="s">
-        <v>1119</v>
-      </c>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A195" s="8" t="s">
-        <v>1062</v>
-      </c>
-      <c r="B195" t="s">
-        <v>1063</v>
-      </c>
-      <c r="C195" t="s">
-        <v>1087</v>
-      </c>
-      <c r="D195" t="s">
-        <v>1100</v>
-      </c>
-      <c r="E195" t="s">
-        <v>1111</v>
-      </c>
-      <c r="F195" t="s">
-        <v>1120</v>
-      </c>
-    </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A196" s="8" t="s">
-        <v>1064</v>
-      </c>
-      <c r="B196" t="s">
-        <v>1065</v>
-      </c>
-      <c r="C196" t="s">
-        <v>1088</v>
-      </c>
-      <c r="D196" t="s">
-        <v>1101</v>
-      </c>
-      <c r="E196" t="s">
-        <v>1133</v>
-      </c>
-      <c r="F196" t="s">
-        <v>1121</v>
-      </c>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A197" t="s">
-        <v>1066</v>
-      </c>
-      <c r="B197" t="s">
-        <v>1067</v>
-      </c>
-      <c r="C197" t="s">
-        <v>1089</v>
-      </c>
-      <c r="D197" t="s">
-        <v>1102</v>
-      </c>
-      <c r="E197" t="s">
-        <v>1134</v>
-      </c>
-      <c r="F197" t="s">
-        <v>1122</v>
-      </c>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A198" s="8" t="s">
-        <v>1068</v>
-      </c>
-      <c r="B198" t="s">
-        <v>1069</v>
-      </c>
-      <c r="C198" t="s">
-        <v>1090</v>
-      </c>
-      <c r="D198" t="s">
-        <v>1103</v>
-      </c>
-      <c r="E198" t="s">
-        <v>1135</v>
-      </c>
-      <c r="F198" t="s">
-        <v>1123</v>
-      </c>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A199" t="s">
-        <v>1070</v>
-      </c>
-      <c r="B199" t="s">
-        <v>22</v>
-      </c>
-      <c r="C199" t="s">
-        <v>321</v>
-      </c>
-      <c r="D199" t="s">
-        <v>423</v>
-      </c>
-      <c r="E199" t="s">
-        <v>529</v>
-      </c>
-      <c r="F199" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A200" t="s">
-        <v>1071</v>
-      </c>
-      <c r="B200" t="s">
-        <v>1072</v>
-      </c>
-      <c r="C200" t="s">
-        <v>1091</v>
-      </c>
-      <c r="D200" t="s">
-        <v>1104</v>
-      </c>
-      <c r="E200" t="s">
+      <c r="F204" t="s">
         <v>1136</v>
       </c>
-      <c r="F200" t="s">
-        <v>1124</v>
-      </c>
-    </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A201" t="s">
-        <v>1073</v>
-      </c>
-      <c r="B201" t="s">
-        <v>1074</v>
-      </c>
-      <c r="C201" t="s">
-        <v>1092</v>
-      </c>
-      <c r="D201" t="s">
-        <v>1105</v>
-      </c>
-      <c r="E201" t="s">
-        <v>1112</v>
-      </c>
-      <c r="F201" t="s">
-        <v>1125</v>
-      </c>
-    </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A202" t="s">
-        <v>1075</v>
-      </c>
-      <c r="B202" t="s">
-        <v>1076</v>
-      </c>
-      <c r="C202" t="s">
-        <v>1093</v>
-      </c>
-      <c r="D202" t="s">
-        <v>1106</v>
-      </c>
-      <c r="E202" t="s">
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
         <v>1137</v>
       </c>
-      <c r="F202" t="s">
-        <v>1126</v>
-      </c>
-    </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A203" t="s">
-        <v>1077</v>
-      </c>
-      <c r="B203" t="s">
-        <v>1078</v>
-      </c>
-      <c r="C203" t="s">
-        <v>1094</v>
-      </c>
-      <c r="D203" t="s">
-        <v>1107</v>
-      </c>
-      <c r="E203" t="s">
-        <v>1113</v>
-      </c>
-      <c r="F203" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A204" t="s">
-        <v>1079</v>
-      </c>
-      <c r="B204" t="s">
-        <v>1081</v>
-      </c>
-      <c r="C204" t="s">
-        <v>1095</v>
-      </c>
-      <c r="D204" t="s">
-        <v>1108</v>
-      </c>
-      <c r="E204" t="s">
-        <v>1114</v>
-      </c>
-      <c r="F204" t="s">
-        <v>1128</v>
-      </c>
-    </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A205" t="s">
-        <v>1080</v>
-      </c>
-      <c r="B205" s="9" t="s">
-        <v>1139</v>
+      <c r="B205" t="s">
+        <v>1138</v>
       </c>
       <c r="C205" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="D205" t="s">
-        <v>1141</v>
+        <v>1138</v>
       </c>
       <c r="E205" t="s">
         <v>1138</v>
       </c>
       <c r="F205" t="s">
-        <v>1142</v>
-      </c>
-    </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>1143</v>
+        <v>1139</v>
       </c>
       <c r="B206" t="s">
-        <v>1144</v>
+        <v>1140</v>
       </c>
       <c r="C206" t="s">
-        <v>1144</v>
+        <v>1150</v>
       </c>
       <c r="D206" t="s">
         <v>1144</v>
       </c>
       <c r="E206" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="F206" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B207" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C207" t="s">
+        <v>1151</v>
+      </c>
+      <c r="D207" t="s">
+        <v>1147</v>
+      </c>
+      <c r="E207" t="s">
+        <v>1148</v>
+      </c>
+      <c r="F207" t="s">
         <v>1149</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A207" t="s">
-        <v>1145</v>
-      </c>
-      <c r="B207" t="s">
-        <v>1146</v>
-      </c>
-      <c r="C207" t="s">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A208" s="2" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B208" s="10" t="s">
+        <v>1153</v>
+      </c>
+      <c r="C208" t="s">
+        <v>1166</v>
+      </c>
+      <c r="D208" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E208" t="s">
+        <v>1180</v>
+      </c>
+      <c r="F208" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A209" s="2" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C209" t="s">
+        <v>1167</v>
+      </c>
+      <c r="D209" t="s">
+        <v>1174</v>
+      </c>
+      <c r="E209" t="s">
+        <v>1167</v>
+      </c>
+      <c r="F209" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A210" s="10" t="s">
         <v>1156</v>
       </c>
-      <c r="D207" t="s">
-        <v>1150</v>
-      </c>
-      <c r="E207" t="s">
-        <v>1151</v>
-      </c>
-      <c r="F207" t="s">
-        <v>1152</v>
-      </c>
-    </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A208" t="s">
-        <v>1147</v>
-      </c>
-      <c r="B208" t="s">
-        <v>1148</v>
-      </c>
-      <c r="C208" t="s">
+      <c r="B210" s="2" t="s">
         <v>1157</v>
       </c>
-      <c r="D208" t="s">
-        <v>1153</v>
-      </c>
-      <c r="E208" t="s">
-        <v>1154</v>
-      </c>
-      <c r="F208" t="s">
-        <v>1155</v>
-      </c>
-    </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A209" s="2" t="s">
+      <c r="C210" t="s">
+        <v>1168</v>
+      </c>
+      <c r="D210" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E210" t="s">
+        <v>1181</v>
+      </c>
+      <c r="F210" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A211" s="2" t="s">
         <v>1158</v>
       </c>
-      <c r="B209" s="11" t="s">
+      <c r="B211" s="2" t="s">
         <v>1159</v>
       </c>
-      <c r="C209" t="s">
+      <c r="C211" t="s">
+        <v>1169</v>
+      </c>
+      <c r="D211" t="s">
+        <v>1176</v>
+      </c>
+      <c r="E211" t="s">
+        <v>1182</v>
+      </c>
+      <c r="F211" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A212" s="10" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B212" s="10" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C212" t="s">
+        <v>1170</v>
+      </c>
+      <c r="D212" t="s">
+        <v>1177</v>
+      </c>
+      <c r="E212" t="s">
+        <v>1170</v>
+      </c>
+      <c r="F212" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A213" s="10" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C213" t="s">
+        <v>1171</v>
+      </c>
+      <c r="D213" t="s">
+        <v>1178</v>
+      </c>
+      <c r="E213" t="s">
+        <v>1163</v>
+      </c>
+      <c r="F213" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A214" s="2" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C214" t="s">
         <v>1172</v>
       </c>
-      <c r="D209" t="s">
+      <c r="D214" t="s">
         <v>1179</v>
       </c>
-      <c r="E209" t="s">
-        <v>1186</v>
-      </c>
-      <c r="F209" t="s">
+      <c r="E214" t="s">
+        <v>1183</v>
+      </c>
+      <c r="F214" t="s">
         <v>1190</v>
-      </c>
-    </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A210" s="2" t="s">
-        <v>1160</v>
-      </c>
-      <c r="B210" s="2" t="s">
-        <v>1161</v>
-      </c>
-      <c r="C210" t="s">
-        <v>1173</v>
-      </c>
-      <c r="D210" t="s">
-        <v>1180</v>
-      </c>
-      <c r="E210" t="s">
-        <v>1173</v>
-      </c>
-      <c r="F210" t="s">
-        <v>1191</v>
-      </c>
-    </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A211" s="11" t="s">
-        <v>1162</v>
-      </c>
-      <c r="B211" s="2" t="s">
-        <v>1163</v>
-      </c>
-      <c r="C211" t="s">
-        <v>1174</v>
-      </c>
-      <c r="D211" t="s">
-        <v>1181</v>
-      </c>
-      <c r="E211" t="s">
-        <v>1187</v>
-      </c>
-      <c r="F211" t="s">
-        <v>1192</v>
-      </c>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A212" s="2" t="s">
-        <v>1164</v>
-      </c>
-      <c r="B212" s="2" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C212" t="s">
-        <v>1175</v>
-      </c>
-      <c r="D212" t="s">
-        <v>1182</v>
-      </c>
-      <c r="E212" t="s">
-        <v>1188</v>
-      </c>
-      <c r="F212" t="s">
-        <v>1193</v>
-      </c>
-    </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A213" s="11" t="s">
-        <v>1166</v>
-      </c>
-      <c r="B213" s="11" t="s">
-        <v>1167</v>
-      </c>
-      <c r="C213" t="s">
-        <v>1176</v>
-      </c>
-      <c r="D213" t="s">
-        <v>1183</v>
-      </c>
-      <c r="E213" t="s">
-        <v>1176</v>
-      </c>
-      <c r="F213" t="s">
-        <v>1194</v>
-      </c>
-    </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A214" s="11" t="s">
-        <v>1168</v>
-      </c>
-      <c r="B214" s="2" t="s">
-        <v>1169</v>
-      </c>
-      <c r="C214" t="s">
-        <v>1177</v>
-      </c>
-      <c r="D214" t="s">
-        <v>1184</v>
-      </c>
-      <c r="E214" t="s">
-        <v>1169</v>
-      </c>
-      <c r="F214" t="s">
-        <v>1195</v>
-      </c>
-    </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A215" s="2" t="s">
-        <v>1170</v>
-      </c>
-      <c r="B215" s="2" t="s">
-        <v>1171</v>
-      </c>
-      <c r="C215" t="s">
-        <v>1178</v>
-      </c>
-      <c r="D215" t="s">
-        <v>1185</v>
-      </c>
-      <c r="E215" t="s">
-        <v>1189</v>
-      </c>
-      <c r="F215" t="s">
-        <v>1196</v>
       </c>
     </row>
   </sheetData>
@@ -8388,17 +8347,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="6e0cf07b-8188-4b76-8f54-3cda03d37414" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="43e153a8-5ef1-4f65-aac7-dc4685f18eaa">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F12BE0DB4A3DF641BF113FBF1C7EA261" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="718598463bd34fa12e450bcb3a6783b8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="43e153a8-5ef1-4f65-aac7-dc4685f18eaa" xmlns:ns3="6e0cf07b-8188-4b76-8f54-3cda03d37414" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="54cbcd1ebcb6479b13808205dc2a6520" ns2:_="" ns3:_="">
     <xsd:import namespace="43e153a8-5ef1-4f65-aac7-dc4685f18eaa"/>
@@ -8627,6 +8575,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="6e0cf07b-8188-4b76-8f54-3cda03d37414" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="43e153a8-5ef1-4f65-aac7-dc4685f18eaa">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -8637,23 +8596,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E20926E-9EFB-4B7E-90D4-905B08F8E59C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="6e0cf07b-8188-4b76-8f54-3cda03d37414"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="43e153a8-5ef1-4f65-aac7-dc4685f18eaa"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBDDFBA8-FF97-4684-8DBF-782A9A0E4D0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8672,6 +8614,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E20926E-9EFB-4B7E-90D4-905B08F8E59C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="6e0cf07b-8188-4b76-8f54-3cda03d37414"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="43e153a8-5ef1-4f65-aac7-dc4685f18eaa"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04FEE910-FEC8-48C6-9CF9-BF01BA5AD6FE}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fixed multiple polygon layers issue with the PerformCollectionFragment.
</commit_message>
<xml_diff>
--- a/translations/translations.xlsx
+++ b/translations/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rmitchell64/Desktop/Projects/GPSSample/gpssample/translations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E98F386-ADF2-9348-9096-355BB7D90906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED514AC-FE8B-0646-93B4-CC346E0867BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24540" yWindow="3360" windowWidth="36140" windowHeight="20720" xr2:uid="{C8C8ACD1-4E76-7942-B525-8D880B4ECA80}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20380" xr2:uid="{C8C8ACD1-4E76-7942-B525-8D880B4ECA80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1518" uniqueCount="1373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="1369">
   <si>
     <t>Settings</t>
   </si>
@@ -2781,9 +2781,6 @@
     <t>Los datos de enumeración se han guardado en el directorio Documentos.</t>
   </si>
   <si>
-    <t>&gt;Localización no encontrada</t>
-  </si>
-  <si>
     <t>¡Oops! Por favor, seleccione una razón para incompleto</t>
   </si>
   <si>
@@ -2874,9 +2871,6 @@
     <t>Les données d'énumération ont été sauvegardées dans le répertoire Documents.</t>
   </si>
   <si>
-    <t>&gt;La configuration a été sauvegardée dans le répertoire Documents.</t>
-  </si>
-  <si>
     <t>Le domicile n'existe pas</t>
   </si>
   <si>
@@ -2916,9 +2910,6 @@
     <t>Os dados de enumeração foram guardados no diretório Documentos.</t>
   </si>
   <si>
-    <t>&gt;Localização não encontrada</t>
-  </si>
-  <si>
     <t>Пожалуйста, подтвердите</t>
   </si>
   <si>
@@ -3019,9 +3010,6 @@
   </si>
   <si>
     <t>Конфигурация была сохранена в каталог Documents.</t>
-  </si>
-  <si>
-    <t>&gt;Местонахождение не найдено</t>
   </si>
   <si>
     <t>Дом не существует</t>
@@ -4234,13 +4222,13 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
@@ -4637,8 +4625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD3E6CC-854C-5841-9577-D3ADD2982DB6}">
   <dimension ref="A1:F253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A218" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C187" sqref="C187"/>
+    <sheetView tabSelected="1" topLeftCell="A166" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B191" sqref="B191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4648,6 +4636,9 @@
     <col min="3" max="3" width="32.6640625" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
     <col min="5" max="5" width="41" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.1640625" customWidth="1"/>
+    <col min="7" max="7" width="42.6640625" customWidth="1"/>
+    <col min="8" max="8" width="44.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -4761,7 +4752,7 @@
         <v>291</v>
       </c>
       <c r="D6" t="s">
-        <v>1324</v>
+        <v>1320</v>
       </c>
       <c r="E6" t="s">
         <v>291</v>
@@ -4961,7 +4952,7 @@
         <v>735</v>
       </c>
       <c r="D16" t="s">
-        <v>1325</v>
+        <v>1321</v>
       </c>
       <c r="E16" t="s">
         <v>744</v>
@@ -5021,7 +5012,7 @@
         <v>736</v>
       </c>
       <c r="D19" t="s">
-        <v>1326</v>
+        <v>1322</v>
       </c>
       <c r="E19" t="s">
         <v>500</v>
@@ -5041,7 +5032,7 @@
         <v>318</v>
       </c>
       <c r="D20" t="s">
-        <v>1327</v>
+        <v>1323</v>
       </c>
       <c r="E20" t="s">
         <v>745</v>
@@ -5061,7 +5052,7 @@
         <v>779</v>
       </c>
       <c r="D21" t="s">
-        <v>1328</v>
+        <v>1324</v>
       </c>
       <c r="E21" t="s">
         <v>501</v>
@@ -5081,7 +5072,7 @@
         <v>320</v>
       </c>
       <c r="D22" t="s">
-        <v>1329</v>
+        <v>1325</v>
       </c>
       <c r="E22" t="s">
         <v>320</v>
@@ -5361,7 +5352,7 @@
         <v>505</v>
       </c>
       <c r="D36" t="s">
-        <v>1330</v>
+        <v>1326</v>
       </c>
       <c r="E36" t="s">
         <v>505</v>
@@ -5401,7 +5392,7 @@
         <v>306</v>
       </c>
       <c r="D38" t="s">
-        <v>1331</v>
+        <v>1327</v>
       </c>
       <c r="E38" t="s">
         <v>750</v>
@@ -5721,7 +5712,7 @@
         <v>322</v>
       </c>
       <c r="D54" t="s">
-        <v>1332</v>
+        <v>1328</v>
       </c>
       <c r="E54" t="s">
         <v>515</v>
@@ -5741,7 +5732,7 @@
         <v>784</v>
       </c>
       <c r="D55" t="s">
-        <v>1333</v>
+        <v>1329</v>
       </c>
       <c r="E55" t="s">
         <v>516</v>
@@ -5761,7 +5752,7 @@
         <v>725</v>
       </c>
       <c r="D56" t="s">
-        <v>1334</v>
+        <v>1330</v>
       </c>
       <c r="E56" t="s">
         <v>752</v>
@@ -5821,7 +5812,7 @@
         <v>356</v>
       </c>
       <c r="D59" t="s">
-        <v>1335</v>
+        <v>1331</v>
       </c>
       <c r="E59" t="s">
         <v>517</v>
@@ -5941,7 +5932,7 @@
         <v>785</v>
       </c>
       <c r="D65" t="s">
-        <v>1337</v>
+        <v>1333</v>
       </c>
       <c r="E65" t="s">
         <v>358</v>
@@ -5981,7 +5972,7 @@
         <v>786</v>
       </c>
       <c r="D67" t="s">
-        <v>1336</v>
+        <v>1332</v>
       </c>
       <c r="E67" t="s">
         <v>290</v>
@@ -6001,7 +5992,7 @@
         <v>289</v>
       </c>
       <c r="D68" t="s">
-        <v>1338</v>
+        <v>1334</v>
       </c>
       <c r="E68" t="s">
         <v>521</v>
@@ -6041,7 +6032,7 @@
         <v>802</v>
       </c>
       <c r="D70" t="s">
-        <v>1339</v>
+        <v>1335</v>
       </c>
       <c r="E70" t="s">
         <v>777</v>
@@ -6061,7 +6052,7 @@
         <v>803</v>
       </c>
       <c r="D71" t="s">
-        <v>1340</v>
+        <v>1336</v>
       </c>
       <c r="E71" t="s">
         <v>778</v>
@@ -6141,7 +6132,7 @@
         <v>788</v>
       </c>
       <c r="D75" t="s">
-        <v>1341</v>
+        <v>1337</v>
       </c>
       <c r="E75" t="s">
         <v>524</v>
@@ -6221,7 +6212,7 @@
         <v>789</v>
       </c>
       <c r="D79" s="15" t="s">
-        <v>1342</v>
+        <v>1338</v>
       </c>
       <c r="E79" t="s">
         <v>526</v>
@@ -6241,7 +6232,7 @@
         <v>790</v>
       </c>
       <c r="D80" s="15" t="s">
-        <v>1343</v>
+        <v>1339</v>
       </c>
       <c r="E80" t="s">
         <v>527</v>
@@ -6421,7 +6412,7 @@
         <v>792</v>
       </c>
       <c r="D89" t="s">
-        <v>1344</v>
+        <v>1340</v>
       </c>
       <c r="E89" t="s">
         <v>535</v>
@@ -6561,7 +6552,7 @@
         <v>363</v>
       </c>
       <c r="D96" s="15" t="s">
-        <v>1345</v>
+        <v>1341</v>
       </c>
       <c r="E96" t="s">
         <v>363</v>
@@ -6581,7 +6572,7 @@
         <v>364</v>
       </c>
       <c r="D97" t="s">
-        <v>1346</v>
+        <v>1342</v>
       </c>
       <c r="E97" t="s">
         <v>539</v>
@@ -6681,7 +6672,7 @@
         <v>367</v>
       </c>
       <c r="D102" s="15" t="s">
-        <v>1347</v>
+        <v>1343</v>
       </c>
       <c r="E102" t="s">
         <v>765</v>
@@ -6881,7 +6872,7 @@
         <v>796</v>
       </c>
       <c r="D112" t="s">
-        <v>1348</v>
+        <v>1344</v>
       </c>
       <c r="E112" t="s">
         <v>549</v>
@@ -6921,7 +6912,7 @@
         <v>798</v>
       </c>
       <c r="D114" s="15" t="s">
-        <v>1361</v>
+        <v>1357</v>
       </c>
       <c r="E114" t="s">
         <v>551</v>
@@ -6961,7 +6952,7 @@
         <v>353</v>
       </c>
       <c r="D116" t="s">
-        <v>1349</v>
+        <v>1345</v>
       </c>
       <c r="E116" t="s">
         <v>552</v>
@@ -7501,7 +7492,7 @@
         <v>348</v>
       </c>
       <c r="D143" t="s">
-        <v>1350</v>
+        <v>1346</v>
       </c>
       <c r="E143" t="s">
         <v>775</v>
@@ -7658,16 +7649,16 @@
         <v>880</v>
       </c>
       <c r="C151" t="s">
-        <v>992</v>
+        <v>988</v>
       </c>
       <c r="D151" t="s">
-        <v>1351</v>
+        <v>1347</v>
       </c>
       <c r="E151" t="s">
-        <v>992</v>
+        <v>988</v>
       </c>
       <c r="F151" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
@@ -7681,13 +7672,13 @@
         <v>881</v>
       </c>
       <c r="D152" t="s">
-        <v>1352</v>
+        <v>1348</v>
       </c>
       <c r="E152" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="F152" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
@@ -7701,13 +7692,13 @@
         <v>882</v>
       </c>
       <c r="D153" t="s">
-        <v>1353</v>
+        <v>1349</v>
       </c>
       <c r="E153" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="F153" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
@@ -7721,13 +7712,13 @@
         <v>883</v>
       </c>
       <c r="D154" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="E154" t="s">
-        <v>996</v>
+        <v>992</v>
       </c>
       <c r="F154" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
@@ -7741,13 +7732,13 @@
         <v>884</v>
       </c>
       <c r="D155" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="E155" t="s">
-        <v>997</v>
+        <v>993</v>
       </c>
       <c r="F155" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
@@ -7761,13 +7752,13 @@
         <v>885</v>
       </c>
       <c r="D156" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="E156" t="s">
-        <v>998</v>
+        <v>994</v>
       </c>
       <c r="F156" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.2">
@@ -7781,13 +7772,13 @@
         <v>886</v>
       </c>
       <c r="D157" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="E157" t="s">
-        <v>999</v>
+        <v>995</v>
       </c>
       <c r="F157" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.2">
@@ -7801,13 +7792,13 @@
         <v>887</v>
       </c>
       <c r="D158" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="E158" t="s">
-        <v>1000</v>
+        <v>996</v>
       </c>
       <c r="F158" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.2">
@@ -7821,13 +7812,13 @@
         <v>888</v>
       </c>
       <c r="D159" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="E159" t="s">
-        <v>1001</v>
+        <v>997</v>
       </c>
       <c r="F159" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.2">
@@ -7841,13 +7832,13 @@
         <v>889</v>
       </c>
       <c r="D160" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="E160" t="s">
-        <v>1002</v>
+        <v>998</v>
       </c>
       <c r="F160" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.2">
@@ -7861,13 +7852,13 @@
         <v>890</v>
       </c>
       <c r="D161" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="E161" t="s">
-        <v>1002</v>
+        <v>998</v>
       </c>
       <c r="F161" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.2">
@@ -7881,13 +7872,13 @@
         <v>891</v>
       </c>
       <c r="D162" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="E162" t="s">
-        <v>1003</v>
+        <v>999</v>
       </c>
       <c r="F162" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.2">
@@ -7901,13 +7892,13 @@
         <v>892</v>
       </c>
       <c r="D163" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="E163" t="s">
-        <v>1004</v>
+        <v>1000</v>
       </c>
       <c r="F163" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.2">
@@ -7921,13 +7912,13 @@
         <v>893</v>
       </c>
       <c r="D164" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="E164" t="s">
-        <v>1005</v>
+        <v>1001</v>
       </c>
       <c r="F164" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.2">
@@ -7941,13 +7932,13 @@
         <v>894</v>
       </c>
       <c r="D165" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="E165" t="s">
-        <v>1006</v>
+        <v>1002</v>
       </c>
       <c r="F165" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.2">
@@ -7961,13 +7952,13 @@
         <v>895</v>
       </c>
       <c r="D166" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="E166" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="F166" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.2">
@@ -7981,13 +7972,13 @@
         <v>896</v>
       </c>
       <c r="D167" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="E167" t="s">
-        <v>1007</v>
+        <v>1003</v>
       </c>
       <c r="F167" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.2">
@@ -7998,16 +7989,16 @@
         <v>864</v>
       </c>
       <c r="C168" t="s">
-        <v>993</v>
+        <v>989</v>
       </c>
       <c r="D168" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="E168" t="s">
-        <v>1008</v>
+        <v>1004</v>
       </c>
       <c r="F168" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.2">
@@ -8021,13 +8012,13 @@
         <v>897</v>
       </c>
       <c r="D169" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="E169" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="F169" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.2">
@@ -8041,13 +8032,13 @@
         <v>898</v>
       </c>
       <c r="D170" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="E170" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="F170" t="s">
-        <v>974</v>
+        <v>971</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.2">
@@ -8061,13 +8052,13 @@
         <v>899</v>
       </c>
       <c r="D171" t="s">
-        <v>1354</v>
+        <v>1350</v>
       </c>
       <c r="E171" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
       <c r="F171" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.2">
@@ -8081,13 +8072,13 @@
         <v>900</v>
       </c>
       <c r="D172" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="E172" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="F172" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.2">
@@ -8101,13 +8092,13 @@
         <v>860</v>
       </c>
       <c r="D173" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="E173" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="F173" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.2">
@@ -8121,13 +8112,13 @@
         <v>901</v>
       </c>
       <c r="D174" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="E174" t="s">
         <v>901</v>
       </c>
       <c r="F174" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.2">
@@ -8141,13 +8132,13 @@
         <v>902</v>
       </c>
       <c r="D175" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="E175" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="F175" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.2">
@@ -8161,13 +8152,13 @@
         <v>903</v>
       </c>
       <c r="D176" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="E176" t="s">
-        <v>1011</v>
+        <v>1007</v>
       </c>
       <c r="F176" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
@@ -8181,13 +8172,13 @@
         <v>904</v>
       </c>
       <c r="D177" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="E177" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="F177" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.2">
@@ -8198,16 +8189,16 @@
         <v>855</v>
       </c>
       <c r="C178" t="s">
-        <v>994</v>
+        <v>990</v>
       </c>
       <c r="D178" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="E178" t="s">
-        <v>1012</v>
+        <v>1008</v>
       </c>
       <c r="F178" t="s">
-        <v>982</v>
+        <v>979</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
@@ -8218,16 +8209,16 @@
         <v>854</v>
       </c>
       <c r="C179" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="D179" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="E179" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="F179" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.2">
@@ -8241,13 +8232,13 @@
         <v>905</v>
       </c>
       <c r="D180" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="E180" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="F180" t="s">
-        <v>984</v>
+        <v>981</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.2">
@@ -8261,13 +8252,13 @@
         <v>891</v>
       </c>
       <c r="D181" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="E181" t="s">
-        <v>1003</v>
+        <v>999</v>
       </c>
       <c r="F181" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.2">
@@ -8281,13 +8272,13 @@
         <v>906</v>
       </c>
       <c r="D182" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="E182" t="s">
-        <v>1014</v>
+        <v>1010</v>
       </c>
       <c r="F182" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.2">
@@ -8301,13 +8292,13 @@
         <v>906</v>
       </c>
       <c r="D183" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="E183" t="s">
-        <v>1014</v>
+        <v>1010</v>
       </c>
       <c r="F183" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.2">
@@ -8321,13 +8312,13 @@
         <v>907</v>
       </c>
       <c r="D184" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="E184" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="F184" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.2">
@@ -8341,13 +8332,13 @@
         <v>908</v>
       </c>
       <c r="D185" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="E185" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="F185" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.2">
@@ -8361,13 +8352,13 @@
         <v>895</v>
       </c>
       <c r="D186" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="E186" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="F186" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.2">
@@ -8375,19 +8366,7 @@
         <v>843</v>
       </c>
       <c r="B187" s="19" t="s">
-        <v>1372</v>
-      </c>
-      <c r="C187" t="s">
-        <v>909</v>
-      </c>
-      <c r="D187" t="s">
-        <v>940</v>
-      </c>
-      <c r="E187" t="s">
-        <v>954</v>
-      </c>
-      <c r="F187" t="s">
-        <v>989</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.2">
@@ -8398,16 +8377,16 @@
         <v>847</v>
       </c>
       <c r="C188" s="7" t="s">
-        <v>1017</v>
+        <v>1013</v>
       </c>
       <c r="D188" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="E188" s="9" t="s">
-        <v>1016</v>
+        <v>1012</v>
       </c>
       <c r="F188" t="s">
-        <v>990</v>
+        <v>986</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.2">
@@ -8418,201 +8397,201 @@
         <v>846</v>
       </c>
       <c r="C189" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="D189" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="E189" t="s">
-        <v>1015</v>
+        <v>1011</v>
       </c>
       <c r="F189" t="s">
-        <v>991</v>
+        <v>987</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190" s="4" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="B190" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="C190" t="s">
-        <v>1048</v>
+        <v>1044</v>
       </c>
       <c r="D190" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
       <c r="E190" t="s">
-        <v>1095</v>
+        <v>1091</v>
       </c>
       <c r="F190" t="s">
-        <v>1081</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191" s="4" t="s">
-        <v>1020</v>
+        <v>1016</v>
       </c>
       <c r="B191" s="5" t="s">
-        <v>1021</v>
+        <v>1017</v>
       </c>
       <c r="C191" t="s">
-        <v>1049</v>
+        <v>1045</v>
       </c>
       <c r="D191" t="s">
-        <v>1075</v>
+        <v>1071</v>
       </c>
       <c r="E191" t="s">
-        <v>1096</v>
+        <v>1092</v>
       </c>
       <c r="F191" t="s">
-        <v>1082</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192" s="4" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="B192" t="s">
-        <v>1023</v>
+        <v>1019</v>
       </c>
       <c r="C192" t="s">
-        <v>1050</v>
+        <v>1046</v>
       </c>
       <c r="D192" t="s">
-        <v>1063</v>
+        <v>1059</v>
       </c>
       <c r="E192" t="s">
-        <v>1097</v>
+        <v>1093</v>
       </c>
       <c r="F192" t="s">
-        <v>1083</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193" s="4" t="s">
-        <v>1024</v>
+        <v>1020</v>
       </c>
       <c r="B193" t="s">
-        <v>1025</v>
+        <v>1021</v>
       </c>
       <c r="C193" t="s">
-        <v>1051</v>
+        <v>1047</v>
       </c>
       <c r="D193" t="s">
-        <v>1064</v>
+        <v>1060</v>
       </c>
       <c r="E193" t="s">
-        <v>1098</v>
+        <v>1094</v>
       </c>
       <c r="F193" t="s">
-        <v>1084</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194" s="4" t="s">
-        <v>1026</v>
+        <v>1022</v>
       </c>
       <c r="B194" t="s">
-        <v>1027</v>
+        <v>1023</v>
       </c>
       <c r="C194" t="s">
-        <v>1052</v>
+        <v>1048</v>
       </c>
       <c r="D194" t="s">
-        <v>1065</v>
+        <v>1061</v>
       </c>
       <c r="E194" t="s">
-        <v>1076</v>
+        <v>1072</v>
       </c>
       <c r="F194" t="s">
-        <v>1085</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195" s="4" t="s">
-        <v>1028</v>
+        <v>1024</v>
       </c>
       <c r="B195" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="C195" t="s">
-        <v>1053</v>
+        <v>1049</v>
       </c>
       <c r="D195" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="E195" t="s">
-        <v>1077</v>
+        <v>1073</v>
       </c>
       <c r="F195" t="s">
-        <v>1086</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196" s="4" t="s">
-        <v>1030</v>
+        <v>1026</v>
       </c>
       <c r="B196" t="s">
-        <v>1031</v>
+        <v>1027</v>
       </c>
       <c r="C196" t="s">
-        <v>1054</v>
+        <v>1050</v>
       </c>
       <c r="D196" t="s">
-        <v>1067</v>
+        <v>1063</v>
       </c>
       <c r="E196" t="s">
-        <v>1099</v>
+        <v>1095</v>
       </c>
       <c r="F196" t="s">
-        <v>1087</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>1032</v>
+        <v>1028</v>
       </c>
       <c r="B197" t="s">
-        <v>1033</v>
+        <v>1029</v>
       </c>
       <c r="C197" t="s">
-        <v>1055</v>
+        <v>1051</v>
       </c>
       <c r="D197" t="s">
-        <v>1068</v>
+        <v>1064</v>
       </c>
       <c r="E197" t="s">
-        <v>1100</v>
+        <v>1096</v>
       </c>
       <c r="F197" t="s">
-        <v>1088</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198" s="4" t="s">
-        <v>1034</v>
+        <v>1030</v>
       </c>
       <c r="B198" t="s">
-        <v>1035</v>
+        <v>1031</v>
       </c>
       <c r="C198" t="s">
-        <v>1056</v>
+        <v>1052</v>
       </c>
       <c r="D198" t="s">
-        <v>1069</v>
+        <v>1065</v>
       </c>
       <c r="E198" t="s">
-        <v>1101</v>
+        <v>1097</v>
       </c>
       <c r="F198" t="s">
-        <v>1089</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>1036</v>
+        <v>1032</v>
       </c>
       <c r="B199" t="s">
         <v>22</v>
@@ -8632,327 +8611,327 @@
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>1037</v>
+        <v>1033</v>
       </c>
       <c r="B200" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="C200" t="s">
-        <v>1057</v>
+        <v>1053</v>
       </c>
       <c r="D200" t="s">
-        <v>1070</v>
+        <v>1066</v>
       </c>
       <c r="E200" t="s">
-        <v>1102</v>
+        <v>1098</v>
       </c>
       <c r="F200" t="s">
-        <v>1090</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>1039</v>
+        <v>1035</v>
       </c>
       <c r="B201" t="s">
-        <v>1040</v>
+        <v>1036</v>
       </c>
       <c r="C201" t="s">
-        <v>1058</v>
+        <v>1054</v>
       </c>
       <c r="D201" t="s">
-        <v>1071</v>
+        <v>1067</v>
       </c>
       <c r="E201" t="s">
-        <v>1078</v>
+        <v>1074</v>
       </c>
       <c r="F201" t="s">
-        <v>1091</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>1041</v>
+        <v>1037</v>
       </c>
       <c r="B202" t="s">
-        <v>1042</v>
+        <v>1038</v>
       </c>
       <c r="C202" t="s">
-        <v>1059</v>
+        <v>1055</v>
       </c>
       <c r="D202" t="s">
-        <v>1072</v>
+        <v>1068</v>
       </c>
       <c r="E202" t="s">
-        <v>1103</v>
+        <v>1099</v>
       </c>
       <c r="F202" t="s">
-        <v>1092</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>1043</v>
+        <v>1039</v>
       </c>
       <c r="B203" t="s">
-        <v>1044</v>
+        <v>1040</v>
       </c>
       <c r="C203" t="s">
-        <v>1060</v>
+        <v>1056</v>
       </c>
       <c r="D203" t="s">
-        <v>1073</v>
+        <v>1069</v>
       </c>
       <c r="E203" t="s">
-        <v>1079</v>
+        <v>1075</v>
       </c>
       <c r="F203" t="s">
-        <v>1093</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>1045</v>
+        <v>1041</v>
       </c>
       <c r="B204" t="s">
-        <v>1047</v>
+        <v>1043</v>
       </c>
       <c r="C204" t="s">
-        <v>1061</v>
+        <v>1057</v>
       </c>
       <c r="D204" t="s">
-        <v>1074</v>
+        <v>1070</v>
       </c>
       <c r="E204" t="s">
-        <v>1080</v>
+        <v>1076</v>
       </c>
       <c r="F204" t="s">
-        <v>1094</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>1046</v>
+        <v>1042</v>
       </c>
       <c r="B205" s="8" t="s">
-        <v>1105</v>
+        <v>1101</v>
       </c>
       <c r="C205" t="s">
-        <v>1106</v>
+        <v>1102</v>
       </c>
       <c r="D205" t="s">
-        <v>1107</v>
+        <v>1103</v>
       </c>
       <c r="E205" t="s">
+        <v>1100</v>
+      </c>
+      <c r="F205" t="s">
         <v>1104</v>
-      </c>
-      <c r="F205" t="s">
-        <v>1108</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>1109</v>
+        <v>1105</v>
       </c>
       <c r="B206" t="s">
-        <v>1110</v>
+        <v>1106</v>
       </c>
       <c r="C206" t="s">
-        <v>1110</v>
+        <v>1106</v>
       </c>
       <c r="D206" t="s">
-        <v>1110</v>
+        <v>1106</v>
       </c>
       <c r="E206" t="s">
-        <v>1110</v>
+        <v>1106</v>
       </c>
       <c r="F206" t="s">
-        <v>1115</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="B207" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C207" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D207" t="s">
         <v>1112</v>
       </c>
-      <c r="C207" t="s">
-        <v>1122</v>
-      </c>
-      <c r="D207" t="s">
-        <v>1116</v>
-      </c>
       <c r="E207" t="s">
-        <v>1117</v>
+        <v>1113</v>
       </c>
       <c r="F207" t="s">
-        <v>1118</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>1113</v>
+        <v>1109</v>
       </c>
       <c r="B208" t="s">
-        <v>1114</v>
+        <v>1110</v>
       </c>
       <c r="C208" t="s">
-        <v>1123</v>
+        <v>1119</v>
       </c>
       <c r="D208" t="s">
-        <v>1119</v>
+        <v>1115</v>
       </c>
       <c r="E208" t="s">
-        <v>1120</v>
+        <v>1116</v>
       </c>
       <c r="F208" t="s">
-        <v>1121</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A209" s="2" t="s">
-        <v>1124</v>
+        <v>1120</v>
       </c>
       <c r="B209" s="10" t="s">
-        <v>1125</v>
+        <v>1121</v>
       </c>
       <c r="C209" t="s">
-        <v>1138</v>
+        <v>1134</v>
       </c>
       <c r="D209" t="s">
-        <v>1145</v>
+        <v>1141</v>
       </c>
       <c r="E209" t="s">
+        <v>1148</v>
+      </c>
+      <c r="F209" t="s">
         <v>1152</v>
-      </c>
-      <c r="F209" t="s">
-        <v>1156</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A210" s="2" t="s">
-        <v>1126</v>
+        <v>1122</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
       <c r="C210" t="s">
-        <v>1139</v>
+        <v>1135</v>
       </c>
       <c r="D210" t="s">
-        <v>1146</v>
+        <v>1142</v>
       </c>
       <c r="E210" t="s">
-        <v>1139</v>
+        <v>1135</v>
       </c>
       <c r="F210" t="s">
-        <v>1157</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A211" s="10" t="s">
-        <v>1128</v>
+        <v>1124</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>1129</v>
+        <v>1125</v>
       </c>
       <c r="C211" t="s">
-        <v>1140</v>
+        <v>1136</v>
       </c>
       <c r="D211" t="s">
-        <v>1147</v>
+        <v>1143</v>
       </c>
       <c r="E211" t="s">
-        <v>1153</v>
+        <v>1149</v>
       </c>
       <c r="F211" t="s">
-        <v>1158</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A212" s="2" t="s">
-        <v>1130</v>
+        <v>1126</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>1131</v>
+        <v>1127</v>
       </c>
       <c r="C212" t="s">
-        <v>1141</v>
+        <v>1137</v>
       </c>
       <c r="D212" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="E212" t="s">
-        <v>1154</v>
+        <v>1150</v>
       </c>
       <c r="F212" t="s">
-        <v>1159</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A213" s="10" t="s">
-        <v>1132</v>
+        <v>1128</v>
       </c>
       <c r="B213" s="10" t="s">
-        <v>1133</v>
+        <v>1129</v>
       </c>
       <c r="C213" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
       <c r="D213" t="s">
-        <v>1149</v>
+        <v>1145</v>
       </c>
       <c r="E213" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
       <c r="F213" t="s">
-        <v>1160</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A214" s="10" t="s">
-        <v>1134</v>
+        <v>1130</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>1135</v>
+        <v>1131</v>
       </c>
       <c r="C214" t="s">
-        <v>1143</v>
+        <v>1139</v>
       </c>
       <c r="D214" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
       <c r="E214" t="s">
-        <v>1135</v>
+        <v>1131</v>
       </c>
       <c r="F214" t="s">
-        <v>1161</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A215" s="2" t="s">
-        <v>1136</v>
+        <v>1132</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>1137</v>
+        <v>1133</v>
       </c>
       <c r="C215" t="s">
-        <v>1144</v>
+        <v>1140</v>
       </c>
       <c r="D215" t="s">
+        <v>1147</v>
+      </c>
+      <c r="E215" t="s">
         <v>1151</v>
       </c>
-      <c r="E215" t="s">
-        <v>1155</v>
-      </c>
       <c r="F215" t="s">
-        <v>1162</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A216" s="11" t="s">
-        <v>1163</v>
+        <v>1159</v>
       </c>
       <c r="B216" s="12" t="s">
         <v>28</v>
@@ -8961,18 +8940,18 @@
         <v>303</v>
       </c>
       <c r="D216" s="13" t="s">
-        <v>1299</v>
+        <v>1295</v>
       </c>
       <c r="E216" s="13" t="s">
         <v>303</v>
       </c>
       <c r="F216" s="13" t="s">
-        <v>1228</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A217" s="14" t="s">
-        <v>1164</v>
+        <v>1160</v>
       </c>
       <c r="B217" s="13" t="s">
         <v>27</v>
@@ -8992,7 +8971,7 @@
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A218" s="14" t="s">
-        <v>1165</v>
+        <v>1161</v>
       </c>
       <c r="B218" s="13" t="s">
         <v>30</v>
@@ -9012,147 +8991,147 @@
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A219" s="14" t="s">
-        <v>1166</v>
+        <v>1162</v>
       </c>
       <c r="B219" s="13" t="s">
-        <v>1167</v>
+        <v>1163</v>
       </c>
       <c r="C219" s="13" t="s">
-        <v>1277</v>
+        <v>1273</v>
       </c>
       <c r="D219" s="13" t="s">
-        <v>1300</v>
+        <v>1296</v>
       </c>
       <c r="E219" s="13" t="s">
-        <v>1257</v>
+        <v>1253</v>
       </c>
       <c r="F219" s="13" t="s">
-        <v>1229</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A220" s="13" t="s">
-        <v>1168</v>
+        <v>1164</v>
       </c>
       <c r="B220" s="13" t="s">
-        <v>1169</v>
+        <v>1165</v>
       </c>
       <c r="C220" s="13" t="s">
-        <v>1278</v>
+        <v>1274</v>
       </c>
       <c r="D220" s="13" t="s">
-        <v>1301</v>
+        <v>1297</v>
       </c>
       <c r="E220" s="13" t="s">
-        <v>1258</v>
+        <v>1254</v>
       </c>
       <c r="F220" s="13" t="s">
-        <v>1230</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A221" s="14" t="s">
-        <v>1170</v>
+        <v>1166</v>
       </c>
       <c r="B221" s="13" t="s">
-        <v>1171</v>
+        <v>1167</v>
       </c>
       <c r="C221" s="13" t="s">
-        <v>1279</v>
+        <v>1275</v>
       </c>
       <c r="D221" s="13" t="s">
-        <v>1302</v>
+        <v>1298</v>
       </c>
       <c r="E221" s="17" t="s">
-        <v>1368</v>
+        <v>1364</v>
       </c>
       <c r="F221" s="13" t="s">
-        <v>1231</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A222" s="14" t="s">
-        <v>1172</v>
+        <v>1168</v>
       </c>
       <c r="B222" s="13" t="s">
-        <v>1173</v>
+        <v>1169</v>
       </c>
       <c r="C222" s="13" t="s">
-        <v>1280</v>
+        <v>1276</v>
       </c>
       <c r="D222" s="13" t="s">
-        <v>1303</v>
+        <v>1299</v>
       </c>
       <c r="E222" s="13" t="s">
-        <v>1259</v>
+        <v>1255</v>
       </c>
       <c r="F222" s="13" t="s">
-        <v>1232</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A223" s="14" t="s">
-        <v>1174</v>
+        <v>1170</v>
       </c>
       <c r="B223" s="13" t="s">
-        <v>1175</v>
+        <v>1171</v>
       </c>
       <c r="C223" s="13" t="s">
-        <v>1281</v>
+        <v>1277</v>
       </c>
       <c r="D223" s="13" t="s">
-        <v>1304</v>
+        <v>1300</v>
       </c>
       <c r="E223" s="17" t="s">
-        <v>1369</v>
+        <v>1365</v>
       </c>
       <c r="F223" s="13" t="s">
-        <v>1233</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A224" s="14" t="s">
-        <v>1176</v>
+        <v>1172</v>
       </c>
       <c r="B224" s="13" t="s">
-        <v>1177</v>
+        <v>1173</v>
       </c>
       <c r="C224" s="13" t="s">
-        <v>1282</v>
+        <v>1278</v>
       </c>
       <c r="D224" s="13" t="s">
-        <v>1305</v>
+        <v>1301</v>
       </c>
       <c r="E224" s="13" t="s">
-        <v>1260</v>
+        <v>1256</v>
       </c>
       <c r="F224" s="13" t="s">
-        <v>1234</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A225" s="14" t="s">
-        <v>1178</v>
+        <v>1174</v>
       </c>
       <c r="B225" s="13" t="s">
-        <v>1179</v>
+        <v>1175</v>
       </c>
       <c r="C225" s="13" t="s">
-        <v>1261</v>
+        <v>1257</v>
       </c>
       <c r="D225" s="13" t="s">
-        <v>1355</v>
+        <v>1351</v>
       </c>
       <c r="E225" s="13" t="s">
-        <v>1261</v>
+        <v>1257</v>
       </c>
       <c r="F225" s="13" t="s">
-        <v>1235</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A226" s="14" t="s">
-        <v>1180</v>
+        <v>1176</v>
       </c>
       <c r="B226" s="13" t="s">
         <v>29</v>
@@ -9161,7 +9140,7 @@
         <v>304</v>
       </c>
       <c r="D226" s="13" t="s">
-        <v>1356</v>
+        <v>1352</v>
       </c>
       <c r="E226" s="13" t="s">
         <v>488</v>
@@ -9172,7 +9151,7 @@
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227" s="14" t="s">
-        <v>1181</v>
+        <v>1177</v>
       </c>
       <c r="B227" s="13" t="s">
         <v>31</v>
@@ -9187,52 +9166,52 @@
         <v>748</v>
       </c>
       <c r="F227" s="13" t="s">
-        <v>1236</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A228" s="14" t="s">
-        <v>1182</v>
+        <v>1178</v>
       </c>
       <c r="B228" s="13" t="s">
-        <v>1183</v>
+        <v>1179</v>
       </c>
       <c r="C228" s="13" t="s">
-        <v>1262</v>
+        <v>1258</v>
       </c>
       <c r="D228" s="13" t="s">
-        <v>1357</v>
+        <v>1353</v>
       </c>
       <c r="E228" s="13" t="s">
-        <v>1262</v>
+        <v>1258</v>
       </c>
       <c r="F228" s="13" t="s">
-        <v>1237</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A229" s="14" t="s">
-        <v>1184</v>
+        <v>1180</v>
       </c>
       <c r="B229" s="13" t="s">
-        <v>1185</v>
+        <v>1181</v>
       </c>
       <c r="C229" s="13" t="s">
-        <v>1283</v>
+        <v>1279</v>
       </c>
       <c r="D229" s="13" t="s">
-        <v>1358</v>
+        <v>1354</v>
       </c>
       <c r="E229" s="13" t="s">
-        <v>1263</v>
+        <v>1259</v>
       </c>
       <c r="F229" s="13" t="s">
-        <v>1238</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230" s="13" t="s">
-        <v>1186</v>
+        <v>1182</v>
       </c>
       <c r="B230" s="13" t="s">
         <v>40</v>
@@ -9252,7 +9231,7 @@
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A231" s="14" t="s">
-        <v>1187</v>
+        <v>1183</v>
       </c>
       <c r="B231" s="13" t="s">
         <v>41</v>
@@ -9272,16 +9251,16 @@
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A232" s="13" t="s">
-        <v>1188</v>
+        <v>1184</v>
       </c>
       <c r="B232" s="13" t="s">
         <v>42</v>
       </c>
       <c r="C232" s="13" t="s">
-        <v>1284</v>
+        <v>1280</v>
       </c>
       <c r="D232" s="13" t="s">
-        <v>1306</v>
+        <v>1302</v>
       </c>
       <c r="E232" s="13" t="s">
         <v>510</v>
@@ -9292,7 +9271,7 @@
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A233" s="13" t="s">
-        <v>1189</v>
+        <v>1185</v>
       </c>
       <c r="B233" s="13" t="s">
         <v>43</v>
@@ -9301,7 +9280,7 @@
         <v>782</v>
       </c>
       <c r="D233" s="13" t="s">
-        <v>1307</v>
+        <v>1303</v>
       </c>
       <c r="E233" s="13" t="s">
         <v>511</v>
@@ -9312,67 +9291,67 @@
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A234" s="13" t="s">
-        <v>1190</v>
+        <v>1186</v>
       </c>
       <c r="B234" s="13" t="s">
-        <v>1191</v>
+        <v>1187</v>
       </c>
       <c r="C234" s="16" t="s">
-        <v>1285</v>
+        <v>1281</v>
       </c>
       <c r="D234" s="13" t="s">
-        <v>1362</v>
+        <v>1358</v>
       </c>
       <c r="E234" s="16" t="s">
-        <v>1264</v>
+        <v>1260</v>
       </c>
       <c r="F234" s="13" t="s">
-        <v>1239</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A235" s="13" t="s">
-        <v>1192</v>
+        <v>1188</v>
       </c>
       <c r="B235" s="13" t="s">
-        <v>1193</v>
+        <v>1189</v>
       </c>
       <c r="C235" s="13" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="D235" s="13" t="s">
-        <v>1308</v>
+        <v>1304</v>
       </c>
       <c r="E235" s="13" t="s">
-        <v>1265</v>
+        <v>1261</v>
       </c>
       <c r="F235" s="13" t="s">
-        <v>1240</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A236" s="13" t="s">
-        <v>1194</v>
+        <v>1190</v>
       </c>
       <c r="B236" s="13" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="C236" s="13" t="s">
-        <v>1287</v>
+        <v>1283</v>
       </c>
       <c r="D236" s="13" t="s">
-        <v>1309</v>
+        <v>1305</v>
       </c>
       <c r="E236" s="13" t="s">
-        <v>1266</v>
+        <v>1262</v>
       </c>
       <c r="F236" s="13" t="s">
-        <v>1241</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A237" s="13" t="s">
-        <v>1196</v>
+        <v>1192</v>
       </c>
       <c r="B237" s="13" t="s">
         <v>32</v>
@@ -9381,250 +9360,250 @@
         <v>305</v>
       </c>
       <c r="D237" s="13" t="s">
-        <v>1310</v>
+        <v>1306</v>
       </c>
       <c r="E237" s="13" t="s">
         <v>305</v>
       </c>
       <c r="F237" s="13" t="s">
-        <v>1242</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A238" s="13" t="s">
-        <v>1197</v>
+        <v>1193</v>
       </c>
       <c r="B238" s="13" t="s">
-        <v>1198</v>
+        <v>1194</v>
       </c>
       <c r="C238" s="13" t="s">
-        <v>1288</v>
+        <v>1284</v>
       </c>
       <c r="D238" s="13" t="s">
-        <v>1311</v>
+        <v>1307</v>
       </c>
       <c r="E238" s="13" t="s">
         <v>489</v>
       </c>
       <c r="F238" s="13" t="s">
-        <v>1243</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A239" s="13" t="s">
-        <v>1199</v>
+        <v>1195</v>
       </c>
       <c r="B239" s="13" t="s">
-        <v>1200</v>
+        <v>1196</v>
       </c>
       <c r="C239" s="13" t="s">
         <v>505</v>
       </c>
       <c r="D239" s="13" t="s">
-        <v>1312</v>
+        <v>1308</v>
       </c>
       <c r="E239" s="13" t="s">
         <v>505</v>
       </c>
       <c r="F239" s="13" t="s">
-        <v>1244</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A240" s="13" t="s">
-        <v>1201</v>
+        <v>1197</v>
       </c>
       <c r="B240" s="13" t="s">
-        <v>1202</v>
+        <v>1198</v>
       </c>
       <c r="C240" s="13" t="s">
         <v>722</v>
       </c>
       <c r="D240" s="13" t="s">
-        <v>1313</v>
+        <v>1309</v>
       </c>
       <c r="E240" s="17" t="s">
         <v>749</v>
       </c>
       <c r="F240" s="13" t="s">
-        <v>1245</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A241" s="13" t="s">
-        <v>1203</v>
+        <v>1199</v>
       </c>
       <c r="B241" s="13" t="s">
-        <v>1204</v>
+        <v>1200</v>
       </c>
       <c r="C241" s="13" t="s">
         <v>306</v>
       </c>
       <c r="D241" s="13" t="s">
-        <v>1314</v>
+        <v>1310</v>
       </c>
       <c r="E241" s="13" t="s">
-        <v>1267</v>
+        <v>1263</v>
       </c>
       <c r="F241" s="13" t="s">
-        <v>1246</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A242" s="13" t="s">
-        <v>1205</v>
+        <v>1201</v>
       </c>
       <c r="B242" s="13" t="s">
-        <v>1363</v>
+        <v>1359</v>
       </c>
       <c r="C242" s="16" t="s">
-        <v>1364</v>
+        <v>1360</v>
       </c>
       <c r="D242" s="13" t="s">
-        <v>1365</v>
+        <v>1361</v>
       </c>
       <c r="E242" s="18" t="s">
-        <v>1371</v>
+        <v>1367</v>
       </c>
       <c r="F242" s="13" t="s">
-        <v>1366</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A243" s="13" t="s">
-        <v>1206</v>
+        <v>1202</v>
       </c>
       <c r="B243" s="13" t="s">
-        <v>1207</v>
+        <v>1203</v>
       </c>
       <c r="C243" s="13" t="s">
-        <v>1289</v>
+        <v>1285</v>
       </c>
       <c r="D243" s="13" t="s">
-        <v>1359</v>
+        <v>1355</v>
       </c>
       <c r="E243" s="13" t="s">
-        <v>1268</v>
+        <v>1264</v>
       </c>
       <c r="F243" s="13" t="s">
-        <v>1247</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A244" s="13" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
       <c r="B244" s="13" t="s">
-        <v>1209</v>
+        <v>1205</v>
       </c>
       <c r="C244" s="13" t="s">
-        <v>1290</v>
+        <v>1286</v>
       </c>
       <c r="D244" s="13" t="s">
-        <v>1315</v>
+        <v>1311</v>
       </c>
       <c r="E244" s="13" t="s">
-        <v>1269</v>
+        <v>1265</v>
       </c>
       <c r="F244" s="13" t="s">
-        <v>1248</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A245" s="13" t="s">
-        <v>1210</v>
+        <v>1206</v>
       </c>
       <c r="B245" s="13" t="s">
-        <v>1211</v>
+        <v>1207</v>
       </c>
       <c r="C245" s="13" t="s">
-        <v>1291</v>
+        <v>1287</v>
       </c>
       <c r="D245" s="13" t="s">
-        <v>1360</v>
+        <v>1356</v>
       </c>
       <c r="E245" s="13" t="s">
-        <v>1270</v>
+        <v>1266</v>
       </c>
       <c r="F245" s="13" t="s">
-        <v>1249</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A246" s="13" t="s">
-        <v>1212</v>
+        <v>1208</v>
       </c>
       <c r="B246" s="13" t="s">
-        <v>1213</v>
+        <v>1209</v>
       </c>
       <c r="C246" s="13" t="s">
-        <v>1292</v>
+        <v>1288</v>
       </c>
       <c r="D246" s="13" t="s">
-        <v>1316</v>
+        <v>1312</v>
       </c>
       <c r="E246" s="13" t="s">
-        <v>1271</v>
+        <v>1267</v>
       </c>
       <c r="F246" s="13" t="s">
-        <v>1250</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A247" s="13" t="s">
-        <v>1214</v>
+        <v>1210</v>
       </c>
       <c r="B247" s="13" t="s">
-        <v>1215</v>
+        <v>1211</v>
       </c>
       <c r="C247" s="13" t="s">
-        <v>1293</v>
+        <v>1289</v>
       </c>
       <c r="D247" s="13" t="s">
-        <v>1317</v>
+        <v>1313</v>
       </c>
       <c r="E247" s="13" t="s">
-        <v>1272</v>
+        <v>1268</v>
       </c>
       <c r="F247" s="13" t="s">
-        <v>1251</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A248" s="13" t="s">
-        <v>1216</v>
+        <v>1212</v>
       </c>
       <c r="B248" s="13" t="s">
-        <v>1217</v>
+        <v>1213</v>
       </c>
       <c r="C248" s="13" t="s">
-        <v>1294</v>
+        <v>1290</v>
       </c>
       <c r="D248" s="13" t="s">
-        <v>1318</v>
+        <v>1314</v>
       </c>
       <c r="E248" s="13" t="s">
-        <v>1273</v>
+        <v>1269</v>
       </c>
       <c r="F248" s="13" t="s">
-        <v>1252</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A249" s="13" t="s">
-        <v>1218</v>
+        <v>1214</v>
       </c>
       <c r="B249" s="13" t="s">
-        <v>1219</v>
+        <v>1215</v>
       </c>
       <c r="C249" s="13" t="s">
-        <v>1295</v>
+        <v>1291</v>
       </c>
       <c r="D249" s="13" t="s">
-        <v>1319</v>
+        <v>1315</v>
       </c>
       <c r="E249" s="17" t="s">
-        <v>1295</v>
+        <v>1291</v>
       </c>
       <c r="F249" s="13" t="s">
         <v>682</v>
@@ -9632,82 +9611,82 @@
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A250" s="13" t="s">
-        <v>1220</v>
+        <v>1216</v>
       </c>
       <c r="B250" s="13" t="s">
-        <v>1221</v>
+        <v>1217</v>
       </c>
       <c r="C250" s="17" t="s">
-        <v>1367</v>
+        <v>1363</v>
       </c>
       <c r="D250" s="13" t="s">
-        <v>1320</v>
+        <v>1316</v>
       </c>
       <c r="E250" s="17" t="s">
-        <v>1370</v>
+        <v>1366</v>
       </c>
       <c r="F250" s="13" t="s">
-        <v>1253</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A251" s="13" t="s">
-        <v>1222</v>
+        <v>1218</v>
       </c>
       <c r="B251" s="13" t="s">
-        <v>1223</v>
+        <v>1219</v>
       </c>
       <c r="C251" s="13" t="s">
-        <v>1296</v>
+        <v>1292</v>
       </c>
       <c r="D251" s="13" t="s">
-        <v>1321</v>
+        <v>1317</v>
       </c>
       <c r="E251" s="13" t="s">
-        <v>1274</v>
+        <v>1270</v>
       </c>
       <c r="F251" s="13" t="s">
-        <v>1254</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A252" s="13" t="s">
-        <v>1224</v>
+        <v>1220</v>
       </c>
       <c r="B252" s="13" t="s">
-        <v>1225</v>
+        <v>1221</v>
       </c>
       <c r="C252" s="13" t="s">
-        <v>1297</v>
+        <v>1293</v>
       </c>
       <c r="D252" s="13" t="s">
-        <v>1322</v>
+        <v>1318</v>
       </c>
       <c r="E252" s="13" t="s">
-        <v>1275</v>
+        <v>1271</v>
       </c>
       <c r="F252" s="13" t="s">
-        <v>1255</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A253" s="13" t="s">
-        <v>1226</v>
+        <v>1222</v>
       </c>
       <c r="B253" s="13" t="s">
-        <v>1227</v>
+        <v>1223</v>
       </c>
       <c r="C253" s="13" t="s">
-        <v>1298</v>
+        <v>1294</v>
       </c>
       <c r="D253" s="13" t="s">
-        <v>1323</v>
+        <v>1319</v>
       </c>
       <c r="E253" s="13" t="s">
-        <v>1276</v>
+        <v>1272</v>
       </c>
       <c r="F253" s="13" t="s">
-        <v>1256</v>
+        <v>1252</v>
       </c>
     </row>
   </sheetData>
@@ -9717,6 +9696,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="6e0cf07b-8188-4b76-8f54-3cda03d37414" xsi:nil="true"/>
@@ -9725,15 +9713,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9966,6 +9945,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04FEE910-FEC8-48C6-9CF9-BF01BA5AD6FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E20926E-9EFB-4B7E-90D4-905B08F8E59C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -9978,14 +9965,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="43e153a8-5ef1-4f65-aac7-dc4685f18eaa"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04FEE910-FEC8-48C6-9CF9-BF01BA5AD6FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added distance to locations for the collection page
</commit_message>
<xml_diff>
--- a/translations/translations.xlsx
+++ b/translations/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rmitchell64/Desktop/Projects/GPSSample/gpssample/translations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A5C467-7A4B-0246-BFBD-EA9A0054D000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D631377-9091-554C-B97D-73EE0C88C8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="760" windowWidth="31560" windowHeight="19980" xr2:uid="{C8C8ACD1-4E76-7942-B525-8D880B4ECA80}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2232" uniqueCount="2065">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2240" uniqueCount="2073">
   <si>
     <t>Settings</t>
   </si>
@@ -6271,6 +6271,30 @@
   </si>
   <si>
     <t>Surveyed</t>
+  </si>
+  <si>
+    <t>meters</t>
+  </si>
+  <si>
+    <t>Meters</t>
+  </si>
+  <si>
+    <t>feet</t>
+  </si>
+  <si>
+    <t>Feet</t>
+  </si>
+  <si>
+    <t>kilometers</t>
+  </si>
+  <si>
+    <t>Kilometers</t>
+  </si>
+  <si>
+    <t>miles</t>
+  </si>
+  <si>
+    <t>Miles</t>
   </si>
 </sst>
 </file>
@@ -6518,8 +6542,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73295AEA-8140-4EAB-A7A6-7D1875F4D7E7}" name="Table1" displayName="Table1" ref="A1:F376" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:F376" xr:uid="{73295AEA-8140-4EAB-A7A6-7D1875F4D7E7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73295AEA-8140-4EAB-A7A6-7D1875F4D7E7}" name="Table1" displayName="Table1" ref="A1:F380" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:F380" xr:uid="{73295AEA-8140-4EAB-A7A6-7D1875F4D7E7}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{DE67F62A-9DCA-4DFE-8C98-83B024E5D946}" name="app_name" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{BCDA3AB5-7BB5-4A21-ABBB-4186B52D559D}" name="GPSSample::en" dataDxfId="0"/>
@@ -6838,10 +6862,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD3E6CC-854C-5841-9577-D3ADD2982DB6}">
-  <dimension ref="A1:F376"/>
+  <dimension ref="A1:F380"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A357" zoomScale="129" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B377" sqref="B377"/>
+      <selection activeCell="B383" sqref="B383"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -14304,6 +14328,38 @@
         <v>2064</v>
       </c>
     </row>
+    <row r="377" spans="1:6">
+      <c r="A377" s="19" t="s">
+        <v>2065</v>
+      </c>
+      <c r="B377" s="15" t="s">
+        <v>2066</v>
+      </c>
+    </row>
+    <row r="378" spans="1:6">
+      <c r="A378" s="19" t="s">
+        <v>2067</v>
+      </c>
+      <c r="B378" s="15" t="s">
+        <v>2068</v>
+      </c>
+    </row>
+    <row r="379" spans="1:6">
+      <c r="A379" s="19" t="s">
+        <v>2069</v>
+      </c>
+      <c r="B379" s="15" t="s">
+        <v>2070</v>
+      </c>
+    </row>
+    <row r="380" spans="1:6">
+      <c r="A380" s="19" t="s">
+        <v>2071</v>
+      </c>
+      <c r="B380" s="15" t="s">
+        <v>2072</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -14315,26 +14371,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="6e0cf07b-8188-4b76-8f54-3cda03d37414" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="43e153a8-5ef1-4f65-aac7-dc4685f18eaa">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F12BE0DB4A3DF641BF113FBF1C7EA261" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c5ed1bf660206bfdbe82102ebcc97d59">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="43e153a8-5ef1-4f65-aac7-dc4685f18eaa" xmlns:ns3="6e0cf07b-8188-4b76-8f54-3cda03d37414" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="72d80d06cf93fc3b44b310d898ba9e05" ns2:_="" ns3:_="">
     <xsd:import namespace="43e153a8-5ef1-4f65-aac7-dc4685f18eaa"/>
@@ -14569,32 +14605,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E20926E-9EFB-4B7E-90D4-905B08F8E59C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="43e153a8-5ef1-4f65-aac7-dc4685f18eaa"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="6e0cf07b-8188-4b76-8f54-3cda03d37414"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04FEE910-FEC8-48C6-9CF9-BF01BA5AD6FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="6e0cf07b-8188-4b76-8f54-3cda03d37414" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="43e153a8-5ef1-4f65-aac7-dc4685f18eaa">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29F0871A-7C24-4792-85DD-9F311CBC7318}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14611,4 +14642,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04FEE910-FEC8-48C6-9CF9-BF01BA5AD6FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E20926E-9EFB-4B7E-90D4-905B08F8E59C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="43e153a8-5ef1-4f65-aac7-dc4685f18eaa"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="6e0cf07b-8188-4b76-8f54-3cda03d37414"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Reduced image size and added warning when you've reached 25Mb of image data.
</commit_message>
<xml_diff>
--- a/translations/translations.xlsx
+++ b/translations/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rmitchell64/Desktop/Projects/GPSSample/gpssample/translations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DF9571-E576-5548-8BFA-1AC34F54E8F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75010B81-DFE7-CD40-BB45-C79C4110FB18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28660" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{C8C8ACD1-4E76-7942-B525-8D880B4ECA80}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="31720" windowHeight="19700" xr2:uid="{C8C8ACD1-4E76-7942-B525-8D880B4ECA80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2640" uniqueCount="2442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2650" uniqueCount="2452">
   <si>
     <t>app_name</t>
   </si>
@@ -7402,6 +7402,36 @@
   </si>
   <si>
     <t>There are no eligible households to sample.</t>
+  </si>
+  <si>
+    <t>walk_enumeration_area</t>
+  </si>
+  <si>
+    <t>mark_current_location</t>
+  </si>
+  <si>
+    <t>delete_last_location</t>
+  </si>
+  <si>
+    <t>clear_map_and_start_over</t>
+  </si>
+  <si>
+    <t>image_size_warning</t>
+  </si>
+  <si>
+    <t>Clear Map and Start Over</t>
+  </si>
+  <si>
+    <t>Delete Last Location</t>
+  </si>
+  <si>
+    <t>Walk Enumeration Area</t>
+  </si>
+  <si>
+    <t>Mark Current Location</t>
+  </si>
+  <si>
+    <t>You've exceeded 25Mb of Image Data. Adding more images will greatly impact data transfer performance.</t>
   </si>
 </sst>
 </file>
@@ -7571,7 +7601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7601,10 +7631,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7706,8 +7735,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73295AEA-8140-4EAB-A7A6-7D1875F4D7E7}" name="Table1" displayName="Table1" ref="A1:G380" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:G380" xr:uid="{73295AEA-8140-4EAB-A7A6-7D1875F4D7E7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73295AEA-8140-4EAB-A7A6-7D1875F4D7E7}" name="Table1" displayName="Table1" ref="A1:G385" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:G385" xr:uid="{73295AEA-8140-4EAB-A7A6-7D1875F4D7E7}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{DE67F62A-9DCA-4DFE-8C98-83B024E5D946}" name="app_name" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{BCDA3AB5-7BB5-4A21-ABBB-4186B52D559D}" name="GPSSample::en" dataDxfId="1"/>
@@ -8027,10 +8056,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD3E6CC-854C-5841-9577-D3ADD2982DB6}">
-  <dimension ref="A1:G380"/>
+  <dimension ref="A1:G385"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A357" zoomScale="129" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B380" sqref="B380"/>
+    <sheetView tabSelected="1" topLeftCell="A356" zoomScale="129" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B384" sqref="B384"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -16694,56 +16723,105 @@
       </c>
     </row>
     <row r="377" spans="1:7">
-      <c r="A377" s="23" t="s">
+      <c r="A377" s="18" t="s">
         <v>2434</v>
       </c>
-      <c r="B377" s="24" t="s">
+      <c r="B377" s="14" t="s">
         <v>2438</v>
       </c>
-      <c r="C377" s="25"/>
-      <c r="D377" s="25"/>
-      <c r="E377" s="25"/>
-      <c r="F377" s="25"/>
-      <c r="G377" s="26"/>
+      <c r="G377" s="23"/>
     </row>
     <row r="378" spans="1:7">
-      <c r="A378" s="23" t="s">
+      <c r="A378" s="18" t="s">
         <v>2435</v>
       </c>
-      <c r="B378" s="24" t="s">
+      <c r="B378" s="14" t="s">
         <v>2439</v>
       </c>
-      <c r="C378" s="25"/>
-      <c r="D378" s="25"/>
-      <c r="E378" s="25"/>
-      <c r="F378" s="25"/>
-      <c r="G378" s="26"/>
+      <c r="G378" s="23"/>
     </row>
     <row r="379" spans="1:7">
-      <c r="A379" s="23" t="s">
+      <c r="A379" s="18" t="s">
         <v>2436</v>
       </c>
-      <c r="B379" s="24" t="s">
+      <c r="B379" s="14" t="s">
         <v>2440</v>
       </c>
-      <c r="C379" s="25"/>
-      <c r="D379" s="25"/>
-      <c r="E379" s="25"/>
-      <c r="F379" s="25"/>
-      <c r="G379" s="26"/>
+      <c r="G379" s="23"/>
     </row>
     <row r="380" spans="1:7">
-      <c r="A380" s="23" t="s">
+      <c r="A380" s="18" t="s">
         <v>2437</v>
       </c>
       <c r="B380" s="14" t="s">
         <v>2441</v>
       </c>
-      <c r="C380" s="25"/>
-      <c r="D380" s="25"/>
-      <c r="E380" s="25"/>
-      <c r="F380" s="25"/>
-      <c r="G380" s="26"/>
+      <c r="G380" s="23"/>
+    </row>
+    <row r="381" spans="1:7">
+      <c r="A381" s="24" t="s">
+        <v>2442</v>
+      </c>
+      <c r="B381" s="14" t="s">
+        <v>2449</v>
+      </c>
+      <c r="C381" s="25"/>
+      <c r="D381" s="25"/>
+      <c r="E381" s="25"/>
+      <c r="F381" s="25"/>
+      <c r="G381" s="23"/>
+    </row>
+    <row r="382" spans="1:7">
+      <c r="A382" s="24" t="s">
+        <v>2443</v>
+      </c>
+      <c r="B382" s="14" t="s">
+        <v>2450</v>
+      </c>
+      <c r="C382" s="25"/>
+      <c r="D382" s="25"/>
+      <c r="E382" s="25"/>
+      <c r="F382" s="25"/>
+      <c r="G382" s="23"/>
+    </row>
+    <row r="383" spans="1:7">
+      <c r="A383" s="24" t="s">
+        <v>2444</v>
+      </c>
+      <c r="B383" s="14" t="s">
+        <v>2448</v>
+      </c>
+      <c r="C383" s="25"/>
+      <c r="D383" s="25"/>
+      <c r="E383" s="25"/>
+      <c r="F383" s="25"/>
+      <c r="G383" s="23"/>
+    </row>
+    <row r="384" spans="1:7">
+      <c r="A384" s="24" t="s">
+        <v>2445</v>
+      </c>
+      <c r="B384" s="14" t="s">
+        <v>2447</v>
+      </c>
+      <c r="C384" s="25"/>
+      <c r="D384" s="25"/>
+      <c r="E384" s="25"/>
+      <c r="F384" s="25"/>
+      <c r="G384" s="23"/>
+    </row>
+    <row r="385" spans="1:7">
+      <c r="A385" s="24" t="s">
+        <v>2446</v>
+      </c>
+      <c r="B385" s="14" t="s">
+        <v>2451</v>
+      </c>
+      <c r="C385" s="25"/>
+      <c r="D385" s="25"/>
+      <c r="E385" s="25"/>
+      <c r="F385" s="25"/>
+      <c r="G385" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16756,26 +16834,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="6e0cf07b-8188-4b76-8f54-3cda03d37414" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="43e153a8-5ef1-4f65-aac7-dc4685f18eaa">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F12BE0DB4A3DF641BF113FBF1C7EA261" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c5ed1bf660206bfdbe82102ebcc97d59">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="43e153a8-5ef1-4f65-aac7-dc4685f18eaa" xmlns:ns3="6e0cf07b-8188-4b76-8f54-3cda03d37414" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="72d80d06cf93fc3b44b310d898ba9e05" ns2:_="" ns3:_="">
     <xsd:import namespace="43e153a8-5ef1-4f65-aac7-dc4685f18eaa"/>
@@ -17010,10 +17068,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="6e0cf07b-8188-4b76-8f54-3cda03d37414" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="43e153a8-5ef1-4f65-aac7-dc4685f18eaa">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04FEE910-FEC8-48C6-9CF9-BF01BA5AD6FE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29F0871A-7C24-4792-85DD-9F311CBC7318}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="43e153a8-5ef1-4f65-aac7-dc4685f18eaa"/>
+    <ds:schemaRef ds:uri="6e0cf07b-8188-4b76-8f54-3cda03d37414"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -17036,20 +17125,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29F0871A-7C24-4792-85DD-9F311CBC7318}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04FEE910-FEC8-48C6-9CF9-BF01BA5AD6FE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="43e153a8-5ef1-4f65-aac7-dc4685f18eaa"/>
-    <ds:schemaRef ds:uri="6e0cf07b-8188-4b76-8f54-3cda03d37414"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Re-added cap to save file to the default location
</commit_message>
<xml_diff>
--- a/translations/translations.xlsx
+++ b/translations/translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cdc.sharepoint.com/teams/CGH-GPSSample/Shared Documents/General/2024/APP- strings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rmitchell64/Desktop/Projects/GPSSample/gpssample/translations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{13EBA67D-FF34-4833-87A5-07FC53546B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2447125E-CEA7-43F1-BB80-E204AD38D004}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D129AD0E-82F0-CC49-BCD0-8598E73D5436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{C8C8ACD1-4E76-7942-B525-8D880B4ECA80}"/>
+    <workbookView xWindow="22260" yWindow="11360" windowWidth="29040" windowHeight="15220" xr2:uid="{C8C8ACD1-4E76-7942-B525-8D880B4ECA80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2737" uniqueCount="2538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2747" uniqueCount="2548">
   <si>
     <t>app_name</t>
   </si>
@@ -7690,6 +7690,36 @@
   </si>
   <si>
     <t>Définir les limites (l x l)</t>
+  </si>
+  <si>
+    <t>config_saved</t>
+  </si>
+  <si>
+    <t>Review All Teams</t>
+  </si>
+  <si>
+    <t>review_all_teams</t>
+  </si>
+  <si>
+    <t>Configuration has been saved.</t>
+  </si>
+  <si>
+    <t>select_file_location</t>
+  </si>
+  <si>
+    <t>Select the file location</t>
+  </si>
+  <si>
+    <t>default_location</t>
+  </si>
+  <si>
+    <t>Default location</t>
+  </si>
+  <si>
+    <t>let_me_choose</t>
+  </si>
+  <si>
+    <t>Let me choose</t>
   </si>
 </sst>
 </file>
@@ -7838,7 +7868,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -7859,11 +7889,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7893,13 +7934,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8001,8 +8043,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73295AEA-8140-4EAB-A7A6-7D1875F4D7E7}" name="Table1" displayName="Table1" ref="A1:G391" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:G391" xr:uid="{73295AEA-8140-4EAB-A7A6-7D1875F4D7E7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73295AEA-8140-4EAB-A7A6-7D1875F4D7E7}" name="Table1" displayName="Table1" ref="A1:G396" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:G396" xr:uid="{73295AEA-8140-4EAB-A7A6-7D1875F4D7E7}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{DE67F62A-9DCA-4DFE-8C98-83B024E5D946}" name="app_name" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{BCDA3AB5-7BB5-4A21-ABBB-4186B52D559D}" name="GPSSample::en" dataDxfId="1"/>
@@ -8017,9 +8059,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -8057,7 +8099,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -8163,7 +8205,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -8305,7 +8347,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8322,22 +8364,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD3E6CC-854C-5841-9577-D3ADD2982DB6}">
-  <dimension ref="A1:G391"/>
+  <dimension ref="A1:G396"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A369" zoomScale="129" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A388" sqref="A388"/>
+    <sheetView tabSelected="1" topLeftCell="A380" zoomScale="129" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B396" sqref="B396"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="40.5" customWidth="1"/>
-    <col min="2" max="2" width="43.375" customWidth="1"/>
-    <col min="3" max="3" width="74.375" customWidth="1"/>
+    <col min="2" max="2" width="43.33203125" customWidth="1"/>
+    <col min="3" max="3" width="74.33203125" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
     <col min="5" max="5" width="41" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.625" customWidth="1"/>
-    <col min="7" max="7" width="42.625" customWidth="1"/>
-    <col min="8" max="8" width="44.875" customWidth="1"/>
+    <col min="6" max="6" width="54.6640625" customWidth="1"/>
+    <col min="7" max="7" width="42.6640625" customWidth="1"/>
+    <col min="8" max="8" width="44.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -9394,7 +9436,7 @@
       <c r="F46" t="s">
         <v>287</v>
       </c>
-      <c r="G46" s="27" t="s">
+      <c r="G46" s="24" t="s">
         <v>2514</v>
       </c>
     </row>
@@ -9865,7 +9907,7 @@
       <c r="B67" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="C67" s="26" t="s">
+      <c r="C67" s="23" t="s">
         <v>425</v>
       </c>
       <c r="D67" t="s">
@@ -17214,7 +17256,7 @@
       <c r="F386" t="s">
         <v>2500</v>
       </c>
-      <c r="G386" s="28" t="s">
+      <c r="G386" s="25" t="s">
         <v>2515</v>
       </c>
     </row>
@@ -17237,7 +17279,7 @@
       <c r="F387" t="s">
         <v>2506</v>
       </c>
-      <c r="G387" s="28" t="s">
+      <c r="G387" s="25" t="s">
         <v>2516</v>
       </c>
     </row>
@@ -17260,7 +17302,7 @@
       <c r="F388" t="s">
         <v>2532</v>
       </c>
-      <c r="G388" s="27" t="s">
+      <c r="G388" s="24" t="s">
         <v>2534</v>
       </c>
     </row>
@@ -17283,55 +17325,120 @@
       <c r="F389" t="s">
         <v>2531</v>
       </c>
-      <c r="G389" s="27" t="s">
+      <c r="G389" s="24" t="s">
         <v>2533</v>
       </c>
     </row>
     <row r="390" spans="1:7">
-      <c r="A390" s="23" t="s">
+      <c r="A390" s="18" t="s">
         <v>2508</v>
       </c>
-      <c r="B390" s="24" t="s">
+      <c r="B390" s="14" t="s">
         <v>2509</v>
       </c>
-      <c r="C390" s="25" t="s">
+      <c r="C390" t="s">
         <v>2510</v>
       </c>
-      <c r="D390" s="25" t="s">
+      <c r="D390" t="s">
         <v>2511</v>
       </c>
-      <c r="E390" s="25" t="s">
+      <c r="E390" t="s">
         <v>2513</v>
       </c>
-      <c r="F390" s="25" t="s">
+      <c r="F390" t="s">
         <v>2512</v>
       </c>
-      <c r="G390" s="28" t="s">
+      <c r="G390" s="25" t="s">
         <v>2517</v>
       </c>
     </row>
     <row r="391" spans="1:7">
-      <c r="A391" s="23" t="s">
+      <c r="A391" s="18" t="s">
         <v>2518</v>
       </c>
-      <c r="B391" s="24" t="s">
+      <c r="B391" s="14" t="s">
         <v>2519</v>
       </c>
-      <c r="C391" s="25" t="s">
+      <c r="C391" t="s">
         <v>2521</v>
       </c>
-      <c r="D391" s="25" t="s">
+      <c r="D391" t="s">
         <v>2520</v>
       </c>
-      <c r="E391" s="25" t="s">
+      <c r="E391" t="s">
         <v>2522</v>
       </c>
-      <c r="F391" s="25" t="s">
+      <c r="F391" t="s">
         <v>2523</v>
       </c>
-      <c r="G391" s="29" t="s">
+      <c r="G391" s="26" t="s">
         <v>2524</v>
       </c>
+    </row>
+    <row r="392" spans="1:7">
+      <c r="A392" s="27" t="s">
+        <v>2540</v>
+      </c>
+      <c r="B392" s="28" t="s">
+        <v>2539</v>
+      </c>
+      <c r="C392" s="29"/>
+      <c r="D392" s="29"/>
+      <c r="E392" s="29"/>
+      <c r="F392" s="29"/>
+      <c r="G392" s="30"/>
+    </row>
+    <row r="393" spans="1:7">
+      <c r="A393" s="27" t="s">
+        <v>2538</v>
+      </c>
+      <c r="B393" s="28" t="s">
+        <v>2541</v>
+      </c>
+      <c r="C393" s="29"/>
+      <c r="D393" s="29"/>
+      <c r="E393" s="29"/>
+      <c r="F393" s="29"/>
+      <c r="G393" s="30"/>
+    </row>
+    <row r="394" spans="1:7">
+      <c r="A394" s="27" t="s">
+        <v>2542</v>
+      </c>
+      <c r="B394" s="28" t="s">
+        <v>2543</v>
+      </c>
+      <c r="C394" s="29"/>
+      <c r="D394" s="29"/>
+      <c r="E394" s="29"/>
+      <c r="F394" s="29"/>
+      <c r="G394" s="30"/>
+    </row>
+    <row r="395" spans="1:7">
+      <c r="A395" s="27" t="s">
+        <v>2544</v>
+      </c>
+      <c r="B395" s="28" t="s">
+        <v>2545</v>
+      </c>
+      <c r="C395" s="29"/>
+      <c r="D395" s="29"/>
+      <c r="E395" s="29"/>
+      <c r="F395" s="29"/>
+      <c r="G395" s="30"/>
+    </row>
+    <row r="396" spans="1:7">
+      <c r="A396" s="27" t="s">
+        <v>2546</v>
+      </c>
+      <c r="B396" s="28" t="s">
+        <v>2547</v>
+      </c>
+      <c r="C396" s="29"/>
+      <c r="D396" s="29"/>
+      <c r="E396" s="29"/>
+      <c r="F396" s="29"/>
+      <c r="G396" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17344,6 +17451,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="6e0cf07b-8188-4b76-8f54-3cda03d37414" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="43e153a8-5ef1-4f65-aac7-dc4685f18eaa">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F12BE0DB4A3DF641BF113FBF1C7EA261" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c5ed1bf660206bfdbe82102ebcc97d59">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="43e153a8-5ef1-4f65-aac7-dc4685f18eaa" xmlns:ns3="6e0cf07b-8188-4b76-8f54-3cda03d37414" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="72d80d06cf93fc3b44b310d898ba9e05" ns2:_="" ns3:_="">
     <xsd:import namespace="43e153a8-5ef1-4f65-aac7-dc4685f18eaa"/>
@@ -17578,41 +17705,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="6e0cf07b-8188-4b76-8f54-3cda03d37414" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="43e153a8-5ef1-4f65-aac7-dc4685f18eaa">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29F0871A-7C24-4792-85DD-9F311CBC7318}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04FEE910-FEC8-48C6-9CF9-BF01BA5AD6FE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="43e153a8-5ef1-4f65-aac7-dc4685f18eaa"/>
-    <ds:schemaRef ds:uri="6e0cf07b-8188-4b76-8f54-3cda03d37414"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -17635,9 +17731,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04FEE910-FEC8-48C6-9CF9-BF01BA5AD6FE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29F0871A-7C24-4792-85DD-9F311CBC7318}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="43e153a8-5ef1-4f65-aac7-dc4685f18eaa"/>
+    <ds:schemaRef ds:uri="6e0cf07b-8188-4b76-8f54-3cda03d37414"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added translations for the date formats
</commit_message>
<xml_diff>
--- a/translations/translations.xlsx
+++ b/translations/translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cdc.sharepoint.com/teams/CGH-GPSSample/Shared Documents/General/2024/APP- strings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rmitchell64/Desktop/Projects/GPSSample/gpssample/translations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{4A214CEA-7D15-754E-A5F2-8E85970F5976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8598EF4E-AD3F-49E9-868F-347DA566BCBC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF3C6BD-BCD5-B44C-B9F1-50E0AC9390D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{C8C8ACD1-4E76-7942-B525-8D880B4ECA80}"/>
+    <workbookView xWindow="5520" yWindow="760" windowWidth="29040" windowHeight="15220" xr2:uid="{C8C8ACD1-4E76-7942-B525-8D880B4ECA80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2779" uniqueCount="2580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2789" uniqueCount="2588">
   <si>
     <t>app_name</t>
   </si>
@@ -7816,6 +7816,30 @@
   </si>
   <si>
     <t>Batas Wilayah Pencacahan ini berpotongan dengan sendirinya. Apakah Anda ingin memperbaiki batasnya?</t>
+  </si>
+  <si>
+    <t>select_the_property_identifier</t>
+  </si>
+  <si>
+    <t>Please select the property identifier that identifies the cluster name</t>
+  </si>
+  <si>
+    <t>select_the_hh_identifiers</t>
+  </si>
+  <si>
+    <t>Please select the HH identifiers to import</t>
+  </si>
+  <si>
+    <t>date_formats</t>
+  </si>
+  <si>
+    <t>dd/mm/yyyy</t>
+  </si>
+  <si>
+    <t>mm/dd/yyyy</t>
+  </si>
+  <si>
+    <t>yyyy/mm/dd</t>
   </si>
 </sst>
 </file>
@@ -7995,7 +8019,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -8028,9 +8052,10 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8132,8 +8157,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73295AEA-8140-4EAB-A7A6-7D1875F4D7E7}" name="Table1" displayName="Table1" ref="A1:G397" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:G397" xr:uid="{73295AEA-8140-4EAB-A7A6-7D1875F4D7E7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73295AEA-8140-4EAB-A7A6-7D1875F4D7E7}" name="Table1" displayName="Table1" ref="A1:G402" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:G402" xr:uid="{73295AEA-8140-4EAB-A7A6-7D1875F4D7E7}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{DE67F62A-9DCA-4DFE-8C98-83B024E5D946}" name="app_name" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{BCDA3AB5-7BB5-4A21-ABBB-4186B52D559D}" name="GPSSample::en" dataDxfId="1"/>
@@ -8148,9 +8173,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -8188,7 +8213,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -8294,7 +8319,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -8436,7 +8461,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8453,22 +8478,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD3E6CC-854C-5841-9577-D3ADD2982DB6}">
-  <dimension ref="A1:G397"/>
+  <dimension ref="A1:G402"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E374" zoomScale="129" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H392" sqref="H392"/>
+    <sheetView tabSelected="1" topLeftCell="A384" zoomScale="129" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B404" sqref="B404"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="40.5" customWidth="1"/>
-    <col min="2" max="2" width="43.375" customWidth="1"/>
-    <col min="3" max="3" width="74.375" customWidth="1"/>
+    <col min="2" max="2" width="54.5" customWidth="1"/>
+    <col min="3" max="3" width="74.33203125" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
     <col min="5" max="5" width="41" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.625" customWidth="1"/>
-    <col min="7" max="7" width="42.625" customWidth="1"/>
-    <col min="8" max="8" width="44.875" customWidth="1"/>
+    <col min="6" max="6" width="54.6640625" customWidth="1"/>
+    <col min="7" max="7" width="42.6640625" customWidth="1"/>
+    <col min="8" max="8" width="44.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -17580,27 +17605,92 @@
       </c>
     </row>
     <row r="397" spans="1:7">
-      <c r="A397" s="26" t="s">
+      <c r="A397" s="18" t="s">
         <v>2573</v>
       </c>
       <c r="B397" s="14" t="s">
         <v>2574</v>
       </c>
-      <c r="C397" s="27" t="s">
+      <c r="C397" t="s">
         <v>2575</v>
       </c>
-      <c r="D397" s="27" t="s">
+      <c r="D397" t="s">
         <v>2578</v>
       </c>
-      <c r="E397" s="27" t="s">
+      <c r="E397" t="s">
         <v>2577</v>
       </c>
-      <c r="F397" s="27" t="s">
+      <c r="F397" t="s">
         <v>2576</v>
       </c>
-      <c r="G397" s="28" t="s">
+      <c r="G397" s="26" t="s">
         <v>2579</v>
       </c>
+    </row>
+    <row r="398" spans="1:7">
+      <c r="A398" s="27" t="s">
+        <v>2580</v>
+      </c>
+      <c r="B398" s="14" t="s">
+        <v>2581</v>
+      </c>
+      <c r="C398" s="29"/>
+      <c r="D398" s="29"/>
+      <c r="E398" s="29"/>
+      <c r="F398" s="29"/>
+      <c r="G398" s="26"/>
+    </row>
+    <row r="399" spans="1:7">
+      <c r="A399" s="27" t="s">
+        <v>2582</v>
+      </c>
+      <c r="B399" s="14" t="s">
+        <v>2583</v>
+      </c>
+      <c r="C399" s="29"/>
+      <c r="D399" s="29"/>
+      <c r="E399" s="29"/>
+      <c r="F399" s="29"/>
+      <c r="G399" s="26"/>
+    </row>
+    <row r="400" spans="1:7">
+      <c r="A400" s="27" t="s">
+        <v>2584</v>
+      </c>
+      <c r="B400" s="28" t="s">
+        <v>2585</v>
+      </c>
+      <c r="C400" s="29"/>
+      <c r="D400" s="29"/>
+      <c r="E400" s="29"/>
+      <c r="F400" s="29"/>
+      <c r="G400" s="26"/>
+    </row>
+    <row r="401" spans="1:7">
+      <c r="A401" s="27" t="s">
+        <v>2584</v>
+      </c>
+      <c r="B401" s="28" t="s">
+        <v>2586</v>
+      </c>
+      <c r="C401" s="29"/>
+      <c r="D401" s="29"/>
+      <c r="E401" s="29"/>
+      <c r="F401" s="29"/>
+      <c r="G401" s="26"/>
+    </row>
+    <row r="402" spans="1:7">
+      <c r="A402" s="27" t="s">
+        <v>2584</v>
+      </c>
+      <c r="B402" s="28" t="s">
+        <v>2587</v>
+      </c>
+      <c r="C402" s="29"/>
+      <c r="D402" s="29"/>
+      <c r="E402" s="29"/>
+      <c r="F402" s="29"/>
+      <c r="G402" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17613,6 +17703,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="6e0cf07b-8188-4b76-8f54-3cda03d37414" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="43e153a8-5ef1-4f65-aac7-dc4685f18eaa">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F12BE0DB4A3DF641BF113FBF1C7EA261" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c5ed1bf660206bfdbe82102ebcc97d59">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="43e153a8-5ef1-4f65-aac7-dc4685f18eaa" xmlns:ns3="6e0cf07b-8188-4b76-8f54-3cda03d37414" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="72d80d06cf93fc3b44b310d898ba9e05" ns2:_="" ns3:_="">
     <xsd:import namespace="43e153a8-5ef1-4f65-aac7-dc4685f18eaa"/>
@@ -17847,17 +17948,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="6e0cf07b-8188-4b76-8f54-3cda03d37414" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="43e153a8-5ef1-4f65-aac7-dc4685f18eaa">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -17868,6 +17958,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E20926E-9EFB-4B7E-90D4-905B08F8E59C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6e0cf07b-8188-4b76-8f54-3cda03d37414"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="43e153a8-5ef1-4f65-aac7-dc4685f18eaa"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29F0871A-7C24-4792-85DD-9F311CBC7318}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17886,23 +17993,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E20926E-9EFB-4B7E-90D4-905B08F8E59C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6e0cf07b-8188-4b76-8f54-3cda03d37414"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="43e153a8-5ef1-4f65-aac7-dc4685f18eaa"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04FEE910-FEC8-48C6-9CF9-BF01BA5AD6FE}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
convert numberValue to Long instead of Int
</commit_message>
<xml_diff>
--- a/translations/translations.xlsx
+++ b/translations/translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cdc.sharepoint.com/teams/CGH-GPSSample/Shared Documents/General/2025/App - Strings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/russell/Projects/GPS-Sample/translations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{8D90111F-CF0E-E24F-9ECC-CB0B4854A2C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66CC3ADC-2325-485D-B050-96E824244CB3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3901BC-0D9F-DB49-A316-83C1DC176C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C8C8ACD1-4E76-7942-B525-8D880B4ECA80}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="27560" windowHeight="13700" xr2:uid="{C8C8ACD1-4E76-7942-B525-8D880B4ECA80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3672" uniqueCount="3379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3696" uniqueCount="3403">
   <si>
     <t>app_name</t>
   </si>
@@ -10222,6 +10222,78 @@
   </si>
   <si>
     <t>Listahan Lamang</t>
+  </si>
+  <si>
+    <t>Not Now → skips permission (feature won’t work)</t>
+  </si>
+  <si>
+    <t>Enable Background Location → triggers Android system permission for “Allow all the time”</t>
+  </si>
+  <si>
+    <t>Ahora no → omite el permiso (la función no funcionará)</t>
+  </si>
+  <si>
+    <t>Habilitar ubicación en segundo plano → activa el permiso del sistema Android para «Permitir siempre»</t>
+  </si>
+  <si>
+    <t>Pas maintenant → ignore l'autorisation (la fonctionnalité ne fonctionnera pas)</t>
+  </si>
+  <si>
+    <t>Activer la localisation en arrière-plan → déclenche l'autorisation du système Android pour « Autoriser tout le temps »</t>
+  </si>
+  <si>
+    <t>Agora não → ignora a permissão (o recurso não funcionará)</t>
+  </si>
+  <si>
+    <t>Ativar localização em segundo plano → aciona a permissão do sistema Android para «Permitir sempre»</t>
+  </si>
+  <si>
+    <t>Не сейчас → пропускает запрос разрешения (функция не будет работать)</t>
+  </si>
+  <si>
+    <t>Включить фоновое определение местоположения → запускает запрос разрешения системы Android «Разрешить всегда»</t>
+  </si>
+  <si>
+    <t>Nanti Saja → melewati izin (fitur tidak akan berfungsi)</t>
+  </si>
+  <si>
+    <t>Aktifkan Lokasi Latar Belakang → memicu izin sistem Android untuk "Izinkan setiap saat"</t>
+  </si>
+  <si>
+    <t>Hindi Ngayon → nilalaktawan ang pahintulot (hindi gagana ang feature)</t>
+  </si>
+  <si>
+    <t>Paganahin ang Lokasyon sa Background → tini-trigger ang pahintulot ng Android system para sa “Payagan sa lahat ng oras”</t>
+  </si>
+  <si>
+    <t>GPSSample records your location in the background while you move between households. This allows the app to track your route (breadcrumb trail), map household locations, and navigate back to selected survey sites. Your location is stored securely on your device and may be exported only if you choose to do so. You can revoke background location access at any time in Android Settings.</t>
+  </si>
+  <si>
+    <t>GPSSample registra su ubicación en segundo plano mientras se desplaza entre hogares. Esto permite a la aplicación realizar un seguimiento de su ruta (rastro de migas de pan), trazar un mapa con la ubicación de los hogares y navegar de vuelta a los lugares seleccionados para la encuesta. Su ubicación se almacena de forma segura en su dispositivo y solo se puede exportar si usted decide hacerlo. Puede revocar el acceso a la ubicación en segundo plano en cualquier momento en los ajustes de Android.</t>
+  </si>
+  <si>
+    <t>GPSSample enregistre votre position en arrière-plan lorsque vous vous déplacez d'un foyer à l'autre. Cela permet à l'application de suivre votre itinéraire (fil d'Ariane), de cartographier l'emplacement des foyers et de vous guider vers les sites d'enquête sélectionnés. Votre position est stockée en toute sécurité sur votre appareil et ne peut être exportée que si vous le souhaitez. Vous pouvez révoquer l'accès à votre position en arrière-plan à tout moment dans les paramètres Android.</t>
+  </si>
+  <si>
+    <t>O GPSSample grava a sua localização em segundo plano enquanto se desloca entre residências. Isso permite que a aplicação acompanhe o seu percurso (trilha de navegação), mapeie as localizações das residências e navegue de volta aos locais selecionados para pesquisa. A sua localização é armazenada com segurança no seu dispositivo e só pode ser exportada se assim o desejar. Pode revogar o acesso à localização em segundo plano a qualquer momento nas Definições do Android.</t>
+  </si>
+  <si>
+    <t>GPSSample записывает ваше местоположение в фоновом режиме, когда вы перемещаетесь между домохозяйствами. Это позволяет приложению отслеживать ваш маршрут (хлебные крошки), отображать на карте местоположение домохозяйств и возвращаться к выбранным местам опроса. Ваше местоположение надежно хранится на вашем устройстве и может быть экспортировано только по вашему желанию. Вы можете отозвать доступ к фоновому местоположению в любое время в настройках Android.</t>
+  </si>
+  <si>
+    <t>GPSSample merekam lokasi Anda di latar belakang saat Anda berpindah antar rumah tangga. Hal ini memungkinkan aplikasi untuk melacak rute Anda (jejak perjalanan), memetakan lokasi rumah tangga, dan menavigasi kembali ke lokasi survei yang dipilih. Lokasi Anda disimpan dengan aman di perangkat Anda dan hanya dapat diekspor jika Anda memilih untuk melakukannya. Anda dapat mencabut akses lokasi latar belakang kapan saja di Pengaturan Android.</t>
+  </si>
+  <si>
+    <t>Itinatala ng GPSSample ang iyong lokasyon sa background habang lumilipat ka sa pagitan ng mga kabahayan. Nagbibigay-daan ito sa app na subaybayan ang iyong ruta (breadcrumb trail), imapa ang mga lokasyon ng kabahayan, at mag-navigate pabalik sa mga piling lugar ng survey. Ang iyong lokasyon ay ligtas na nakaimbak sa iyong device at maaari lamang i-export kung pipiliin mong gawin ito. Maaari mong bawiin ang access sa lokasyon sa background anumang oras sa Mga Setting ng Android.</t>
+  </si>
+  <si>
+    <t>privacy_policy_statement</t>
+  </si>
+  <si>
+    <t>accept_privacy_policy</t>
+  </si>
+  <si>
+    <t>decline_privacy_policy</t>
   </si>
 </sst>
 </file>
@@ -10423,7 +10495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -10462,6 +10534,15 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10564,8 +10645,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73295AEA-8140-4EAB-A7A6-7D1875F4D7E7}" name="Table1" displayName="Table1" ref="A1:H459" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:H459" xr:uid="{73295AEA-8140-4EAB-A7A6-7D1875F4D7E7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73295AEA-8140-4EAB-A7A6-7D1875F4D7E7}" name="Table1" displayName="Table1" ref="A1:H462" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:H462" xr:uid="{73295AEA-8140-4EAB-A7A6-7D1875F4D7E7}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{DE67F62A-9DCA-4DFE-8C98-83B024E5D946}" name="app_name" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{BCDA3AB5-7BB5-4A21-ABBB-4186B52D559D}" name="GPSSample::en" dataDxfId="1"/>
@@ -10889,13 +10970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD3E6CC-854C-5841-9577-D3ADD2982DB6}">
-  <dimension ref="A1:H459"/>
+  <dimension ref="A1:H462"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F442" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H460" sqref="H460"/>
+    <sheetView tabSelected="1" topLeftCell="A449" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A462" sqref="A462"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="22.6640625" customWidth="1"/>
     <col min="2" max="2" width="103.6640625" bestFit="1" customWidth="1"/>
@@ -10903,8 +10984,8 @@
     <col min="4" max="4" width="134.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="111.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="131" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="44.4140625" customWidth="1"/>
-    <col min="8" max="8" width="42.6640625" customWidth="1"/>
+    <col min="7" max="7" width="75.5" customWidth="1"/>
+    <col min="8" max="8" width="105.33203125" customWidth="1"/>
     <col min="9" max="9" width="44.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12936,7 +13017,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="16">
+    <row r="79" spans="1:8">
       <c r="A79" t="s">
         <v>452</v>
       </c>
@@ -12962,7 +13043,7 @@
         <v>2951</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="16">
+    <row r="80" spans="1:8">
       <c r="A80" t="s">
         <v>457</v>
       </c>
@@ -13378,7 +13459,7 @@
         <v>2967</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="16">
+    <row r="96" spans="1:8">
       <c r="A96" t="s">
         <v>563</v>
       </c>
@@ -13534,7 +13615,7 @@
         <v>2973</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="16">
+    <row r="102" spans="1:8">
       <c r="A102" t="s">
         <v>601</v>
       </c>
@@ -13820,7 +13901,7 @@
         <v>2984</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="16">
+    <row r="113" spans="1:8">
       <c r="A113" t="s">
         <v>672</v>
       </c>
@@ -17278,7 +17359,7 @@
         <v>3240</v>
       </c>
     </row>
-    <row r="246" spans="1:8" ht="16">
+    <row r="246" spans="1:8">
       <c r="A246" s="12" t="s">
         <v>1451</v>
       </c>
@@ -17304,7 +17385,7 @@
         <v>3241</v>
       </c>
     </row>
-    <row r="247" spans="1:8" ht="16">
+    <row r="247" spans="1:8">
       <c r="A247" s="12" t="s">
         <v>1455</v>
       </c>
@@ -17330,7 +17411,7 @@
         <v>3242</v>
       </c>
     </row>
-    <row r="248" spans="1:8" ht="16">
+    <row r="248" spans="1:8">
       <c r="A248" s="12" t="s">
         <v>1461</v>
       </c>
@@ -17356,7 +17437,7 @@
         <v>3243</v>
       </c>
     </row>
-    <row r="249" spans="1:8" ht="16">
+    <row r="249" spans="1:8">
       <c r="A249" s="12" t="s">
         <v>1467</v>
       </c>
@@ -17382,7 +17463,7 @@
         <v>3244</v>
       </c>
     </row>
-    <row r="250" spans="1:8" ht="16">
+    <row r="250" spans="1:8">
       <c r="A250" s="12" t="s">
         <v>1474</v>
       </c>
@@ -17408,7 +17489,7 @@
         <v>3245</v>
       </c>
     </row>
-    <row r="251" spans="1:8" ht="16">
+    <row r="251" spans="1:8">
       <c r="A251" s="12" t="s">
         <v>1478</v>
       </c>
@@ -17434,7 +17515,7 @@
         <v>3222</v>
       </c>
     </row>
-    <row r="252" spans="1:8" ht="16">
+    <row r="252" spans="1:8">
       <c r="A252" s="12" t="s">
         <v>1483</v>
       </c>
@@ -17460,7 +17541,7 @@
         <v>3223</v>
       </c>
     </row>
-    <row r="253" spans="1:8" ht="16">
+    <row r="253" spans="1:8">
       <c r="A253" s="12" t="s">
         <v>1487</v>
       </c>
@@ -17486,7 +17567,7 @@
         <v>3224</v>
       </c>
     </row>
-    <row r="254" spans="1:8" ht="16">
+    <row r="254" spans="1:8">
       <c r="A254" s="12" t="s">
         <v>1491</v>
       </c>
@@ -17512,7 +17593,7 @@
         <v>3225</v>
       </c>
     </row>
-    <row r="255" spans="1:8" ht="16">
+    <row r="255" spans="1:8">
       <c r="A255" s="12" t="s">
         <v>1498</v>
       </c>
@@ -17538,7 +17619,7 @@
         <v>3226</v>
       </c>
     </row>
-    <row r="256" spans="1:8" ht="16">
+    <row r="256" spans="1:8">
       <c r="A256" s="12" t="s">
         <v>1505</v>
       </c>
@@ -17564,7 +17645,7 @@
         <v>3227</v>
       </c>
     </row>
-    <row r="257" spans="1:8" ht="16">
+    <row r="257" spans="1:8">
       <c r="A257" s="12" t="s">
         <v>1510</v>
       </c>
@@ -17590,7 +17671,7 @@
         <v>3228</v>
       </c>
     </row>
-    <row r="258" spans="1:8" ht="16">
+    <row r="258" spans="1:8">
       <c r="A258" s="12" t="s">
         <v>1517</v>
       </c>
@@ -17616,7 +17697,7 @@
         <v>3229</v>
       </c>
     </row>
-    <row r="259" spans="1:8" ht="16">
+    <row r="259" spans="1:8">
       <c r="A259" s="12" t="s">
         <v>1523</v>
       </c>
@@ -17642,7 +17723,7 @@
         <v>3230</v>
       </c>
     </row>
-    <row r="260" spans="1:8" ht="16">
+    <row r="260" spans="1:8">
       <c r="A260" s="12" t="s">
         <v>1529</v>
       </c>
@@ -17668,7 +17749,7 @@
         <v>3230</v>
       </c>
     </row>
-    <row r="261" spans="1:8" ht="16">
+    <row r="261" spans="1:8">
       <c r="A261" s="12" t="s">
         <v>1530</v>
       </c>
@@ -17694,7 +17775,7 @@
         <v>3231</v>
       </c>
     </row>
-    <row r="262" spans="1:8" ht="16">
+    <row r="262" spans="1:8">
       <c r="A262" s="12" t="s">
         <v>1535</v>
       </c>
@@ -17720,7 +17801,7 @@
         <v>1535</v>
       </c>
     </row>
-    <row r="263" spans="1:8" ht="16">
+    <row r="263" spans="1:8">
       <c r="A263" s="12" t="s">
         <v>1536</v>
       </c>
@@ -17746,7 +17827,7 @@
         <v>1537</v>
       </c>
     </row>
-    <row r="264" spans="1:8" ht="16">
+    <row r="264" spans="1:8">
       <c r="A264" s="12" t="s">
         <v>1541</v>
       </c>
@@ -17772,7 +17853,7 @@
         <v>1542</v>
       </c>
     </row>
-    <row r="265" spans="1:8" ht="16">
+    <row r="265" spans="1:8">
       <c r="A265" s="12" t="s">
         <v>1546</v>
       </c>
@@ -17798,7 +17879,7 @@
         <v>3135</v>
       </c>
     </row>
-    <row r="266" spans="1:8" ht="16">
+    <row r="266" spans="1:8">
       <c r="A266" s="12" t="s">
         <v>1553</v>
       </c>
@@ -17824,7 +17905,7 @@
         <v>3136</v>
       </c>
     </row>
-    <row r="267" spans="1:8" ht="16">
+    <row r="267" spans="1:8">
       <c r="A267" s="12" t="s">
         <v>1558</v>
       </c>
@@ -17850,7 +17931,7 @@
         <v>3137</v>
       </c>
     </row>
-    <row r="268" spans="1:8" ht="16">
+    <row r="268" spans="1:8">
       <c r="A268" s="12" t="s">
         <v>1565</v>
       </c>
@@ -17876,7 +17957,7 @@
         <v>3138</v>
       </c>
     </row>
-    <row r="269" spans="1:8" ht="16">
+    <row r="269" spans="1:8">
       <c r="A269" s="12" t="s">
         <v>1572</v>
       </c>
@@ -17902,7 +17983,7 @@
         <v>3139</v>
       </c>
     </row>
-    <row r="270" spans="1:8" ht="16">
+    <row r="270" spans="1:8">
       <c r="A270" s="12" t="s">
         <v>1578</v>
       </c>
@@ -17928,7 +18009,7 @@
         <v>3140</v>
       </c>
     </row>
-    <row r="271" spans="1:8" ht="16">
+    <row r="271" spans="1:8">
       <c r="A271" s="12" t="s">
         <v>1583</v>
       </c>
@@ -17954,7 +18035,7 @@
         <v>3141</v>
       </c>
     </row>
-    <row r="272" spans="1:8" ht="16">
+    <row r="272" spans="1:8">
       <c r="A272" s="12" t="s">
         <v>1590</v>
       </c>
@@ -17980,7 +18061,7 @@
         <v>3142</v>
       </c>
     </row>
-    <row r="273" spans="1:8" ht="16">
+    <row r="273" spans="1:8">
       <c r="A273" s="12" t="s">
         <v>1597</v>
       </c>
@@ -18006,7 +18087,7 @@
         <v>3143</v>
       </c>
     </row>
-    <row r="274" spans="1:8" ht="16">
+    <row r="274" spans="1:8">
       <c r="A274" s="12" t="s">
         <v>1604</v>
       </c>
@@ -18032,7 +18113,7 @@
         <v>3203</v>
       </c>
     </row>
-    <row r="275" spans="1:8" ht="16">
+    <row r="275" spans="1:8">
       <c r="A275" s="12" t="s">
         <v>1611</v>
       </c>
@@ -18058,7 +18139,7 @@
         <v>3204</v>
       </c>
     </row>
-    <row r="276" spans="1:8" ht="16">
+    <row r="276" spans="1:8">
       <c r="A276" s="12" t="s">
         <v>1617</v>
       </c>
@@ -18136,7 +18217,7 @@
         <v>3206</v>
       </c>
     </row>
-    <row r="279" spans="1:8" ht="16">
+    <row r="279" spans="1:8">
       <c r="A279" s="15" t="s">
         <v>1631</v>
       </c>
@@ -18162,7 +18243,7 @@
         <v>3207</v>
       </c>
     </row>
-    <row r="280" spans="1:8" ht="16">
+    <row r="280" spans="1:8">
       <c r="A280" s="15" t="s">
         <v>1636</v>
       </c>
@@ -18188,7 +18269,7 @@
         <v>3208</v>
       </c>
     </row>
-    <row r="281" spans="1:8" ht="16">
+    <row r="281" spans="1:8">
       <c r="A281" s="15" t="s">
         <v>1642</v>
       </c>
@@ -18266,7 +18347,7 @@
         <v>3210</v>
       </c>
     </row>
-    <row r="284" spans="1:8" ht="16">
+    <row r="284" spans="1:8">
       <c r="A284" s="15" t="s">
         <v>1661</v>
       </c>
@@ -22840,6 +22921,84 @@
       </c>
       <c r="H459" t="s">
         <v>3378</v>
+      </c>
+    </row>
+    <row r="460" spans="1:8" ht="102">
+      <c r="A460" s="18" t="s">
+        <v>3400</v>
+      </c>
+      <c r="B460" s="31" t="s">
+        <v>3393</v>
+      </c>
+      <c r="C460" s="32" t="s">
+        <v>3394</v>
+      </c>
+      <c r="D460" s="32" t="s">
+        <v>3395</v>
+      </c>
+      <c r="E460" s="32" t="s">
+        <v>3396</v>
+      </c>
+      <c r="F460" s="32" t="s">
+        <v>3397</v>
+      </c>
+      <c r="G460" s="33" t="s">
+        <v>3398</v>
+      </c>
+      <c r="H460" s="32" t="s">
+        <v>3399</v>
+      </c>
+    </row>
+    <row r="461" spans="1:8" ht="34">
+      <c r="A461" s="18" t="s">
+        <v>3401</v>
+      </c>
+      <c r="B461" s="31" t="s">
+        <v>3380</v>
+      </c>
+      <c r="C461" s="32" t="s">
+        <v>3382</v>
+      </c>
+      <c r="D461" s="32" t="s">
+        <v>3384</v>
+      </c>
+      <c r="E461" s="32" t="s">
+        <v>3386</v>
+      </c>
+      <c r="F461" s="32" t="s">
+        <v>3388</v>
+      </c>
+      <c r="G461" s="33" t="s">
+        <v>3390</v>
+      </c>
+      <c r="H461" s="32" t="s">
+        <v>3392</v>
+      </c>
+    </row>
+    <row r="462" spans="1:8">
+      <c r="A462" s="18" t="s">
+        <v>3402</v>
+      </c>
+      <c r="B462" s="14" t="s">
+        <v>3379</v>
+      </c>
+      <c r="C462" t="s">
+        <v>3381</v>
+      </c>
+      <c r="D462" t="s">
+        <v>3383</v>
+      </c>
+      <c r="E462" t="s">
+        <v>3385</v>
+      </c>
+      <c r="F462" t="s">
+        <v>3387</v>
+      </c>
+      <c r="G462" s="26" t="s">
+        <v>3389</v>
+      </c>
+      <c r="H462" t="s">
+        <v>3391</v>
       </c>
     </row>
   </sheetData>
@@ -22854,17 +23013,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F12BE0DB4A3DF641BF113FBF1C7EA261" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="28c053331c12fbc62292d36b1bc55ed6">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="43e153a8-5ef1-4f65-aac7-dc4685f18eaa" xmlns:ns3="6e0cf07b-8188-4b76-8f54-3cda03d37414" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="22da4ad5a98080e11d5a1bb4312b4b9d" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F12BE0DB4A3DF641BF113FBF1C7EA261" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e32f6aa5b44672ac6fa3a2698066c012">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="43e153a8-5ef1-4f65-aac7-dc4685f18eaa" xmlns:ns3="6e0cf07b-8188-4b76-8f54-3cda03d37414" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="89bbc5cb1abb29866a927cf0e3afecbc" ns2:_="" ns3:_="">
     <xsd:import namespace="43e153a8-5ef1-4f65-aac7-dc4685f18eaa"/>
     <xsd:import namespace="6e0cf07b-8188-4b76-8f54-3cda03d37414"/>
     <xsd:element name="properties">
@@ -22887,6 +23037,7 @@
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceBillingMetadata" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -22952,6 +23103,11 @@
       </xsd:simpleType>
     </xsd:element>
     <xsd:element name="MediaServiceSearchProperties" ma:index="22" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceBillingMetadata" ma:index="23" nillable="true" ma:displayName="MediaServiceBillingMetadata" ma:hidden="true" ma:internalName="MediaServiceBillingMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
@@ -23097,7 +23253,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="6e0cf07b-8188-4b76-8f54-3cda03d37414" xsi:nil="true"/>
@@ -23108,16 +23264,17 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04FEE910-FEC8-48C6-9CF9-BF01BA5AD6FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6939F493-2774-4738-8826-4A42598DC3F5}">
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42447327-F0FE-419B-8CF4-916C8DF31BF4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -23135,19 +23292,27 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E20926E-9EFB-4B7E-90D4-905B08F8E59C}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6e0cf07b-8188-4b76-8f54-3cda03d37414"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="43e153a8-5ef1-4f65-aac7-dc4685f18eaa"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="6e0cf07b-8188-4b76-8f54-3cda03d37414"/>
-    <ds:schemaRef ds:uri="43e153a8-5ef1-4f65-aac7-dc4685f18eaa"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04FEE910-FEC8-48C6-9CF9-BF01BA5AD6FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>